<commit_message>
Modifica limite per casse con lunghezza inferiore ai 5800mm
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB7723C-EAF0-40BF-8410-96DB5A5E86E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758DA11A-09AA-4A58-9CD6-BFBE87EE9B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="SimulazioneConf1" sheetId="3" r:id="rId3"/>
     <sheet name="SimulazioneConf7" sheetId="6" r:id="rId4"/>
     <sheet name="SimulazioneConf6" sheetId="4" r:id="rId5"/>
+    <sheet name="Database" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$16</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -96,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="111">
   <si>
     <t>Diagonali</t>
   </si>
@@ -342,6 +346,97 @@
   </si>
   <si>
     <t>Diametro corr</t>
+  </si>
+  <si>
+    <t>Alt. Tot</t>
+  </si>
+  <si>
+    <t>Traversino</t>
+  </si>
+  <si>
+    <t>Lamiera superiore</t>
+  </si>
+  <si>
+    <t>Bordo + nastro</t>
+  </si>
+  <si>
+    <t>Diam corrugato</t>
+  </si>
+  <si>
+    <t>N. Commessa</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Lunghezza Nastro</t>
+  </si>
+  <si>
+    <t>Larghezza nastro</t>
+  </si>
+  <si>
+    <t>Altezza Bordo</t>
+  </si>
+  <si>
+    <t>Tipologia</t>
+  </si>
+  <si>
+    <t>Lunghezza cassa</t>
+  </si>
+  <si>
+    <t>Larghezza cassa</t>
+  </si>
+  <si>
+    <t>Altezza cassa</t>
+  </si>
+  <si>
+    <t>Numero file</t>
+  </si>
+  <si>
+    <t>CALCOLATA</t>
+  </si>
+  <si>
+    <t>REALE</t>
+  </si>
+  <si>
+    <t>Conf.</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Bordi e tazze</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Cassa in legno</t>
+  </si>
+  <si>
+    <t>Aperto
+Chiuso</t>
+  </si>
+  <si>
+    <t>Aperto</t>
+  </si>
+  <si>
+    <t>Cassa in ferro</t>
+  </si>
+  <si>
+    <t>RISULTATO</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>Chiuso</t>
+  </si>
+  <si>
+    <t>Solo bordi</t>
   </si>
 </sst>
 </file>
@@ -352,7 +447,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,8 +498,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,8 +543,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -744,6 +853,221 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -751,7 +1075,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -870,6 +1194,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -894,6 +1220,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -901,7 +1323,22 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1253,16 +1690,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>458023</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>124242</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>115123</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>417</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1277,22 +1714,132 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="5169"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9286875" y="1514475"/>
-          <a:ext cx="5896798" cy="2991267"/>
+          <a:off x="8639175" y="2171700"/>
+          <a:ext cx="5591998" cy="2591217"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9391650" y="3257550"/>
+          <a:ext cx="619125" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13535025" y="3343275"/>
+          <a:ext cx="600075" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1342,6 +1889,540 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10067925" y="2762250"/>
+          <a:ext cx="28576" cy="2752726"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10182225" y="5257800"/>
+          <a:ext cx="342900" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10191750" y="4981575"/>
+          <a:ext cx="342900" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="4714875"/>
+          <a:ext cx="342900" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10210800" y="4419600"/>
+          <a:ext cx="276225" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9763125" y="3667125"/>
+          <a:ext cx="314325" cy="123825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9791700" y="3533775"/>
+          <a:ext cx="314325" cy="123825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9772650" y="2990850"/>
+          <a:ext cx="276225" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9772650" y="2886075"/>
+          <a:ext cx="276225" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1711,10 +2792,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="57"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -2248,21 +3329,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="56" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="59" t="s">
+      <c r="H1" s="59"/>
+      <c r="I1" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="61" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2291,8 +3372,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -2645,7 +3726,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,11 +3760,11 @@
         <v>65</v>
       </c>
       <c r="B2" s="1">
-        <v>11800</v>
+        <v>15000</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="52">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="E2" s="52">
         <v>350</v>
@@ -2697,14 +3778,14 @@
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="52">
         <v>200</v>
       </c>
       <c r="E3" s="52">
-        <v>650</v>
+        <v>350</v>
       </c>
       <c r="F3" s="53">
         <v>400</v>
@@ -2715,7 +3796,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="1">
-        <v>90000</v>
+        <v>100000</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
@@ -2726,7 +3807,7 @@
         <v>68</v>
       </c>
       <c r="B5" s="1">
-        <v>400</v>
+        <v>630</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -2737,7 +3818,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="1">
-        <v>650</v>
+        <v>900</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
@@ -2756,14 +3837,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2791,22 +3872,22 @@
       </c>
       <c r="B11" s="1">
         <f>B2-B6/2</f>
-        <v>11475</v>
+        <v>14550</v>
       </c>
       <c r="C11" s="1">
         <f>IF(ISEVEN(A11),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>1021.0176124166827</v>
+        <v>1413.7166941154069</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
         <f>MAX(D11:D23)</f>
-        <v>2600</v>
+        <v>2700</v>
       </c>
       <c r="F11" s="1">
         <f>SUM(B11:B32) + SUM(C11:C32)</f>
-        <v>95749.999246391162</v>
+        <v>88029.357668809753</v>
       </c>
       <c r="N11">
         <f>2240/300</f>
@@ -2819,15 +3900,15 @@
       </c>
       <c r="B12" s="1">
         <f>IF(ISEVEN(A12),B11-$B$5*0.5-$B$3,B11-$B$5*0.5-$B$6*0.5)</f>
-        <v>11075</v>
+        <v>14175</v>
       </c>
       <c r="C12" s="1">
         <f>IF(ISEVEN(A12),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>942.47779607693792</v>
+        <v>1484.4025288211774</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D19" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
-        <v>650</v>
+        <f t="shared" ref="D12:D16" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <v>900</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2836,15 +3917,15 @@
       </c>
       <c r="B13" s="1">
         <f>IF(ISEVEN(A13),B12-$B$5*0.5-$B$3,B12-$B$5*0.5-$B$6*0.5)</f>
-        <v>10550</v>
+        <v>13410</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:C19" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>1021.0176124166827</v>
+        <f t="shared" ref="C13:C16" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
+        <v>1413.7166941154069</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>750</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2852,16 +3933,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:B19" si="2">IF(ISEVEN(A14),B13-$B$5*0.5-$B$3,B13-$B$5*0.5-$B$6*0.5)</f>
-        <v>10150</v>
+        <f t="shared" ref="B14:B16" si="2">IF(ISEVEN(A14),B13-$B$5*0.5-$B$3,B13-$B$5*0.5-$B$6*0.5)</f>
+        <v>13035</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>942.47779607693792</v>
+        <v>1484.4025288211774</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2870,15 +3951,15 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="2"/>
-        <v>9625</v>
+        <v>12270</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>1021.0176124166827</v>
+        <v>1413.7166941154069</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>810</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2887,125 +3968,126 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="2"/>
-        <v>9225</v>
+        <v>11895</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>942.47779607693792</v>
+        <v>1484.4025288211774</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="1">
-        <f t="shared" si="2"/>
-        <v>8700</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="1"/>
-        <v>1021.0176124166827</v>
-      </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
-      <c r="B18" s="1">
-        <f t="shared" si="2"/>
-        <v>8300</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="1"/>
-        <v>942.47779607693792</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
-      <c r="B19" s="1">
-        <f t="shared" si="2"/>
-        <v>7775</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="1"/>
-        <v>1021.0176124166827</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>11</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>14</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>15</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>16</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26">
+        <f>SUM(I19:I25)</f>
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>17</v>
       </c>
@@ -3013,7 +4095,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>18</v>
       </c>
@@ -3021,7 +4103,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>19</v>
       </c>
@@ -3029,7 +4111,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>20</v>
       </c>
@@ -3037,7 +4119,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>21</v>
       </c>
@@ -3045,7 +4127,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>22</v>
       </c>
@@ -3067,8 +4149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA6E99C-AB9E-4667-BE9F-DF6A69A1542A}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,7 +4160,7 @@
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3102,7 +4184,7 @@
         <v>65</v>
       </c>
       <c r="B2" s="1">
-        <v>9500</v>
+        <v>15900</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="52">
@@ -3120,7 +4202,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="52">
@@ -3190,14 +4272,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3225,7 +4307,7 @@
       </c>
       <c r="B11" s="1">
         <f>B2-B6/2</f>
-        <v>9050</v>
+        <v>15450</v>
       </c>
       <c r="C11" s="1">
         <f>IF(ISEVEN(A11),$B$5*PI()*0.75,$B$6*PI()/2)</f>
@@ -3240,7 +4322,7 @@
       </c>
       <c r="F11" s="1">
         <f>SUM(B11:B32) + SUM(C11:C32)</f>
-        <v>52959.357668809753</v>
+        <v>122188.47689174634</v>
       </c>
       <c r="N11">
         <f>2240/300</f>
@@ -3253,14 +4335,14 @@
       </c>
       <c r="B12" s="1">
         <f>B11-B5/2-B3</f>
-        <v>8435</v>
+        <v>14855</v>
       </c>
       <c r="C12" s="1">
         <f>IF(ISEVEN(A12),$B$5*PI()*0.75,$B$6*PI()/2)</f>
         <v>1484.4025288211774</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D19" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <f t="shared" ref="D12:D15" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>900</v>
       </c>
     </row>
@@ -3270,15 +4352,15 @@
       </c>
       <c r="B13" s="1">
         <f>B12-1.5*B6-B3</f>
-        <v>6785</v>
+        <v>13225</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:C19" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
+        <f t="shared" ref="C13:C18" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
         <v>1413.7166941154069</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>1230</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3287,15 +4369,21 @@
       </c>
       <c r="B14" s="1">
         <f>B13-B5-B3</f>
-        <v>5855</v>
+        <v>12315</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
         <v>1484.4025288211774</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>1800</v>
+        <f>IF(ISEVEN(A14),B3*A14/2+B6,(A14-((A14-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <v>1460</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3304,7 +4392,7 @@
       </c>
       <c r="B15" s="1">
         <f>B14+B6</f>
-        <v>6755</v>
+        <v>13215</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
@@ -3312,7 +4400,13 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>1530</v>
+        <v>1470</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3321,90 +4415,155 @@
       </c>
       <c r="B16" s="1">
         <f>B15+B5</f>
-        <v>7385</v>
+        <v>13845</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
         <v>1484.4025288211774</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <v>1800</v>
+      </c>
+      <c r="F16" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <f>B16</f>
+        <v>13845</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>1413.7166941154069</v>
+      </c>
+      <c r="D17" s="1">
+        <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <v>1750</v>
+      </c>
+      <c r="F17" s="65"/>
+      <c r="G17" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <f>B17+B7</f>
+        <v>13846</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>1484.4025288211774</v>
+      </c>
+      <c r="D18" s="1">
+        <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <v>2700</v>
+      </c>
+      <c r="F18" s="65"/>
+      <c r="G18" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="65"/>
+      <c r="G19" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" s="65"/>
+      <c r="G20" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>11</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="65"/>
+      <c r="G21" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="65"/>
+      <c r="G22" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="66"/>
+      <c r="G23" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>14</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>15</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="55">
+        <f>SUM(G14:G24)</f>
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>16</v>
       </c>
@@ -3412,7 +4571,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>17</v>
       </c>
@@ -3420,7 +4579,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>18</v>
       </c>
@@ -3428,7 +4587,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>19</v>
       </c>
@@ -3436,7 +4595,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>20</v>
       </c>
@@ -3444,7 +4603,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>21</v>
       </c>
@@ -3452,7 +4611,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>22</v>
       </c>
@@ -3461,8 +4620,9 @@
       <c r="D32" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A9:F9"/>
+    <mergeCell ref="F16:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3565,14 +4725,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3882,4 +5042,2347 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
+  <dimension ref="A1:AG75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="94" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q2" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="S2" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" s="95"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="77">
+        <v>20210538</v>
+      </c>
+      <c r="B3" s="78">
+        <v>44566</v>
+      </c>
+      <c r="C3" s="79">
+        <v>10200</v>
+      </c>
+      <c r="D3" s="79">
+        <v>400</v>
+      </c>
+      <c r="E3" s="79">
+        <v>100</v>
+      </c>
+      <c r="F3" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="77">
+        <v>1200</v>
+      </c>
+      <c r="I3" s="87">
+        <v>800</v>
+      </c>
+      <c r="J3" s="79">
+        <v>600</v>
+      </c>
+      <c r="K3" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" s="77">
+        <v>1200</v>
+      </c>
+      <c r="O3" s="79">
+        <v>1200</v>
+      </c>
+      <c r="P3" s="79">
+        <v>600</v>
+      </c>
+      <c r="Q3" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T3" s="91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="81">
+        <v>20210304</v>
+      </c>
+      <c r="B4" s="86">
+        <v>44411</v>
+      </c>
+      <c r="C4" s="52">
+        <v>33000</v>
+      </c>
+      <c r="D4" s="52">
+        <v>1200</v>
+      </c>
+      <c r="E4" s="79">
+        <v>120</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="88">
+        <v>2400</v>
+      </c>
+      <c r="I4" s="87">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="87">
+        <v>1400</v>
+      </c>
+      <c r="K4" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="88">
+        <v>3700</v>
+      </c>
+      <c r="O4" s="87">
+        <v>1350</v>
+      </c>
+      <c r="P4" s="87">
+        <v>2200</v>
+      </c>
+      <c r="Q4" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="S4" s="85">
+        <v>1</v>
+      </c>
+      <c r="T4" s="92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="81">
+        <v>20210152</v>
+      </c>
+      <c r="B5" s="86">
+        <v>44445</v>
+      </c>
+      <c r="C5" s="52">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="52">
+        <v>650</v>
+      </c>
+      <c r="E5" s="79">
+        <v>200</v>
+      </c>
+      <c r="F5" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="88">
+        <v>7000</v>
+      </c>
+      <c r="I5" s="87">
+        <v>790</v>
+      </c>
+      <c r="J5" s="79">
+        <v>2240</v>
+      </c>
+      <c r="K5" s="79">
+        <v>7</v>
+      </c>
+      <c r="L5" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="89">
+        <v>1</v>
+      </c>
+      <c r="N5" s="88">
+        <v>5000</v>
+      </c>
+      <c r="O5" s="87">
+        <v>1600</v>
+      </c>
+      <c r="P5" s="79">
+        <v>2240</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="S5" s="90">
+        <v>2</v>
+      </c>
+      <c r="T5" s="92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="81">
+        <v>20210164</v>
+      </c>
+      <c r="B6" s="86">
+        <v>44407</v>
+      </c>
+      <c r="C6" s="52">
+        <v>120000</v>
+      </c>
+      <c r="D6" s="52">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="79">
+        <v>240</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="88">
+        <v>8400</v>
+      </c>
+      <c r="I6" s="79">
+        <v>2230</v>
+      </c>
+      <c r="J6" s="79">
+        <v>2530</v>
+      </c>
+      <c r="K6" s="79">
+        <v>7</v>
+      </c>
+      <c r="L6" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="80">
+        <v>2</v>
+      </c>
+      <c r="N6" s="88">
+        <v>9500</v>
+      </c>
+      <c r="O6" s="79">
+        <v>2300</v>
+      </c>
+      <c r="P6" s="79">
+        <v>2450</v>
+      </c>
+      <c r="Q6" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="S6" s="85">
+        <v>2</v>
+      </c>
+      <c r="T6" s="92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="81">
+        <v>20210296</v>
+      </c>
+      <c r="B7" s="86">
+        <v>44414</v>
+      </c>
+      <c r="C7" s="52">
+        <v>22000</v>
+      </c>
+      <c r="D7" s="52">
+        <v>650</v>
+      </c>
+      <c r="E7" s="79">
+        <v>120</v>
+      </c>
+      <c r="F7" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="88">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="87">
+        <v>2000</v>
+      </c>
+      <c r="J7" s="79">
+        <v>850</v>
+      </c>
+      <c r="K7" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N7" s="77">
+        <v>1800</v>
+      </c>
+      <c r="O7" s="79">
+        <v>1800</v>
+      </c>
+      <c r="P7" s="79">
+        <v>800</v>
+      </c>
+      <c r="Q7" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S7" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T7" s="92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="81">
+        <v>20210250</v>
+      </c>
+      <c r="B8" s="86">
+        <v>44362</v>
+      </c>
+      <c r="C8" s="52">
+        <v>13200</v>
+      </c>
+      <c r="D8" s="52">
+        <v>800</v>
+      </c>
+      <c r="E8" s="79">
+        <v>50</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="77">
+        <v>1200</v>
+      </c>
+      <c r="I8" s="79">
+        <v>800</v>
+      </c>
+      <c r="J8" s="79">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M8" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="77">
+        <v>1200</v>
+      </c>
+      <c r="O8" s="79">
+        <v>800</v>
+      </c>
+      <c r="P8" s="79">
+        <v>950</v>
+      </c>
+      <c r="Q8" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S8" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T8" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="81">
+        <v>20210187</v>
+      </c>
+      <c r="B9" s="86">
+        <v>44326</v>
+      </c>
+      <c r="C9" s="52">
+        <v>17000</v>
+      </c>
+      <c r="D9" s="52">
+        <v>300</v>
+      </c>
+      <c r="E9" s="79">
+        <v>80</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="77">
+        <v>1400</v>
+      </c>
+      <c r="I9" s="79">
+        <v>1400</v>
+      </c>
+      <c r="J9" s="79">
+        <v>500</v>
+      </c>
+      <c r="K9" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" s="77">
+        <v>1350</v>
+      </c>
+      <c r="O9" s="79">
+        <v>1350</v>
+      </c>
+      <c r="P9" s="79">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R9" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S9" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T9" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="81">
+        <v>20210272</v>
+      </c>
+      <c r="B10" s="86">
+        <v>44398</v>
+      </c>
+      <c r="C10" s="52">
+        <v>28440</v>
+      </c>
+      <c r="D10" s="52">
+        <v>650</v>
+      </c>
+      <c r="E10" s="79">
+        <v>80</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="77">
+        <v>1800</v>
+      </c>
+      <c r="I10" s="79">
+        <v>1800</v>
+      </c>
+      <c r="J10" s="79">
+        <v>850</v>
+      </c>
+      <c r="K10" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="77">
+        <v>1800</v>
+      </c>
+      <c r="O10" s="79">
+        <v>1800</v>
+      </c>
+      <c r="P10" s="79">
+        <v>900</v>
+      </c>
+      <c r="Q10" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S10" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T10" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="81">
+        <v>20210264</v>
+      </c>
+      <c r="B11" s="86">
+        <v>44393</v>
+      </c>
+      <c r="C11" s="52">
+        <v>7562</v>
+      </c>
+      <c r="D11" s="52">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="79">
+        <v>100</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="77">
+        <v>1400</v>
+      </c>
+      <c r="I11" s="79">
+        <v>1400</v>
+      </c>
+      <c r="J11" s="79">
+        <v>1200</v>
+      </c>
+      <c r="K11" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N11" s="77">
+        <v>1300</v>
+      </c>
+      <c r="O11" s="79">
+        <v>1300</v>
+      </c>
+      <c r="P11" s="79">
+        <v>1200</v>
+      </c>
+      <c r="Q11" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R11" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S11" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T11" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="81">
+        <v>20210235</v>
+      </c>
+      <c r="B12" s="86">
+        <v>44382</v>
+      </c>
+      <c r="C12" s="52">
+        <v>10000</v>
+      </c>
+      <c r="D12" s="52">
+        <v>1400</v>
+      </c>
+      <c r="E12" s="79">
+        <v>100</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="77">
+        <v>1800</v>
+      </c>
+      <c r="I12" s="79">
+        <v>1800</v>
+      </c>
+      <c r="J12" s="79">
+        <v>1600</v>
+      </c>
+      <c r="K12" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N12" s="77">
+        <v>2000</v>
+      </c>
+      <c r="O12" s="79">
+        <v>1800</v>
+      </c>
+      <c r="P12" s="79">
+        <v>1600</v>
+      </c>
+      <c r="Q12" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R12" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S12" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T12" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="81">
+        <v>20210245</v>
+      </c>
+      <c r="B13" s="86">
+        <v>44412</v>
+      </c>
+      <c r="C13" s="52">
+        <v>26000</v>
+      </c>
+      <c r="D13" s="52">
+        <v>1200</v>
+      </c>
+      <c r="E13" s="79">
+        <v>80</v>
+      </c>
+      <c r="F13" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="77">
+        <v>1800</v>
+      </c>
+      <c r="I13" s="79">
+        <v>1800</v>
+      </c>
+      <c r="J13" s="79">
+        <v>1400</v>
+      </c>
+      <c r="K13" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N13" s="77">
+        <v>1800</v>
+      </c>
+      <c r="O13" s="79">
+        <v>1800</v>
+      </c>
+      <c r="P13" s="79">
+        <v>1400</v>
+      </c>
+      <c r="Q13" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R13" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="S13" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="T13" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="81">
+        <v>20200269</v>
+      </c>
+      <c r="B14" s="86">
+        <v>44119</v>
+      </c>
+      <c r="C14" s="52">
+        <v>93500</v>
+      </c>
+      <c r="D14" s="52">
+        <v>800</v>
+      </c>
+      <c r="E14" s="79">
+        <v>240</v>
+      </c>
+      <c r="F14" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="77">
+        <v>7600</v>
+      </c>
+      <c r="I14" s="79">
+        <v>1830</v>
+      </c>
+      <c r="J14" s="79">
+        <v>2240</v>
+      </c>
+      <c r="K14" s="79">
+        <v>7</v>
+      </c>
+      <c r="L14" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="80">
+        <v>2</v>
+      </c>
+      <c r="N14" s="77">
+        <v>8000</v>
+      </c>
+      <c r="O14" s="79">
+        <v>1900</v>
+      </c>
+      <c r="P14" s="79">
+        <v>2240</v>
+      </c>
+      <c r="Q14" s="79">
+        <v>7</v>
+      </c>
+      <c r="R14" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="S14" s="85">
+        <v>2</v>
+      </c>
+      <c r="T14" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="81">
+        <v>20200368</v>
+      </c>
+      <c r="B15" s="86">
+        <v>44144</v>
+      </c>
+      <c r="C15" s="52">
+        <v>29000</v>
+      </c>
+      <c r="D15" s="52">
+        <v>650</v>
+      </c>
+      <c r="E15" s="79">
+        <v>120</v>
+      </c>
+      <c r="F15" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="77">
+        <v>3800</v>
+      </c>
+      <c r="I15" s="79">
+        <v>790</v>
+      </c>
+      <c r="J15" s="79">
+        <v>2240</v>
+      </c>
+      <c r="K15" s="79">
+        <v>1</v>
+      </c>
+      <c r="L15" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="80">
+        <v>1</v>
+      </c>
+      <c r="N15" s="77">
+        <v>3000</v>
+      </c>
+      <c r="O15" s="79">
+        <v>800</v>
+      </c>
+      <c r="P15" s="79">
+        <v>2240</v>
+      </c>
+      <c r="Q15" s="79">
+        <v>3</v>
+      </c>
+      <c r="R15" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="S15" s="85">
+        <v>1</v>
+      </c>
+      <c r="T15" s="92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="81">
+        <v>20200306</v>
+      </c>
+      <c r="B16" s="86">
+        <v>44109</v>
+      </c>
+      <c r="C16" s="52">
+        <v>34500</v>
+      </c>
+      <c r="D16" s="52">
+        <v>800</v>
+      </c>
+      <c r="E16" s="79">
+        <v>80</v>
+      </c>
+      <c r="F16" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="77">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="79">
+        <v>2000</v>
+      </c>
+      <c r="J16" s="79">
+        <v>1000</v>
+      </c>
+      <c r="K16" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M16" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="N16" s="88">
+        <v>3000</v>
+      </c>
+      <c r="O16" s="87">
+        <v>1000</v>
+      </c>
+      <c r="P16" s="87">
+        <v>2240</v>
+      </c>
+      <c r="Q16" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R16" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="S16" s="85">
+        <v>1</v>
+      </c>
+      <c r="T16" s="92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="81"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="79"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="79"/>
+      <c r="R17" s="79"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="92"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="81"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="92"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79"/>
+      <c r="R19" s="79"/>
+      <c r="S19" s="85"/>
+      <c r="T19" s="92"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="81"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="79"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="85"/>
+      <c r="T20" s="92"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="81"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="92"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="81"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="92"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="81"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="79"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="92"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="81"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="77"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="85"/>
+      <c r="T24" s="92"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="81"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="77"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="85"/>
+      <c r="T25" s="92"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="81"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="85"/>
+      <c r="T26" s="92"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="81"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="77"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="79"/>
+      <c r="R27" s="79"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="92"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="81"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="77"/>
+      <c r="O28" s="79"/>
+      <c r="P28" s="79"/>
+      <c r="Q28" s="79"/>
+      <c r="R28" s="79"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="92"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="81"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="77"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="79"/>
+      <c r="R29" s="79"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="92"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="81"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="92"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="81"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="80"/>
+      <c r="N31" s="77"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="79"/>
+      <c r="R31" s="79"/>
+      <c r="S31" s="85"/>
+      <c r="T31" s="92"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="81"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="79"/>
+      <c r="P32" s="79"/>
+      <c r="Q32" s="79"/>
+      <c r="R32" s="79"/>
+      <c r="S32" s="85"/>
+      <c r="T32" s="92"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="81"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="79"/>
+      <c r="P33" s="79"/>
+      <c r="Q33" s="79"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="85"/>
+      <c r="T33" s="92"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="81"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="79"/>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="79"/>
+      <c r="S34" s="85"/>
+      <c r="T34" s="92"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="81"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="85"/>
+      <c r="T35" s="92"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="81"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="77"/>
+      <c r="O36" s="79"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="79"/>
+      <c r="R36" s="79"/>
+      <c r="S36" s="85"/>
+      <c r="T36" s="92"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="81"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="77"/>
+      <c r="O37" s="79"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="79"/>
+      <c r="S37" s="85"/>
+      <c r="T37" s="92"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="81"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="77"/>
+      <c r="O38" s="79"/>
+      <c r="P38" s="79"/>
+      <c r="Q38" s="79"/>
+      <c r="R38" s="79"/>
+      <c r="S38" s="85"/>
+      <c r="T38" s="92"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="81"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="79"/>
+      <c r="P39" s="79"/>
+      <c r="Q39" s="79"/>
+      <c r="R39" s="79"/>
+      <c r="S39" s="85"/>
+      <c r="T39" s="92"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="81"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="80"/>
+      <c r="N40" s="77"/>
+      <c r="O40" s="79"/>
+      <c r="P40" s="79"/>
+      <c r="Q40" s="79"/>
+      <c r="R40" s="79"/>
+      <c r="S40" s="85"/>
+      <c r="T40" s="92"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="81"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="77"/>
+      <c r="O41" s="79"/>
+      <c r="P41" s="79"/>
+      <c r="Q41" s="79"/>
+      <c r="R41" s="79"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="92"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="81"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="80"/>
+      <c r="N42" s="77"/>
+      <c r="O42" s="79"/>
+      <c r="P42" s="79"/>
+      <c r="Q42" s="79"/>
+      <c r="R42" s="79"/>
+      <c r="S42" s="85"/>
+      <c r="T42" s="92"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="81"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="79"/>
+      <c r="J43" s="79"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="79"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="77"/>
+      <c r="O43" s="79"/>
+      <c r="P43" s="79"/>
+      <c r="Q43" s="79"/>
+      <c r="R43" s="79"/>
+      <c r="S43" s="85"/>
+      <c r="T43" s="92"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="81"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="80"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="79"/>
+      <c r="P44" s="79"/>
+      <c r="Q44" s="79"/>
+      <c r="R44" s="79"/>
+      <c r="S44" s="85"/>
+      <c r="T44" s="92"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="81"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="79"/>
+      <c r="P45" s="79"/>
+      <c r="Q45" s="79"/>
+      <c r="R45" s="79"/>
+      <c r="S45" s="85"/>
+      <c r="T45" s="92"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="81"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="79"/>
+      <c r="M46" s="80"/>
+      <c r="N46" s="77"/>
+      <c r="O46" s="79"/>
+      <c r="P46" s="79"/>
+      <c r="Q46" s="79"/>
+      <c r="R46" s="79"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="92"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="81"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="79"/>
+      <c r="M47" s="80"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="79"/>
+      <c r="P47" s="79"/>
+      <c r="Q47" s="79"/>
+      <c r="R47" s="79"/>
+      <c r="S47" s="85"/>
+      <c r="T47" s="92"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="81"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="79"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="77"/>
+      <c r="O48" s="79"/>
+      <c r="P48" s="79"/>
+      <c r="Q48" s="79"/>
+      <c r="R48" s="79"/>
+      <c r="S48" s="85"/>
+      <c r="T48" s="92"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="81"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="79"/>
+      <c r="J49" s="79"/>
+      <c r="K49" s="79"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="80"/>
+      <c r="N49" s="77"/>
+      <c r="O49" s="79"/>
+      <c r="P49" s="79"/>
+      <c r="Q49" s="79"/>
+      <c r="R49" s="79"/>
+      <c r="S49" s="85"/>
+      <c r="T49" s="92"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="81"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="79"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="79"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="80"/>
+      <c r="N50" s="77"/>
+      <c r="O50" s="79"/>
+      <c r="P50" s="79"/>
+      <c r="Q50" s="79"/>
+      <c r="R50" s="79"/>
+      <c r="S50" s="85"/>
+      <c r="T50" s="92"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="81"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="79"/>
+      <c r="M51" s="80"/>
+      <c r="N51" s="77"/>
+      <c r="O51" s="79"/>
+      <c r="P51" s="79"/>
+      <c r="Q51" s="79"/>
+      <c r="R51" s="79"/>
+      <c r="S51" s="85"/>
+      <c r="T51" s="92"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="81"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="79"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="80"/>
+      <c r="N52" s="77"/>
+      <c r="O52" s="79"/>
+      <c r="P52" s="79"/>
+      <c r="Q52" s="79"/>
+      <c r="R52" s="79"/>
+      <c r="S52" s="85"/>
+      <c r="T52" s="92"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="81"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="80"/>
+      <c r="N53" s="77"/>
+      <c r="O53" s="79"/>
+      <c r="P53" s="79"/>
+      <c r="Q53" s="79"/>
+      <c r="R53" s="79"/>
+      <c r="S53" s="85"/>
+      <c r="T53" s="92"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="81"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="80"/>
+      <c r="N54" s="77"/>
+      <c r="O54" s="79"/>
+      <c r="P54" s="79"/>
+      <c r="Q54" s="79"/>
+      <c r="R54" s="79"/>
+      <c r="S54" s="85"/>
+      <c r="T54" s="92"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="81"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="79"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="79"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="80"/>
+      <c r="N55" s="77"/>
+      <c r="O55" s="79"/>
+      <c r="P55" s="79"/>
+      <c r="Q55" s="79"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="85"/>
+      <c r="T55" s="92"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="81"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="79"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="80"/>
+      <c r="N56" s="77"/>
+      <c r="O56" s="79"/>
+      <c r="P56" s="79"/>
+      <c r="Q56" s="79"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="85"/>
+      <c r="T56" s="92"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="81"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="77"/>
+      <c r="I57" s="79"/>
+      <c r="J57" s="79"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="80"/>
+      <c r="N57" s="77"/>
+      <c r="O57" s="79"/>
+      <c r="P57" s="79"/>
+      <c r="Q57" s="79"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="85"/>
+      <c r="T57" s="92"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="81"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="80"/>
+      <c r="N58" s="77"/>
+      <c r="O58" s="79"/>
+      <c r="P58" s="79"/>
+      <c r="Q58" s="79"/>
+      <c r="R58" s="79"/>
+      <c r="S58" s="85"/>
+      <c r="T58" s="92"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="81"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="79"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="77"/>
+      <c r="I59" s="79"/>
+      <c r="J59" s="79"/>
+      <c r="K59" s="79"/>
+      <c r="L59" s="79"/>
+      <c r="M59" s="80"/>
+      <c r="N59" s="77"/>
+      <c r="O59" s="79"/>
+      <c r="P59" s="79"/>
+      <c r="Q59" s="79"/>
+      <c r="R59" s="79"/>
+      <c r="S59" s="85"/>
+      <c r="T59" s="92"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="81"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="79"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="77"/>
+      <c r="I60" s="79"/>
+      <c r="J60" s="79"/>
+      <c r="K60" s="79"/>
+      <c r="L60" s="79"/>
+      <c r="M60" s="80"/>
+      <c r="N60" s="77"/>
+      <c r="O60" s="79"/>
+      <c r="P60" s="79"/>
+      <c r="Q60" s="79"/>
+      <c r="R60" s="79"/>
+      <c r="S60" s="85"/>
+      <c r="T60" s="92"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="81"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="79"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="77"/>
+      <c r="I61" s="79"/>
+      <c r="J61" s="79"/>
+      <c r="K61" s="79"/>
+      <c r="L61" s="79"/>
+      <c r="M61" s="80"/>
+      <c r="N61" s="77"/>
+      <c r="O61" s="79"/>
+      <c r="P61" s="79"/>
+      <c r="Q61" s="79"/>
+      <c r="R61" s="79"/>
+      <c r="S61" s="85"/>
+      <c r="T61" s="92"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="81"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="79"/>
+      <c r="F62" s="85"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="77"/>
+      <c r="I62" s="79"/>
+      <c r="J62" s="79"/>
+      <c r="K62" s="79"/>
+      <c r="L62" s="79"/>
+      <c r="M62" s="80"/>
+      <c r="N62" s="77"/>
+      <c r="O62" s="79"/>
+      <c r="P62" s="79"/>
+      <c r="Q62" s="79"/>
+      <c r="R62" s="79"/>
+      <c r="S62" s="85"/>
+      <c r="T62" s="92"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="81"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="80"/>
+      <c r="H63" s="77"/>
+      <c r="I63" s="79"/>
+      <c r="J63" s="79"/>
+      <c r="K63" s="79"/>
+      <c r="L63" s="79"/>
+      <c r="M63" s="80"/>
+      <c r="N63" s="77"/>
+      <c r="O63" s="79"/>
+      <c r="P63" s="79"/>
+      <c r="Q63" s="79"/>
+      <c r="R63" s="79"/>
+      <c r="S63" s="85"/>
+      <c r="T63" s="92"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="81"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="79"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="80"/>
+      <c r="H64" s="77"/>
+      <c r="I64" s="79"/>
+      <c r="J64" s="79"/>
+      <c r="K64" s="79"/>
+      <c r="L64" s="79"/>
+      <c r="M64" s="80"/>
+      <c r="N64" s="77"/>
+      <c r="O64" s="79"/>
+      <c r="P64" s="79"/>
+      <c r="Q64" s="79"/>
+      <c r="R64" s="79"/>
+      <c r="S64" s="85"/>
+      <c r="T64" s="92"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="81"/>
+      <c r="B65" s="52"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="79"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="80"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="79"/>
+      <c r="J65" s="79"/>
+      <c r="K65" s="79"/>
+      <c r="L65" s="79"/>
+      <c r="M65" s="80"/>
+      <c r="N65" s="77"/>
+      <c r="O65" s="79"/>
+      <c r="P65" s="79"/>
+      <c r="Q65" s="79"/>
+      <c r="R65" s="79"/>
+      <c r="S65" s="85"/>
+      <c r="T65" s="92"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="81"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="80"/>
+      <c r="H66" s="77"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="79"/>
+      <c r="K66" s="79"/>
+      <c r="L66" s="79"/>
+      <c r="M66" s="80"/>
+      <c r="N66" s="77"/>
+      <c r="O66" s="79"/>
+      <c r="P66" s="79"/>
+      <c r="Q66" s="79"/>
+      <c r="R66" s="79"/>
+      <c r="S66" s="85"/>
+      <c r="T66" s="92"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="81"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="79"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="80"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="79"/>
+      <c r="J67" s="79"/>
+      <c r="K67" s="79"/>
+      <c r="L67" s="79"/>
+      <c r="M67" s="80"/>
+      <c r="N67" s="77"/>
+      <c r="O67" s="79"/>
+      <c r="P67" s="79"/>
+      <c r="Q67" s="79"/>
+      <c r="R67" s="79"/>
+      <c r="S67" s="85"/>
+      <c r="T67" s="92"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="81"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="79"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="80"/>
+      <c r="H68" s="77"/>
+      <c r="I68" s="79"/>
+      <c r="J68" s="79"/>
+      <c r="K68" s="79"/>
+      <c r="L68" s="79"/>
+      <c r="M68" s="80"/>
+      <c r="N68" s="77"/>
+      <c r="O68" s="79"/>
+      <c r="P68" s="79"/>
+      <c r="Q68" s="79"/>
+      <c r="R68" s="79"/>
+      <c r="S68" s="85"/>
+      <c r="T68" s="92"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="81"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="85"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="77"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="79"/>
+      <c r="K69" s="79"/>
+      <c r="L69" s="79"/>
+      <c r="M69" s="80"/>
+      <c r="N69" s="77"/>
+      <c r="O69" s="79"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="79"/>
+      <c r="R69" s="79"/>
+      <c r="S69" s="85"/>
+      <c r="T69" s="92"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="81"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="79"/>
+      <c r="F70" s="85"/>
+      <c r="G70" s="80"/>
+      <c r="H70" s="77"/>
+      <c r="I70" s="79"/>
+      <c r="J70" s="79"/>
+      <c r="K70" s="79"/>
+      <c r="L70" s="79"/>
+      <c r="M70" s="80"/>
+      <c r="N70" s="77"/>
+      <c r="O70" s="79"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="79"/>
+      <c r="R70" s="79"/>
+      <c r="S70" s="85"/>
+      <c r="T70" s="92"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="81"/>
+      <c r="B71" s="52"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="79"/>
+      <c r="F71" s="85"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="77"/>
+      <c r="I71" s="79"/>
+      <c r="J71" s="79"/>
+      <c r="K71" s="79"/>
+      <c r="L71" s="79"/>
+      <c r="M71" s="80"/>
+      <c r="N71" s="77"/>
+      <c r="O71" s="79"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="79"/>
+      <c r="R71" s="79"/>
+      <c r="S71" s="85"/>
+      <c r="T71" s="92"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="81"/>
+      <c r="B72" s="52"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="79"/>
+      <c r="F72" s="85"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="77"/>
+      <c r="I72" s="79"/>
+      <c r="J72" s="79"/>
+      <c r="K72" s="79"/>
+      <c r="L72" s="79"/>
+      <c r="M72" s="80"/>
+      <c r="N72" s="77"/>
+      <c r="O72" s="79"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="79"/>
+      <c r="R72" s="79"/>
+      <c r="S72" s="85"/>
+      <c r="T72" s="92"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="81"/>
+      <c r="B73" s="52"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="79"/>
+      <c r="F73" s="85"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="79"/>
+      <c r="J73" s="79"/>
+      <c r="K73" s="79"/>
+      <c r="L73" s="79"/>
+      <c r="M73" s="80"/>
+      <c r="N73" s="77"/>
+      <c r="O73" s="79"/>
+      <c r="P73" s="79"/>
+      <c r="Q73" s="79"/>
+      <c r="R73" s="79"/>
+      <c r="S73" s="85"/>
+      <c r="T73" s="92"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="81"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="79"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="80"/>
+      <c r="H74" s="77"/>
+      <c r="I74" s="79"/>
+      <c r="J74" s="79"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="80"/>
+      <c r="N74" s="77"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="79"/>
+      <c r="Q74" s="79"/>
+      <c r="R74" s="79"/>
+      <c r="S74" s="85"/>
+      <c r="T74" s="92"/>
+    </row>
+    <row r="75" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="82"/>
+      <c r="B75" s="83"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="83"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="85"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="77"/>
+      <c r="I75" s="79"/>
+      <c r="J75" s="79"/>
+      <c r="K75" s="79"/>
+      <c r="L75" s="79"/>
+      <c r="M75" s="80"/>
+      <c r="N75" s="77"/>
+      <c r="O75" s="79"/>
+      <c r="P75" s="79"/>
+      <c r="Q75" s="79"/>
+      <c r="R75" s="79"/>
+      <c r="S75" s="85"/>
+      <c r="T75" s="93"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:T16" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
+  <mergeCells count="4">
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="T1:T2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="T3:T75">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="NOK">
+      <formula>LEFT(T3,LEN("NOK"))="NOK"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="OK">
+      <formula>LEFT(T3,LEN("OK"))="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G75" xr:uid="{4832D533-7A08-40E1-9AA1-2EB7D4098823}">
+      <formula1>"Solo tazze, Solo bordi, Bordi e tazze,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K75 Q3:Q75" xr:uid="{1680938F-FEBA-4BD0-AD9E-C379B9D51075}">
+      <formula1>"1,2,3,4,5,6,7,-,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L75 R3:R75" xr:uid="{52775BBC-9B41-4CCF-8CE4-E19D926CD49C}">
+      <formula1>"Cassa in ferro, Cassa in legno,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M75 S3:S75" xr:uid="{F60DF200-FBE7-451E-8A72-514BC952C463}">
+      <formula1>"1,2,-,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F75" xr:uid="{5865F76D-6592-4088-891A-E3BB5A14F46D}">
+      <formula1>"Aperto, Chiuso,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E75" xr:uid="{D3B60138-7714-448B-8CA2-3F4C37A74F08}">
+      <formula1>"40,50,60,80,100,120,140,160,200,240,280,300,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T75" xr:uid="{ACF13385-C338-4011-A851-2E1C2C226567}">
+      <formula1>"OK,NOK,"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sopra i 25m vado in ogni caso con la cassa in ferro.
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758DA11A-09AA-4A58-9CD6-BFBE87EE9B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8D69A9-E052-49C1-8147-2EDE109A1CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="SimulazioneConf7" sheetId="6" r:id="rId4"/>
     <sheet name="SimulazioneConf6" sheetId="4" r:id="rId5"/>
     <sheet name="Database" sheetId="7" r:id="rId6"/>
+    <sheet name="Trasporti" sheetId="8" r:id="rId7"/>
+    <sheet name="Rinforzi" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -100,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="138">
   <si>
     <t>Diagonali</t>
   </si>
@@ -437,6 +439,87 @@
   </si>
   <si>
     <t>Solo bordi</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>Da ricontrollare l'altezza e salvare immagine. In base alla foto l'altezza non può essere 2240, perchè se si considerano 9 strati di bordo da 200 + l'altezza del nastro, non ci stiamo dentro.</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Trasporto</t>
+  </si>
+  <si>
+    <t>Nave; Camion;</t>
+  </si>
+  <si>
+    <t>Camion STD</t>
+  </si>
+  <si>
+    <t>Camion</t>
+  </si>
+  <si>
+    <t>Open top</t>
+  </si>
+  <si>
+    <t>Fuori std</t>
+  </si>
+  <si>
+    <t>Diagonali ad incrocio</t>
+  </si>
+  <si>
+    <t>Fondo in lamiera</t>
+  </si>
+  <si>
+    <t>Cassa solo ritti</t>
+  </si>
+  <si>
+    <t>Criterio 1</t>
+  </si>
+  <si>
+    <t>Criterio 2</t>
+  </si>
+  <si>
+    <t>Criterio 3</t>
+  </si>
+  <si>
+    <t>SIG</t>
+  </si>
+  <si>
+    <t>L&lt;6m</t>
+  </si>
+  <si>
+    <t>20ft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 ft </t>
+  </si>
+  <si>
+    <t>40 ft HC</t>
+  </si>
+  <si>
+    <t>Altezza porta [mm]</t>
+  </si>
+  <si>
+    <t>Larghezza porta [mm]</t>
+  </si>
+  <si>
+    <t>28/'1/2022</t>
+  </si>
+  <si>
+    <t>Al momento questo nastro non è calcolabile</t>
+  </si>
+  <si>
+    <t>Da verificare</t>
+  </si>
+  <si>
+    <t>Da capire. Fare prova con 100m se ci sta negli 11,8</t>
+  </si>
+  <si>
+    <t>Ricontrollare versione nuova</t>
   </si>
 </sst>
 </file>
@@ -447,7 +530,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +589,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -550,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1068,6 +1157,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1075,7 +1175,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1196,6 +1296,88 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1229,8 +1411,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1241,80 +1429,32 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2792,10 +2932,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="87"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3329,21 +3469,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="58" t="s">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="61" t="s">
+      <c r="H1" s="89"/>
+      <c r="I1" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="91" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3372,8 +3512,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -3837,14 +3977,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4272,14 +4412,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4425,7 +4565,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="94" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -4448,7 +4588,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="65"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -4469,7 +4609,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="65"/>
+      <c r="F18" s="95"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -4481,7 +4621,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="65"/>
+      <c r="F19" s="95"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -4493,7 +4633,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="65"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -4505,7 +4645,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="65"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -4517,7 +4657,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="65"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -4529,7 +4669,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="66"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -4725,14 +4865,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5048,14 +5188,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -5073,178 +5213,185 @@
     <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="100" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="71" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="71" t="s">
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="94" t="s">
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="103" t="s">
         <v>107</v>
       </c>
+      <c r="U1" s="103" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="2" spans="1:33" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="75" t="s">
+      <c r="K2" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="75" t="s">
+      <c r="L2" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="N2" s="74" t="s">
+      <c r="N2" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="75" t="s">
+      <c r="O2" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="75" t="s">
+      <c r="P2" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="Q2" s="75" t="s">
+      <c r="Q2" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="75" t="s">
+      <c r="R2" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="S2" s="76" t="s">
+      <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="95"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67"/>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="67"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="56"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="77">
+      <c r="A3" s="60">
         <v>20210538</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="61">
         <v>44566</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="62">
         <v>10200</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="62">
         <v>400</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="62">
         <v>100</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="77">
+      <c r="H3" s="60">
         <v>1200</v>
       </c>
-      <c r="I3" s="87">
+      <c r="I3" s="70">
         <v>800</v>
       </c>
-      <c r="J3" s="79">
+      <c r="J3" s="62">
         <v>600</v>
       </c>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L3" s="79" t="s">
+      <c r="L3" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="80" t="s">
+      <c r="M3" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="77">
+      <c r="N3" s="60">
         <v>1200</v>
       </c>
-      <c r="O3" s="79">
+      <c r="O3" s="62">
         <v>1200</v>
       </c>
-      <c r="P3" s="79">
+      <c r="P3" s="62">
         <v>600</v>
       </c>
-      <c r="Q3" s="79" t="s">
+      <c r="Q3" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R3" s="79" t="s">
+      <c r="R3" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S3" s="85" t="s">
+      <c r="S3" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T3" s="91" t="s">
+      <c r="T3" s="73" t="s">
         <v>108</v>
       </c>
+      <c r="U3" s="76" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="81">
+      <c r="A4" s="64">
         <v>20210304</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B4" s="69">
         <v>44411</v>
       </c>
       <c r="C4" s="52">
@@ -5253,60 +5400,61 @@
       <c r="D4" s="52">
         <v>1200</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="62">
         <v>120</v>
       </c>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="G4" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="88">
+      <c r="H4" s="106">
         <v>2400</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="107">
         <v>2400</v>
       </c>
-      <c r="J4" s="87">
+      <c r="J4" s="107">
         <v>1400</v>
       </c>
-      <c r="K4" s="79" t="s">
+      <c r="K4" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="79" t="s">
+      <c r="L4" s="107" t="s">
         <v>103</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="M4" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="88">
+      <c r="N4" s="106">
         <v>3700</v>
       </c>
-      <c r="O4" s="87">
+      <c r="O4" s="107">
         <v>1350</v>
       </c>
-      <c r="P4" s="87">
+      <c r="P4" s="107">
         <v>2200</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S4" s="85">
+      <c r="S4" s="68">
         <v>1</v>
       </c>
-      <c r="T4" s="92" t="s">
-        <v>108</v>
-      </c>
+      <c r="T4" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" s="77"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="81">
+      <c r="A5" s="64">
         <v>20210152</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B5" s="69">
         <v>44445</v>
       </c>
       <c r="C5" s="52">
@@ -5315,60 +5463,61 @@
       <c r="D5" s="52">
         <v>650</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="62">
         <v>200</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="106">
         <v>7000</v>
       </c>
-      <c r="I5" s="87">
+      <c r="I5" s="107">
         <v>790</v>
       </c>
-      <c r="J5" s="79">
+      <c r="J5" s="107">
         <v>2240</v>
       </c>
-      <c r="K5" s="79">
+      <c r="K5" s="107">
         <v>7</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="89">
+      <c r="M5" s="108">
         <v>1</v>
       </c>
-      <c r="N5" s="88">
+      <c r="N5" s="106">
         <v>5000</v>
       </c>
-      <c r="O5" s="87">
+      <c r="O5" s="107">
         <v>1600</v>
       </c>
-      <c r="P5" s="79">
+      <c r="P5" s="62">
         <v>2240</v>
       </c>
-      <c r="Q5" s="79" t="s">
+      <c r="Q5" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R5" s="79" t="s">
+      <c r="R5" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S5" s="90">
+      <c r="S5" s="72">
         <v>2</v>
       </c>
-      <c r="T5" s="92" t="s">
-        <v>108</v>
-      </c>
+      <c r="T5" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" s="77"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="81">
+      <c r="A6" s="64">
         <v>20210164</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="69">
         <v>44407</v>
       </c>
       <c r="C6" s="52">
@@ -5377,60 +5526,63 @@
       <c r="D6" s="52">
         <v>1000</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E6" s="62">
         <v>240</v>
       </c>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="88">
+      <c r="H6" s="71">
         <v>8400</v>
       </c>
-      <c r="I6" s="79">
+      <c r="I6" s="62">
         <v>2230</v>
       </c>
-      <c r="J6" s="79">
+      <c r="J6" s="62">
         <v>2530</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="62">
         <v>7</v>
       </c>
-      <c r="L6" s="79" t="s">
+      <c r="L6" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="80">
+      <c r="M6" s="63">
         <v>2</v>
       </c>
-      <c r="N6" s="88">
+      <c r="N6" s="71">
         <v>9500</v>
       </c>
-      <c r="O6" s="79">
+      <c r="O6" s="62">
         <v>2300</v>
       </c>
-      <c r="P6" s="79">
+      <c r="P6" s="62">
         <v>2450</v>
       </c>
-      <c r="Q6" s="79" t="s">
+      <c r="Q6" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R6" s="79" t="s">
+      <c r="R6" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S6" s="85">
+      <c r="S6" s="68">
         <v>2</v>
       </c>
-      <c r="T6" s="92" t="s">
+      <c r="T6" s="74" t="s">
         <v>108</v>
       </c>
+      <c r="U6" s="77" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="81">
+      <c r="A7" s="64">
         <v>20210296</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="69">
         <v>44414</v>
       </c>
       <c r="C7" s="52">
@@ -5439,60 +5591,61 @@
       <c r="D7" s="52">
         <v>650</v>
       </c>
-      <c r="E7" s="79">
+      <c r="E7" s="62">
         <v>120</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="80" t="s">
+      <c r="G7" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="88">
+      <c r="H7" s="106">
         <v>2000</v>
       </c>
-      <c r="I7" s="87">
+      <c r="I7" s="107">
         <v>2000</v>
       </c>
-      <c r="J7" s="79">
+      <c r="J7" s="62">
         <v>850</v>
       </c>
-      <c r="K7" s="79" t="s">
+      <c r="K7" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M7" s="80" t="s">
+      <c r="M7" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N7" s="77">
+      <c r="N7" s="60">
         <v>1800</v>
       </c>
-      <c r="O7" s="79">
+      <c r="O7" s="62">
         <v>1800</v>
       </c>
-      <c r="P7" s="79">
+      <c r="P7" s="62">
         <v>800</v>
       </c>
-      <c r="Q7" s="79" t="s">
+      <c r="Q7" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R7" s="79" t="s">
+      <c r="R7" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S7" s="85" t="s">
+      <c r="S7" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T7" s="92" t="s">
-        <v>108</v>
-      </c>
+      <c r="T7" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="77"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="81">
+      <c r="A8" s="64">
         <v>20210250</v>
       </c>
-      <c r="B8" s="86">
+      <c r="B8" s="69">
         <v>44362</v>
       </c>
       <c r="C8" s="52">
@@ -5501,60 +5654,61 @@
       <c r="D8" s="52">
         <v>800</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="62">
         <v>50</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="80" t="s">
+      <c r="G8" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="60">
         <v>1200</v>
       </c>
-      <c r="I8" s="79">
+      <c r="I8" s="62">
         <v>800</v>
       </c>
-      <c r="J8" s="79">
+      <c r="J8" s="62">
         <v>1000</v>
       </c>
-      <c r="K8" s="79" t="s">
+      <c r="K8" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L8" s="79" t="s">
+      <c r="L8" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M8" s="80" t="s">
+      <c r="M8" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N8" s="77">
+      <c r="N8" s="60">
         <v>1200</v>
       </c>
-      <c r="O8" s="79">
+      <c r="O8" s="62">
         <v>800</v>
       </c>
-      <c r="P8" s="79">
+      <c r="P8" s="62">
         <v>950</v>
       </c>
-      <c r="Q8" s="79" t="s">
+      <c r="Q8" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R8" s="79" t="s">
+      <c r="R8" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S8" s="85" t="s">
+      <c r="S8" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T8" s="92" t="s">
+      <c r="T8" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U8" s="77"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="81">
+      <c r="A9" s="64">
         <v>20210187</v>
       </c>
-      <c r="B9" s="86">
+      <c r="B9" s="69">
         <v>44326</v>
       </c>
       <c r="C9" s="52">
@@ -5563,60 +5717,61 @@
       <c r="D9" s="52">
         <v>300</v>
       </c>
-      <c r="E9" s="79">
+      <c r="E9" s="62">
         <v>80</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="80" t="s">
+      <c r="G9" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="60">
         <v>1400</v>
       </c>
-      <c r="I9" s="79">
+      <c r="I9" s="62">
         <v>1400</v>
       </c>
-      <c r="J9" s="79">
+      <c r="J9" s="62">
         <v>500</v>
       </c>
-      <c r="K9" s="79" t="s">
+      <c r="K9" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M9" s="80" t="s">
+      <c r="M9" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="77">
+      <c r="N9" s="60">
         <v>1350</v>
       </c>
-      <c r="O9" s="79">
+      <c r="O9" s="62">
         <v>1350</v>
       </c>
-      <c r="P9" s="79">
+      <c r="P9" s="62">
         <v>50</v>
       </c>
-      <c r="Q9" s="79" t="s">
+      <c r="Q9" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R9" s="79" t="s">
+      <c r="R9" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S9" s="85" t="s">
+      <c r="S9" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T9" s="92" t="s">
+      <c r="T9" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U9" s="77"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="81">
+      <c r="A10" s="64">
         <v>20210272</v>
       </c>
-      <c r="B10" s="86">
+      <c r="B10" s="69">
         <v>44398</v>
       </c>
       <c r="C10" s="52">
@@ -5625,60 +5780,61 @@
       <c r="D10" s="52">
         <v>650</v>
       </c>
-      <c r="E10" s="79">
+      <c r="E10" s="62">
         <v>80</v>
       </c>
-      <c r="F10" s="85" t="s">
+      <c r="F10" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="G10" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="60">
         <v>1800</v>
       </c>
-      <c r="I10" s="79">
+      <c r="I10" s="62">
         <v>1800</v>
       </c>
-      <c r="J10" s="79">
+      <c r="J10" s="62">
         <v>850</v>
       </c>
-      <c r="K10" s="79" t="s">
+      <c r="K10" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L10" s="79" t="s">
+      <c r="L10" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M10" s="80" t="s">
+      <c r="M10" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="77">
+      <c r="N10" s="60">
         <v>1800</v>
       </c>
-      <c r="O10" s="79">
+      <c r="O10" s="62">
         <v>1800</v>
       </c>
-      <c r="P10" s="79">
+      <c r="P10" s="62">
         <v>900</v>
       </c>
-      <c r="Q10" s="79" t="s">
+      <c r="Q10" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R10" s="79" t="s">
+      <c r="R10" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S10" s="85" t="s">
+      <c r="S10" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T10" s="92" t="s">
+      <c r="T10" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U10" s="77"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="81">
+      <c r="A11" s="64">
         <v>20210264</v>
       </c>
-      <c r="B11" s="86">
+      <c r="B11" s="69">
         <v>44393</v>
       </c>
       <c r="C11" s="52">
@@ -5687,60 +5843,61 @@
       <c r="D11" s="52">
         <v>1000</v>
       </c>
-      <c r="E11" s="79">
+      <c r="E11" s="62">
         <v>100</v>
       </c>
-      <c r="F11" s="85" t="s">
+      <c r="F11" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="80" t="s">
+      <c r="G11" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="60">
         <v>1400</v>
       </c>
-      <c r="I11" s="79">
+      <c r="I11" s="62">
         <v>1400</v>
       </c>
-      <c r="J11" s="79">
+      <c r="J11" s="62">
         <v>1200</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L11" s="79" t="s">
+      <c r="L11" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M11" s="80" t="s">
+      <c r="M11" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N11" s="77">
+      <c r="N11" s="60">
         <v>1300</v>
       </c>
-      <c r="O11" s="79">
+      <c r="O11" s="62">
         <v>1300</v>
       </c>
-      <c r="P11" s="79">
+      <c r="P11" s="62">
         <v>1200</v>
       </c>
-      <c r="Q11" s="79" t="s">
+      <c r="Q11" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R11" s="79" t="s">
+      <c r="R11" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S11" s="85" t="s">
+      <c r="S11" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T11" s="92" t="s">
+      <c r="T11" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U11" s="77"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="81">
+      <c r="A12" s="64">
         <v>20210235</v>
       </c>
-      <c r="B12" s="86">
+      <c r="B12" s="69">
         <v>44382</v>
       </c>
       <c r="C12" s="52">
@@ -5749,60 +5906,61 @@
       <c r="D12" s="52">
         <v>1400</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="62">
         <v>100</v>
       </c>
-      <c r="F12" s="85" t="s">
+      <c r="F12" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="60">
         <v>1800</v>
       </c>
-      <c r="I12" s="79">
+      <c r="I12" s="62">
         <v>1800</v>
       </c>
-      <c r="J12" s="79">
+      <c r="J12" s="62">
         <v>1600</v>
       </c>
-      <c r="K12" s="79" t="s">
+      <c r="K12" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="79" t="s">
+      <c r="L12" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M12" s="80" t="s">
+      <c r="M12" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N12" s="77">
+      <c r="N12" s="60">
         <v>2000</v>
       </c>
-      <c r="O12" s="79">
+      <c r="O12" s="62">
         <v>1800</v>
       </c>
-      <c r="P12" s="79">
+      <c r="P12" s="62">
         <v>1600</v>
       </c>
-      <c r="Q12" s="79" t="s">
+      <c r="Q12" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R12" s="79" t="s">
+      <c r="R12" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S12" s="85" t="s">
+      <c r="S12" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T12" s="92" t="s">
+      <c r="T12" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U12" s="77"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="81">
+      <c r="A13" s="64">
         <v>20210245</v>
       </c>
-      <c r="B13" s="86">
+      <c r="B13" s="69">
         <v>44412</v>
       </c>
       <c r="C13" s="52">
@@ -5811,60 +5969,61 @@
       <c r="D13" s="52">
         <v>1200</v>
       </c>
-      <c r="E13" s="79">
+      <c r="E13" s="62">
         <v>80</v>
       </c>
-      <c r="F13" s="85" t="s">
+      <c r="F13" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="80" t="s">
+      <c r="G13" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="77">
+      <c r="H13" s="60">
         <v>1800</v>
       </c>
-      <c r="I13" s="79">
+      <c r="I13" s="62">
         <v>1800</v>
       </c>
-      <c r="J13" s="79">
+      <c r="J13" s="62">
         <v>1400</v>
       </c>
-      <c r="K13" s="79" t="s">
+      <c r="K13" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L13" s="79" t="s">
+      <c r="L13" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M13" s="80" t="s">
+      <c r="M13" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N13" s="77">
+      <c r="N13" s="60">
         <v>1800</v>
       </c>
-      <c r="O13" s="79">
+      <c r="O13" s="62">
         <v>1800</v>
       </c>
-      <c r="P13" s="79">
+      <c r="P13" s="62">
         <v>1400</v>
       </c>
-      <c r="Q13" s="79" t="s">
+      <c r="Q13" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="R13" s="79" t="s">
+      <c r="R13" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="S13" s="85" t="s">
+      <c r="S13" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T13" s="92" t="s">
+      <c r="T13" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U13" s="77"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="81">
+      <c r="A14" s="64">
         <v>20200269</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B14" s="69">
         <v>44119</v>
       </c>
       <c r="C14" s="52">
@@ -5873,60 +6032,61 @@
       <c r="D14" s="52">
         <v>800</v>
       </c>
-      <c r="E14" s="79">
+      <c r="E14" s="62">
         <v>240</v>
       </c>
-      <c r="F14" s="85" t="s">
+      <c r="F14" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="80" t="s">
+      <c r="G14" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="77">
+      <c r="H14" s="60">
         <v>7600</v>
       </c>
-      <c r="I14" s="79">
+      <c r="I14" s="62">
         <v>1830</v>
       </c>
-      <c r="J14" s="79">
+      <c r="J14" s="62">
         <v>2240</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="62">
         <v>7</v>
       </c>
-      <c r="L14" s="79" t="s">
+      <c r="L14" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="80">
+      <c r="M14" s="63">
         <v>2</v>
       </c>
-      <c r="N14" s="77">
+      <c r="N14" s="60">
         <v>8000</v>
       </c>
-      <c r="O14" s="79">
+      <c r="O14" s="62">
         <v>1900</v>
       </c>
-      <c r="P14" s="79">
+      <c r="P14" s="62">
         <v>2240</v>
       </c>
-      <c r="Q14" s="79">
+      <c r="Q14" s="62">
         <v>7</v>
       </c>
-      <c r="R14" s="79" t="s">
+      <c r="R14" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S14" s="85">
+      <c r="S14" s="68">
         <v>2</v>
       </c>
-      <c r="T14" s="92" t="s">
+      <c r="T14" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U14" s="77"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="81">
+      <c r="A15" s="64">
         <v>20200368</v>
       </c>
-      <c r="B15" s="86">
+      <c r="B15" s="69">
         <v>44144</v>
       </c>
       <c r="C15" s="52">
@@ -5935,60 +6095,61 @@
       <c r="D15" s="52">
         <v>650</v>
       </c>
-      <c r="E15" s="79">
+      <c r="E15" s="62">
         <v>120</v>
       </c>
-      <c r="F15" s="85" t="s">
+      <c r="F15" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="80" t="s">
+      <c r="G15" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H15" s="77">
+      <c r="H15" s="60">
         <v>3800</v>
       </c>
-      <c r="I15" s="79">
+      <c r="I15" s="62">
         <v>790</v>
       </c>
-      <c r="J15" s="79">
+      <c r="J15" s="62">
         <v>2240</v>
       </c>
-      <c r="K15" s="79">
+      <c r="K15" s="62">
         <v>1</v>
       </c>
-      <c r="L15" s="79" t="s">
+      <c r="L15" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="M15" s="80">
+      <c r="M15" s="63">
         <v>1</v>
       </c>
-      <c r="N15" s="77">
+      <c r="N15" s="60">
         <v>3000</v>
       </c>
-      <c r="O15" s="79">
+      <c r="O15" s="62">
         <v>800</v>
       </c>
-      <c r="P15" s="79">
+      <c r="P15" s="62">
         <v>2240</v>
       </c>
-      <c r="Q15" s="79">
+      <c r="Q15" s="62">
         <v>3</v>
       </c>
-      <c r="R15" s="79" t="s">
+      <c r="R15" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S15" s="85">
+      <c r="S15" s="68">
         <v>1</v>
       </c>
-      <c r="T15" s="92" t="s">
+      <c r="T15" s="74" t="s">
         <v>23</v>
       </c>
+      <c r="U15" s="77"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="81">
+      <c r="A16" s="64">
         <v>20200306</v>
       </c>
-      <c r="B16" s="86">
+      <c r="B16" s="69">
         <v>44109</v>
       </c>
       <c r="C16" s="52">
@@ -5997,1360 +6158,1653 @@
       <c r="D16" s="52">
         <v>800</v>
       </c>
-      <c r="E16" s="79">
+      <c r="E16" s="62">
         <v>80</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="77">
+      <c r="H16" s="60">
         <v>2000</v>
       </c>
-      <c r="I16" s="79">
+      <c r="I16" s="62">
         <v>2000</v>
       </c>
-      <c r="J16" s="79">
+      <c r="J16" s="62">
         <v>1000</v>
       </c>
-      <c r="K16" s="79" t="s">
+      <c r="K16" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L16" s="79" t="s">
+      <c r="L16" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="M16" s="80" t="s">
+      <c r="M16" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="88">
+      <c r="N16" s="106">
         <v>3000</v>
       </c>
-      <c r="O16" s="87">
+      <c r="O16" s="107">
         <v>1000</v>
       </c>
-      <c r="P16" s="87">
+      <c r="P16" s="107">
         <v>2240</v>
       </c>
-      <c r="Q16" s="79" t="s">
+      <c r="Q16" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="R16" s="87" t="s">
+      <c r="R16" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="S16" s="85">
+      <c r="S16" s="68">
         <v>1</v>
       </c>
-      <c r="T16" s="92" t="s">
+      <c r="T16" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" s="77"/>
+    </row>
+    <row r="17" spans="1:21" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
+        <v>20210468</v>
+      </c>
+      <c r="B17" s="79">
+        <v>44592</v>
+      </c>
+      <c r="C17" s="17">
+        <v>48000</v>
+      </c>
+      <c r="D17" s="17">
+        <v>650</v>
+      </c>
+      <c r="E17" s="80">
+        <v>200</v>
+      </c>
+      <c r="F17" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="109">
+        <v>6700</v>
+      </c>
+      <c r="I17" s="110">
+        <v>790</v>
+      </c>
+      <c r="J17" s="110">
+        <v>2240</v>
+      </c>
+      <c r="K17" s="110">
+        <v>7</v>
+      </c>
+      <c r="L17" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="M17" s="111">
+        <v>1</v>
+      </c>
+      <c r="N17" s="109">
+        <v>6000</v>
+      </c>
+      <c r="O17" s="110">
+        <v>800</v>
+      </c>
+      <c r="P17" s="110">
+        <v>2450</v>
+      </c>
+      <c r="Q17" s="80">
+        <v>7</v>
+      </c>
+      <c r="R17" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="S17" s="81">
+        <v>1</v>
+      </c>
+      <c r="T17" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="U17" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="64">
+        <v>20210423</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="52">
+        <v>23700</v>
+      </c>
+      <c r="D18" s="52">
+        <v>650</v>
+      </c>
+      <c r="E18" s="62">
+        <v>120</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="60">
+        <v>2000</v>
+      </c>
+      <c r="I18" s="62">
+        <v>2000</v>
+      </c>
+      <c r="J18" s="62">
+        <v>850</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="L18" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N18" s="60">
+        <v>2000</v>
+      </c>
+      <c r="O18" s="62">
+        <v>2000</v>
+      </c>
+      <c r="P18" s="62">
+        <v>850</v>
+      </c>
+      <c r="Q18" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="S18" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="T18" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U18" s="77"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="64">
+        <v>20210312</v>
+      </c>
+      <c r="B19" s="69">
+        <v>44589</v>
+      </c>
+      <c r="C19" s="52">
+        <v>120000</v>
+      </c>
+      <c r="D19" s="52">
+        <v>1400</v>
+      </c>
+      <c r="E19" s="62">
+        <v>400</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="60"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="60">
+        <v>13600</v>
+      </c>
+      <c r="O19" s="62">
+        <v>2220</v>
+      </c>
+      <c r="P19" s="62">
+        <v>3000</v>
+      </c>
+      <c r="Q19" s="62">
+        <v>7</v>
+      </c>
+      <c r="R19" s="62"/>
+      <c r="S19" s="68">
+        <v>1</v>
+      </c>
+      <c r="T19" s="74" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="80"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
-      <c r="S17" s="85"/>
-      <c r="T17" s="92"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="77"/>
-      <c r="O18" s="79"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="79"/>
-      <c r="S18" s="85"/>
-      <c r="T18" s="92"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="81"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="92"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="85"/>
-      <c r="T20" s="92"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="81"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="85"/>
-      <c r="T21" s="92"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="81"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="79"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="85"/>
-      <c r="T22" s="92"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="81"/>
+      <c r="U19" s="77" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
+        <v>20210133</v>
+      </c>
+      <c r="B20" s="69">
+        <v>44586</v>
+      </c>
+      <c r="C20" s="52">
+        <v>101500</v>
+      </c>
+      <c r="D20" s="52">
+        <v>1000</v>
+      </c>
+      <c r="E20" s="62">
+        <v>180</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="60">
+        <v>7100</v>
+      </c>
+      <c r="I20" s="62">
+        <v>2230</v>
+      </c>
+      <c r="J20" s="70">
+        <v>1680</v>
+      </c>
+      <c r="K20" s="62">
+        <v>1</v>
+      </c>
+      <c r="L20" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" s="63">
+        <v>2</v>
+      </c>
+      <c r="N20" s="60">
+        <v>11800</v>
+      </c>
+      <c r="O20" s="62">
+        <v>1150</v>
+      </c>
+      <c r="P20" s="62">
+        <v>2240</v>
+      </c>
+      <c r="Q20" s="62">
+        <v>7</v>
+      </c>
+      <c r="R20" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S20" s="68">
+        <v>1</v>
+      </c>
+      <c r="T20" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="U20" s="77" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
+        <v>20210277</v>
+      </c>
+      <c r="B21" s="69">
+        <v>44592</v>
+      </c>
+      <c r="C21" s="52">
+        <v>48000</v>
+      </c>
+      <c r="D21" s="52">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="62">
+        <v>200</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="60">
+        <v>6700</v>
+      </c>
+      <c r="I21" s="62">
+        <v>1340</v>
+      </c>
+      <c r="J21" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K21" s="62">
+        <v>7</v>
+      </c>
+      <c r="L21" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M21" s="63">
+        <v>1</v>
+      </c>
+      <c r="N21" s="60">
+        <v>6500</v>
+      </c>
+      <c r="O21" s="62">
+        <v>1400</v>
+      </c>
+      <c r="P21" s="62">
+        <v>2050</v>
+      </c>
+      <c r="Q21" s="62">
+        <v>7</v>
+      </c>
+      <c r="R21" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S21" s="68">
+        <v>1</v>
+      </c>
+      <c r="T21" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" s="77"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
+        <v>20210528</v>
+      </c>
+      <c r="B22" s="69">
+        <v>44602</v>
+      </c>
+      <c r="C22" s="52">
+        <v>108110</v>
+      </c>
+      <c r="D22" s="52">
+        <v>1000</v>
+      </c>
+      <c r="E22" s="62">
+        <v>200</v>
+      </c>
+      <c r="F22" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="60">
+        <v>7600</v>
+      </c>
+      <c r="I22" s="62">
+        <v>2230</v>
+      </c>
+      <c r="J22" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K22" s="62">
+        <v>7</v>
+      </c>
+      <c r="L22" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M22" s="63">
+        <v>2</v>
+      </c>
+      <c r="N22" s="60">
+        <v>11000</v>
+      </c>
+      <c r="O22" s="62">
+        <v>2300</v>
+      </c>
+      <c r="P22" s="62">
+        <v>2240</v>
+      </c>
+      <c r="Q22" s="62">
+        <v>1</v>
+      </c>
+      <c r="R22" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S22" s="68">
+        <v>2</v>
+      </c>
+      <c r="T22" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="77"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="64"/>
       <c r="B23" s="52"/>
       <c r="C23" s="52"/>
       <c r="D23" s="52"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="80"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="85"/>
-      <c r="T23" s="92"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="68"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="77"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="64"/>
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
       <c r="D24" s="52"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="85"/>
-      <c r="T24" s="92"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="62"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62"/>
+      <c r="S24" s="68"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="77"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="64"/>
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="52"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="79"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="79"/>
-      <c r="S25" s="85"/>
-      <c r="T25" s="92"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="68"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="77"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="64"/>
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
       <c r="D26" s="52"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="85"/>
-      <c r="T26" s="92"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62"/>
+      <c r="S26" s="68"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="77"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="64"/>
       <c r="B27" s="52"/>
       <c r="C27" s="52"/>
       <c r="D27" s="52"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="85"/>
-      <c r="T27" s="92"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="74"/>
+      <c r="U27" s="77"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="64"/>
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="77"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="79"/>
-      <c r="S28" s="85"/>
-      <c r="T28" s="92"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="81"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="74"/>
+      <c r="U28" s="77"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="64"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="80"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="79"/>
-      <c r="S29" s="85"/>
-      <c r="T29" s="92"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="81"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="62"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="77"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="64"/>
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="52"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="80"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="79"/>
-      <c r="P30" s="79"/>
-      <c r="Q30" s="79"/>
-      <c r="R30" s="79"/>
-      <c r="S30" s="85"/>
-      <c r="T30" s="92"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="81"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="62"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="62"/>
+      <c r="S30" s="68"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="77"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="64"/>
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
       <c r="D31" s="52"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="80"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="79"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="79"/>
-      <c r="R31" s="79"/>
-      <c r="S31" s="85"/>
-      <c r="T31" s="92"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="81"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="77"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="64"/>
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
       <c r="D32" s="52"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="79"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
-      <c r="M32" s="80"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="79"/>
-      <c r="P32" s="79"/>
-      <c r="Q32" s="79"/>
-      <c r="R32" s="79"/>
-      <c r="S32" s="85"/>
-      <c r="T32" s="92"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="81"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="62"/>
+      <c r="R32" s="62"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="74"/>
+      <c r="U32" s="77"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="64"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
       <c r="D33" s="52"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="80"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="79"/>
-      <c r="P33" s="79"/>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="79"/>
-      <c r="S33" s="85"/>
-      <c r="T33" s="92"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="74"/>
+      <c r="U33" s="77"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="64"/>
       <c r="B34" s="52"/>
       <c r="C34" s="52"/>
       <c r="D34" s="52"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="79"/>
-      <c r="P34" s="79"/>
-      <c r="Q34" s="79"/>
-      <c r="R34" s="79"/>
-      <c r="S34" s="85"/>
-      <c r="T34" s="92"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="81"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+      <c r="Q34" s="62"/>
+      <c r="R34" s="62"/>
+      <c r="S34" s="68"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="77"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="64"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
       <c r="D35" s="52"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="79"/>
-      <c r="S35" s="85"/>
-      <c r="T35" s="92"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="68"/>
+      <c r="T35" s="74"/>
+      <c r="U35" s="77"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="64"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
       <c r="D36" s="52"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="85"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="80"/>
-      <c r="N36" s="77"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="79"/>
-      <c r="R36" s="79"/>
-      <c r="S36" s="85"/>
-      <c r="T36" s="92"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="81"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="68"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="77"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="64"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
       <c r="D37" s="52"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="79"/>
-      <c r="S37" s="85"/>
-      <c r="T37" s="92"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="81"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="62"/>
+      <c r="R37" s="62"/>
+      <c r="S37" s="68"/>
+      <c r="T37" s="74"/>
+      <c r="U37" s="77"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="64"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
       <c r="D38" s="52"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="80"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="79"/>
-      <c r="R38" s="79"/>
-      <c r="S38" s="85"/>
-      <c r="T38" s="92"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="81"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
+      <c r="R38" s="62"/>
+      <c r="S38" s="68"/>
+      <c r="T38" s="74"/>
+      <c r="U38" s="77"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="64"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
       <c r="D39" s="52"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="80"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="79"/>
-      <c r="S39" s="85"/>
-      <c r="T39" s="92"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="81"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
+      <c r="R39" s="62"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="74"/>
+      <c r="U39" s="77"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="64"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
       <c r="D40" s="52"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="85"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="79"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
-      <c r="S40" s="85"/>
-      <c r="T40" s="92"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="81"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="68"/>
+      <c r="T40" s="74"/>
+      <c r="U40" s="77"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="64"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52"/>
       <c r="D41" s="52"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="80"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="80"/>
-      <c r="N41" s="77"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="79"/>
-      <c r="Q41" s="79"/>
-      <c r="R41" s="79"/>
-      <c r="S41" s="85"/>
-      <c r="T41" s="92"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="81"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="62"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="62"/>
+      <c r="R41" s="62"/>
+      <c r="S41" s="68"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="77"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="64"/>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
       <c r="D42" s="52"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="80"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="79"/>
-      <c r="J42" s="79"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="80"/>
-      <c r="N42" s="77"/>
-      <c r="O42" s="79"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="79"/>
-      <c r="R42" s="79"/>
-      <c r="S42" s="85"/>
-      <c r="T42" s="92"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="81"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="68"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="77"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="64"/>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
       <c r="D43" s="52"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="77"/>
-      <c r="O43" s="79"/>
-      <c r="P43" s="79"/>
-      <c r="Q43" s="79"/>
-      <c r="R43" s="79"/>
-      <c r="S43" s="85"/>
-      <c r="T43" s="92"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="81"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="68"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="77"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="64"/>
       <c r="B44" s="52"/>
       <c r="C44" s="52"/>
       <c r="D44" s="52"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="80"/>
-      <c r="N44" s="77"/>
-      <c r="O44" s="79"/>
-      <c r="P44" s="79"/>
-      <c r="Q44" s="79"/>
-      <c r="R44" s="79"/>
-      <c r="S44" s="85"/>
-      <c r="T44" s="92"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="81"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="68"/>
+      <c r="T44" s="74"/>
+      <c r="U44" s="77"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="64"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
       <c r="D45" s="52"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="77"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="80"/>
-      <c r="N45" s="77"/>
-      <c r="O45" s="79"/>
-      <c r="P45" s="79"/>
-      <c r="Q45" s="79"/>
-      <c r="R45" s="79"/>
-      <c r="S45" s="85"/>
-      <c r="T45" s="92"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="81"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="60"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="74"/>
+      <c r="U45" s="77"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="64"/>
       <c r="B46" s="52"/>
       <c r="C46" s="52"/>
       <c r="D46" s="52"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="77"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="77"/>
-      <c r="O46" s="79"/>
-      <c r="P46" s="79"/>
-      <c r="Q46" s="79"/>
-      <c r="R46" s="79"/>
-      <c r="S46" s="85"/>
-      <c r="T46" s="92"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="81"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="68"/>
+      <c r="T46" s="74"/>
+      <c r="U46" s="77"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="64"/>
       <c r="B47" s="52"/>
       <c r="C47" s="52"/>
       <c r="D47" s="52"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="79"/>
-      <c r="J47" s="79"/>
-      <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-      <c r="M47" s="80"/>
-      <c r="N47" s="77"/>
-      <c r="O47" s="79"/>
-      <c r="P47" s="79"/>
-      <c r="Q47" s="79"/>
-      <c r="R47" s="79"/>
-      <c r="S47" s="85"/>
-      <c r="T47" s="92"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="81"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="62"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="60"/>
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="68"/>
+      <c r="T47" s="74"/>
+      <c r="U47" s="77"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="64"/>
       <c r="B48" s="52"/>
       <c r="C48" s="52"/>
       <c r="D48" s="52"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="79"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="77"/>
-      <c r="O48" s="79"/>
-      <c r="P48" s="79"/>
-      <c r="Q48" s="79"/>
-      <c r="R48" s="79"/>
-      <c r="S48" s="85"/>
-      <c r="T48" s="92"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="81"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="60"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="68"/>
+      <c r="T48" s="74"/>
+      <c r="U48" s="77"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="64"/>
       <c r="B49" s="52"/>
       <c r="C49" s="52"/>
       <c r="D49" s="52"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="80"/>
-      <c r="N49" s="77"/>
-      <c r="O49" s="79"/>
-      <c r="P49" s="79"/>
-      <c r="Q49" s="79"/>
-      <c r="R49" s="79"/>
-      <c r="S49" s="85"/>
-      <c r="T49" s="92"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="81"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="62"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="60"/>
+      <c r="O49" s="62"/>
+      <c r="P49" s="62"/>
+      <c r="Q49" s="62"/>
+      <c r="R49" s="62"/>
+      <c r="S49" s="68"/>
+      <c r="T49" s="74"/>
+      <c r="U49" s="77"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="64"/>
       <c r="B50" s="52"/>
       <c r="C50" s="52"/>
       <c r="D50" s="52"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="79"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="79"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="80"/>
-      <c r="N50" s="77"/>
-      <c r="O50" s="79"/>
-      <c r="P50" s="79"/>
-      <c r="Q50" s="79"/>
-      <c r="R50" s="79"/>
-      <c r="S50" s="85"/>
-      <c r="T50" s="92"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="81"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="62"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="62"/>
+      <c r="P50" s="62"/>
+      <c r="Q50" s="62"/>
+      <c r="R50" s="62"/>
+      <c r="S50" s="68"/>
+      <c r="T50" s="74"/>
+      <c r="U50" s="77"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="64"/>
       <c r="B51" s="52"/>
       <c r="C51" s="52"/>
       <c r="D51" s="52"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="80"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="79"/>
-      <c r="K51" s="79"/>
-      <c r="L51" s="79"/>
-      <c r="M51" s="80"/>
-      <c r="N51" s="77"/>
-      <c r="O51" s="79"/>
-      <c r="P51" s="79"/>
-      <c r="Q51" s="79"/>
-      <c r="R51" s="79"/>
-      <c r="S51" s="85"/>
-      <c r="T51" s="92"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="81"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="62"/>
+      <c r="L51" s="62"/>
+      <c r="M51" s="63"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="62"/>
+      <c r="P51" s="62"/>
+      <c r="Q51" s="62"/>
+      <c r="R51" s="62"/>
+      <c r="S51" s="68"/>
+      <c r="T51" s="74"/>
+      <c r="U51" s="77"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="64"/>
       <c r="B52" s="52"/>
       <c r="C52" s="52"/>
       <c r="D52" s="52"/>
-      <c r="E52" s="79"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="80"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="79"/>
-      <c r="J52" s="79"/>
-      <c r="K52" s="79"/>
-      <c r="L52" s="79"/>
-      <c r="M52" s="80"/>
-      <c r="N52" s="77"/>
-      <c r="O52" s="79"/>
-      <c r="P52" s="79"/>
-      <c r="Q52" s="79"/>
-      <c r="R52" s="79"/>
-      <c r="S52" s="85"/>
-      <c r="T52" s="92"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="81"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="62"/>
+      <c r="M52" s="63"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="62"/>
+      <c r="P52" s="62"/>
+      <c r="Q52" s="62"/>
+      <c r="R52" s="62"/>
+      <c r="S52" s="68"/>
+      <c r="T52" s="74"/>
+      <c r="U52" s="77"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="64"/>
       <c r="B53" s="52"/>
       <c r="C53" s="52"/>
       <c r="D53" s="52"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="80"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
-      <c r="M53" s="80"/>
-      <c r="N53" s="77"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="79"/>
-      <c r="R53" s="79"/>
-      <c r="S53" s="85"/>
-      <c r="T53" s="92"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="81"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="63"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="62"/>
+      <c r="P53" s="62"/>
+      <c r="Q53" s="62"/>
+      <c r="R53" s="62"/>
+      <c r="S53" s="68"/>
+      <c r="T53" s="74"/>
+      <c r="U53" s="77"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="64"/>
       <c r="B54" s="52"/>
       <c r="C54" s="52"/>
       <c r="D54" s="52"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="80"/>
-      <c r="H54" s="77"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="80"/>
-      <c r="N54" s="77"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="79"/>
-      <c r="S54" s="85"/>
-      <c r="T54" s="92"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="81"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="60"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="62"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="60"/>
+      <c r="O54" s="62"/>
+      <c r="P54" s="62"/>
+      <c r="Q54" s="62"/>
+      <c r="R54" s="62"/>
+      <c r="S54" s="68"/>
+      <c r="T54" s="74"/>
+      <c r="U54" s="77"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="64"/>
       <c r="B55" s="52"/>
       <c r="C55" s="52"/>
       <c r="D55" s="52"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="85"/>
-      <c r="G55" s="80"/>
-      <c r="H55" s="77"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="80"/>
-      <c r="N55" s="77"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="79"/>
-      <c r="S55" s="85"/>
-      <c r="T55" s="92"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="81"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62"/>
+      <c r="L55" s="62"/>
+      <c r="M55" s="63"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="62"/>
+      <c r="P55" s="62"/>
+      <c r="Q55" s="62"/>
+      <c r="R55" s="62"/>
+      <c r="S55" s="68"/>
+      <c r="T55" s="74"/>
+      <c r="U55" s="77"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="64"/>
       <c r="B56" s="52"/>
       <c r="C56" s="52"/>
       <c r="D56" s="52"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="85"/>
-      <c r="G56" s="80"/>
-      <c r="H56" s="77"/>
-      <c r="I56" s="79"/>
-      <c r="J56" s="79"/>
-      <c r="K56" s="79"/>
-      <c r="L56" s="79"/>
-      <c r="M56" s="80"/>
-      <c r="N56" s="77"/>
-      <c r="O56" s="79"/>
-      <c r="P56" s="79"/>
-      <c r="Q56" s="79"/>
-      <c r="R56" s="79"/>
-      <c r="S56" s="85"/>
-      <c r="T56" s="92"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="81"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62"/>
+      <c r="L56" s="62"/>
+      <c r="M56" s="63"/>
+      <c r="N56" s="60"/>
+      <c r="O56" s="62"/>
+      <c r="P56" s="62"/>
+      <c r="Q56" s="62"/>
+      <c r="R56" s="62"/>
+      <c r="S56" s="68"/>
+      <c r="T56" s="74"/>
+      <c r="U56" s="77"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="64"/>
       <c r="B57" s="52"/>
       <c r="C57" s="52"/>
       <c r="D57" s="52"/>
-      <c r="E57" s="79"/>
-      <c r="F57" s="85"/>
-      <c r="G57" s="80"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="80"/>
-      <c r="N57" s="77"/>
-      <c r="O57" s="79"/>
-      <c r="P57" s="79"/>
-      <c r="Q57" s="79"/>
-      <c r="R57" s="79"/>
-      <c r="S57" s="85"/>
-      <c r="T57" s="92"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="81"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="62"/>
+      <c r="M57" s="63"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="62"/>
+      <c r="P57" s="62"/>
+      <c r="Q57" s="62"/>
+      <c r="R57" s="62"/>
+      <c r="S57" s="68"/>
+      <c r="T57" s="74"/>
+      <c r="U57" s="77"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="64"/>
       <c r="B58" s="52"/>
       <c r="C58" s="52"/>
       <c r="D58" s="52"/>
-      <c r="E58" s="79"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="80"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="79"/>
-      <c r="J58" s="79"/>
-      <c r="K58" s="79"/>
-      <c r="L58" s="79"/>
-      <c r="M58" s="80"/>
-      <c r="N58" s="77"/>
-      <c r="O58" s="79"/>
-      <c r="P58" s="79"/>
-      <c r="Q58" s="79"/>
-      <c r="R58" s="79"/>
-      <c r="S58" s="85"/>
-      <c r="T58" s="92"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="81"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="62"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="62"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="60"/>
+      <c r="O58" s="62"/>
+      <c r="P58" s="62"/>
+      <c r="Q58" s="62"/>
+      <c r="R58" s="62"/>
+      <c r="S58" s="68"/>
+      <c r="T58" s="74"/>
+      <c r="U58" s="77"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="64"/>
       <c r="B59" s="52"/>
       <c r="C59" s="52"/>
       <c r="D59" s="52"/>
-      <c r="E59" s="79"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="80"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="79"/>
-      <c r="J59" s="79"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="80"/>
-      <c r="N59" s="77"/>
-      <c r="O59" s="79"/>
-      <c r="P59" s="79"/>
-      <c r="Q59" s="79"/>
-      <c r="R59" s="79"/>
-      <c r="S59" s="85"/>
-      <c r="T59" s="92"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="81"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="62"/>
+      <c r="M59" s="63"/>
+      <c r="N59" s="60"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="62"/>
+      <c r="Q59" s="62"/>
+      <c r="R59" s="62"/>
+      <c r="S59" s="68"/>
+      <c r="T59" s="74"/>
+      <c r="U59" s="77"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="64"/>
       <c r="B60" s="52"/>
       <c r="C60" s="52"/>
       <c r="D60" s="52"/>
-      <c r="E60" s="79"/>
-      <c r="F60" s="85"/>
-      <c r="G60" s="80"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="79"/>
-      <c r="J60" s="79"/>
-      <c r="K60" s="79"/>
-      <c r="L60" s="79"/>
-      <c r="M60" s="80"/>
-      <c r="N60" s="77"/>
-      <c r="O60" s="79"/>
-      <c r="P60" s="79"/>
-      <c r="Q60" s="79"/>
-      <c r="R60" s="79"/>
-      <c r="S60" s="85"/>
-      <c r="T60" s="92"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="81"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="63"/>
+      <c r="N60" s="60"/>
+      <c r="O60" s="62"/>
+      <c r="P60" s="62"/>
+      <c r="Q60" s="62"/>
+      <c r="R60" s="62"/>
+      <c r="S60" s="68"/>
+      <c r="T60" s="74"/>
+      <c r="U60" s="77"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="64"/>
       <c r="B61" s="52"/>
       <c r="C61" s="52"/>
       <c r="D61" s="52"/>
-      <c r="E61" s="79"/>
-      <c r="F61" s="85"/>
-      <c r="G61" s="80"/>
-      <c r="H61" s="77"/>
-      <c r="I61" s="79"/>
-      <c r="J61" s="79"/>
-      <c r="K61" s="79"/>
-      <c r="L61" s="79"/>
-      <c r="M61" s="80"/>
-      <c r="N61" s="77"/>
-      <c r="O61" s="79"/>
-      <c r="P61" s="79"/>
-      <c r="Q61" s="79"/>
-      <c r="R61" s="79"/>
-      <c r="S61" s="85"/>
-      <c r="T61" s="92"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="81"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="68"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="62"/>
+      <c r="L61" s="62"/>
+      <c r="M61" s="63"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="62"/>
+      <c r="P61" s="62"/>
+      <c r="Q61" s="62"/>
+      <c r="R61" s="62"/>
+      <c r="S61" s="68"/>
+      <c r="T61" s="74"/>
+      <c r="U61" s="77"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="64"/>
       <c r="B62" s="52"/>
       <c r="C62" s="52"/>
       <c r="D62" s="52"/>
-      <c r="E62" s="79"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="80"/>
-      <c r="H62" s="77"/>
-      <c r="I62" s="79"/>
-      <c r="J62" s="79"/>
-      <c r="K62" s="79"/>
-      <c r="L62" s="79"/>
-      <c r="M62" s="80"/>
-      <c r="N62" s="77"/>
-      <c r="O62" s="79"/>
-      <c r="P62" s="79"/>
-      <c r="Q62" s="79"/>
-      <c r="R62" s="79"/>
-      <c r="S62" s="85"/>
-      <c r="T62" s="92"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="81"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="60"/>
+      <c r="I62" s="62"/>
+      <c r="J62" s="62"/>
+      <c r="K62" s="62"/>
+      <c r="L62" s="62"/>
+      <c r="M62" s="63"/>
+      <c r="N62" s="60"/>
+      <c r="O62" s="62"/>
+      <c r="P62" s="62"/>
+      <c r="Q62" s="62"/>
+      <c r="R62" s="62"/>
+      <c r="S62" s="68"/>
+      <c r="T62" s="74"/>
+      <c r="U62" s="77"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="64"/>
       <c r="B63" s="52"/>
       <c r="C63" s="52"/>
       <c r="D63" s="52"/>
-      <c r="E63" s="79"/>
-      <c r="F63" s="85"/>
-      <c r="G63" s="80"/>
-      <c r="H63" s="77"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="79"/>
-      <c r="K63" s="79"/>
-      <c r="L63" s="79"/>
-      <c r="M63" s="80"/>
-      <c r="N63" s="77"/>
-      <c r="O63" s="79"/>
-      <c r="P63" s="79"/>
-      <c r="Q63" s="79"/>
-      <c r="R63" s="79"/>
-      <c r="S63" s="85"/>
-      <c r="T63" s="92"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="81"/>
+      <c r="E63" s="62"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="62"/>
+      <c r="K63" s="62"/>
+      <c r="L63" s="62"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="60"/>
+      <c r="O63" s="62"/>
+      <c r="P63" s="62"/>
+      <c r="Q63" s="62"/>
+      <c r="R63" s="62"/>
+      <c r="S63" s="68"/>
+      <c r="T63" s="74"/>
+      <c r="U63" s="77"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="64"/>
       <c r="B64" s="52"/>
       <c r="C64" s="52"/>
       <c r="D64" s="52"/>
-      <c r="E64" s="79"/>
-      <c r="F64" s="85"/>
-      <c r="G64" s="80"/>
-      <c r="H64" s="77"/>
-      <c r="I64" s="79"/>
-      <c r="J64" s="79"/>
-      <c r="K64" s="79"/>
-      <c r="L64" s="79"/>
-      <c r="M64" s="80"/>
-      <c r="N64" s="77"/>
-      <c r="O64" s="79"/>
-      <c r="P64" s="79"/>
-      <c r="Q64" s="79"/>
-      <c r="R64" s="79"/>
-      <c r="S64" s="85"/>
-      <c r="T64" s="92"/>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="81"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="62"/>
+      <c r="L64" s="62"/>
+      <c r="M64" s="63"/>
+      <c r="N64" s="60"/>
+      <c r="O64" s="62"/>
+      <c r="P64" s="62"/>
+      <c r="Q64" s="62"/>
+      <c r="R64" s="62"/>
+      <c r="S64" s="68"/>
+      <c r="T64" s="74"/>
+      <c r="U64" s="77"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="64"/>
       <c r="B65" s="52"/>
       <c r="C65" s="52"/>
       <c r="D65" s="52"/>
-      <c r="E65" s="79"/>
-      <c r="F65" s="85"/>
-      <c r="G65" s="80"/>
-      <c r="H65" s="77"/>
-      <c r="I65" s="79"/>
-      <c r="J65" s="79"/>
-      <c r="K65" s="79"/>
-      <c r="L65" s="79"/>
-      <c r="M65" s="80"/>
-      <c r="N65" s="77"/>
-      <c r="O65" s="79"/>
-      <c r="P65" s="79"/>
-      <c r="Q65" s="79"/>
-      <c r="R65" s="79"/>
-      <c r="S65" s="85"/>
-      <c r="T65" s="92"/>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="81"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="62"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="63"/>
+      <c r="N65" s="60"/>
+      <c r="O65" s="62"/>
+      <c r="P65" s="62"/>
+      <c r="Q65" s="62"/>
+      <c r="R65" s="62"/>
+      <c r="S65" s="68"/>
+      <c r="T65" s="74"/>
+      <c r="U65" s="77"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="64"/>
       <c r="B66" s="52"/>
       <c r="C66" s="52"/>
       <c r="D66" s="52"/>
-      <c r="E66" s="79"/>
-      <c r="F66" s="85"/>
-      <c r="G66" s="80"/>
-      <c r="H66" s="77"/>
-      <c r="I66" s="79"/>
-      <c r="J66" s="79"/>
-      <c r="K66" s="79"/>
-      <c r="L66" s="79"/>
-      <c r="M66" s="80"/>
-      <c r="N66" s="77"/>
-      <c r="O66" s="79"/>
-      <c r="P66" s="79"/>
-      <c r="Q66" s="79"/>
-      <c r="R66" s="79"/>
-      <c r="S66" s="85"/>
-      <c r="T66" s="92"/>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="81"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="62"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="62"/>
+      <c r="L66" s="62"/>
+      <c r="M66" s="63"/>
+      <c r="N66" s="60"/>
+      <c r="O66" s="62"/>
+      <c r="P66" s="62"/>
+      <c r="Q66" s="62"/>
+      <c r="R66" s="62"/>
+      <c r="S66" s="68"/>
+      <c r="T66" s="74"/>
+      <c r="U66" s="77"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="64"/>
       <c r="B67" s="52"/>
       <c r="C67" s="52"/>
       <c r="D67" s="52"/>
-      <c r="E67" s="79"/>
-      <c r="F67" s="85"/>
-      <c r="G67" s="80"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="79"/>
-      <c r="J67" s="79"/>
-      <c r="K67" s="79"/>
-      <c r="L67" s="79"/>
-      <c r="M67" s="80"/>
-      <c r="N67" s="77"/>
-      <c r="O67" s="79"/>
-      <c r="P67" s="79"/>
-      <c r="Q67" s="79"/>
-      <c r="R67" s="79"/>
-      <c r="S67" s="85"/>
-      <c r="T67" s="92"/>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="81"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="60"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="62"/>
+      <c r="L67" s="62"/>
+      <c r="M67" s="63"/>
+      <c r="N67" s="60"/>
+      <c r="O67" s="62"/>
+      <c r="P67" s="62"/>
+      <c r="Q67" s="62"/>
+      <c r="R67" s="62"/>
+      <c r="S67" s="68"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="77"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="64"/>
       <c r="B68" s="52"/>
       <c r="C68" s="52"/>
       <c r="D68" s="52"/>
-      <c r="E68" s="79"/>
-      <c r="F68" s="85"/>
-      <c r="G68" s="80"/>
-      <c r="H68" s="77"/>
-      <c r="I68" s="79"/>
-      <c r="J68" s="79"/>
-      <c r="K68" s="79"/>
-      <c r="L68" s="79"/>
-      <c r="M68" s="80"/>
-      <c r="N68" s="77"/>
-      <c r="O68" s="79"/>
-      <c r="P68" s="79"/>
-      <c r="Q68" s="79"/>
-      <c r="R68" s="79"/>
-      <c r="S68" s="85"/>
-      <c r="T68" s="92"/>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="81"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="60"/>
+      <c r="I68" s="62"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="62"/>
+      <c r="L68" s="62"/>
+      <c r="M68" s="63"/>
+      <c r="N68" s="60"/>
+      <c r="O68" s="62"/>
+      <c r="P68" s="62"/>
+      <c r="Q68" s="62"/>
+      <c r="R68" s="62"/>
+      <c r="S68" s="68"/>
+      <c r="T68" s="74"/>
+      <c r="U68" s="77"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="64"/>
       <c r="B69" s="52"/>
       <c r="C69" s="52"/>
       <c r="D69" s="52"/>
-      <c r="E69" s="79"/>
-      <c r="F69" s="85"/>
-      <c r="G69" s="80"/>
-      <c r="H69" s="77"/>
-      <c r="I69" s="79"/>
-      <c r="J69" s="79"/>
-      <c r="K69" s="79"/>
-      <c r="L69" s="79"/>
-      <c r="M69" s="80"/>
-      <c r="N69" s="77"/>
-      <c r="O69" s="79"/>
-      <c r="P69" s="79"/>
-      <c r="Q69" s="79"/>
-      <c r="R69" s="79"/>
-      <c r="S69" s="85"/>
-      <c r="T69" s="92"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="81"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="60"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="62"/>
+      <c r="L69" s="62"/>
+      <c r="M69" s="63"/>
+      <c r="N69" s="60"/>
+      <c r="O69" s="62"/>
+      <c r="P69" s="62"/>
+      <c r="Q69" s="62"/>
+      <c r="R69" s="62"/>
+      <c r="S69" s="68"/>
+      <c r="T69" s="74"/>
+      <c r="U69" s="77"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="64"/>
       <c r="B70" s="52"/>
       <c r="C70" s="52"/>
       <c r="D70" s="52"/>
-      <c r="E70" s="79"/>
-      <c r="F70" s="85"/>
-      <c r="G70" s="80"/>
-      <c r="H70" s="77"/>
-      <c r="I70" s="79"/>
-      <c r="J70" s="79"/>
-      <c r="K70" s="79"/>
-      <c r="L70" s="79"/>
-      <c r="M70" s="80"/>
-      <c r="N70" s="77"/>
-      <c r="O70" s="79"/>
-      <c r="P70" s="79"/>
-      <c r="Q70" s="79"/>
-      <c r="R70" s="79"/>
-      <c r="S70" s="85"/>
-      <c r="T70" s="92"/>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="81"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="63"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="62"/>
+      <c r="J70" s="62"/>
+      <c r="K70" s="62"/>
+      <c r="L70" s="62"/>
+      <c r="M70" s="63"/>
+      <c r="N70" s="60"/>
+      <c r="O70" s="62"/>
+      <c r="P70" s="62"/>
+      <c r="Q70" s="62"/>
+      <c r="R70" s="62"/>
+      <c r="S70" s="68"/>
+      <c r="T70" s="74"/>
+      <c r="U70" s="77"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="64"/>
       <c r="B71" s="52"/>
       <c r="C71" s="52"/>
       <c r="D71" s="52"/>
-      <c r="E71" s="79"/>
-      <c r="F71" s="85"/>
-      <c r="G71" s="80"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="79"/>
-      <c r="J71" s="79"/>
-      <c r="K71" s="79"/>
-      <c r="L71" s="79"/>
-      <c r="M71" s="80"/>
-      <c r="N71" s="77"/>
-      <c r="O71" s="79"/>
-      <c r="P71" s="79"/>
-      <c r="Q71" s="79"/>
-      <c r="R71" s="79"/>
-      <c r="S71" s="85"/>
-      <c r="T71" s="92"/>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="81"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="62"/>
+      <c r="L71" s="62"/>
+      <c r="M71" s="63"/>
+      <c r="N71" s="60"/>
+      <c r="O71" s="62"/>
+      <c r="P71" s="62"/>
+      <c r="Q71" s="62"/>
+      <c r="R71" s="62"/>
+      <c r="S71" s="68"/>
+      <c r="T71" s="74"/>
+      <c r="U71" s="77"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="64"/>
       <c r="B72" s="52"/>
       <c r="C72" s="52"/>
       <c r="D72" s="52"/>
-      <c r="E72" s="79"/>
-      <c r="F72" s="85"/>
-      <c r="G72" s="80"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="79"/>
-      <c r="J72" s="79"/>
-      <c r="K72" s="79"/>
-      <c r="L72" s="79"/>
-      <c r="M72" s="80"/>
-      <c r="N72" s="77"/>
-      <c r="O72" s="79"/>
-      <c r="P72" s="79"/>
-      <c r="Q72" s="79"/>
-      <c r="R72" s="79"/>
-      <c r="S72" s="85"/>
-      <c r="T72" s="92"/>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="81"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="62"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="62"/>
+      <c r="L72" s="62"/>
+      <c r="M72" s="63"/>
+      <c r="N72" s="60"/>
+      <c r="O72" s="62"/>
+      <c r="P72" s="62"/>
+      <c r="Q72" s="62"/>
+      <c r="R72" s="62"/>
+      <c r="S72" s="68"/>
+      <c r="T72" s="74"/>
+      <c r="U72" s="77"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="64"/>
       <c r="B73" s="52"/>
       <c r="C73" s="52"/>
       <c r="D73" s="52"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="85"/>
-      <c r="G73" s="80"/>
-      <c r="H73" s="77"/>
-      <c r="I73" s="79"/>
-      <c r="J73" s="79"/>
-      <c r="K73" s="79"/>
-      <c r="L73" s="79"/>
-      <c r="M73" s="80"/>
-      <c r="N73" s="77"/>
-      <c r="O73" s="79"/>
-      <c r="P73" s="79"/>
-      <c r="Q73" s="79"/>
-      <c r="R73" s="79"/>
-      <c r="S73" s="85"/>
-      <c r="T73" s="92"/>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="81"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="63"/>
+      <c r="H73" s="60"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="62"/>
+      <c r="L73" s="62"/>
+      <c r="M73" s="63"/>
+      <c r="N73" s="60"/>
+      <c r="O73" s="62"/>
+      <c r="P73" s="62"/>
+      <c r="Q73" s="62"/>
+      <c r="R73" s="62"/>
+      <c r="S73" s="68"/>
+      <c r="T73" s="74"/>
+      <c r="U73" s="77"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="64"/>
       <c r="B74" s="52"/>
       <c r="C74" s="52"/>
       <c r="D74" s="52"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="85"/>
-      <c r="G74" s="80"/>
-      <c r="H74" s="77"/>
-      <c r="I74" s="79"/>
-      <c r="J74" s="79"/>
-      <c r="K74" s="79"/>
-      <c r="L74" s="79"/>
-      <c r="M74" s="80"/>
-      <c r="N74" s="77"/>
-      <c r="O74" s="79"/>
-      <c r="P74" s="79"/>
-      <c r="Q74" s="79"/>
-      <c r="R74" s="79"/>
-      <c r="S74" s="85"/>
-      <c r="T74" s="92"/>
-    </row>
-    <row r="75" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="82"/>
-      <c r="B75" s="83"/>
-      <c r="C75" s="83"/>
-      <c r="D75" s="83"/>
-      <c r="E75" s="79"/>
-      <c r="F75" s="85"/>
-      <c r="G75" s="80"/>
-      <c r="H75" s="77"/>
-      <c r="I75" s="79"/>
-      <c r="J75" s="79"/>
-      <c r="K75" s="79"/>
-      <c r="L75" s="79"/>
-      <c r="M75" s="80"/>
-      <c r="N75" s="77"/>
-      <c r="O75" s="79"/>
-      <c r="P75" s="79"/>
-      <c r="Q75" s="79"/>
-      <c r="R75" s="79"/>
-      <c r="S75" s="85"/>
-      <c r="T75" s="93"/>
+      <c r="E74" s="62"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="63"/>
+      <c r="H74" s="60"/>
+      <c r="I74" s="62"/>
+      <c r="J74" s="62"/>
+      <c r="K74" s="62"/>
+      <c r="L74" s="62"/>
+      <c r="M74" s="63"/>
+      <c r="N74" s="60"/>
+      <c r="O74" s="62"/>
+      <c r="P74" s="62"/>
+      <c r="Q74" s="62"/>
+      <c r="R74" s="62"/>
+      <c r="S74" s="68"/>
+      <c r="T74" s="74"/>
+      <c r="U74" s="77"/>
+    </row>
+    <row r="75" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="65"/>
+      <c r="B75" s="66"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="62"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="63"/>
+      <c r="H75" s="60"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="62"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="62"/>
+      <c r="M75" s="63"/>
+      <c r="N75" s="60"/>
+      <c r="O75" s="62"/>
+      <c r="P75" s="62"/>
+      <c r="Q75" s="62"/>
+      <c r="R75" s="62"/>
+      <c r="S75" s="68"/>
+      <c r="T75" s="75"/>
+      <c r="U75" s="78"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T16" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
-  <mergeCells count="4">
+  <autoFilter ref="A2:T20" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
+  <mergeCells count="5">
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <conditionalFormatting sqref="T3:T75">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="NOK">
@@ -7360,7 +7814,7 @@
       <formula>LEFT(T3,LEN("OK"))="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G75" xr:uid="{4832D533-7A08-40E1-9AA1-2EB7D4098823}">
       <formula1>"Solo tazze, Solo bordi, Bordi e tazze,"</formula1>
     </dataValidation>
@@ -7376,13 +7830,234 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F75" xr:uid="{5865F76D-6592-4088-891A-E3BB5A14F46D}">
       <formula1>"Aperto, Chiuso,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E75" xr:uid="{D3B60138-7714-448B-8CA2-3F4C37A74F08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E18" xr:uid="{D3B60138-7714-448B-8CA2-3F4C37A74F08}">
       <formula1>"40,50,60,80,100,120,140,160,200,240,280,300,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T75" xr:uid="{ACF13385-C338-4011-A851-2E1C2C226567}">
       <formula1>"OK,NOK,"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19 E21:E75" xr:uid="{F585DE42-5F16-4935-91FB-DA6277F96BA9}">
+      <formula1>"40,50,60,80,100,120,140,160,200,240,280,300,400,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20" xr:uid="{D9599817-B3A8-41B0-8B39-BC65074E54F4}">
+      <formula1>"40,50,60,80,100,120,140,160,180,200,240,280,300,400,"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1B73F-CED5-48D1-ADA9-1E1DEE931281}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="85">
+        <v>5898</v>
+      </c>
+      <c r="C2" s="85">
+        <v>2240</v>
+      </c>
+      <c r="D2" s="85">
+        <v>2340</v>
+      </c>
+      <c r="E2" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="50"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="52">
+        <v>11800</v>
+      </c>
+      <c r="C3" s="52">
+        <v>2240</v>
+      </c>
+      <c r="D3" s="85">
+        <v>2340</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="52"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="52">
+        <v>11800</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2580</v>
+      </c>
+      <c r="D4" s="85">
+        <v>2340</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="52"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="52">
+        <v>13600</v>
+      </c>
+      <c r="C7" s="52">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="52">
+        <v>2450</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D51992-89CF-4CBB-8C6E-CFE0CD0D8D71}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Consente di scegliere la tipologia di imballo
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570791AD-22B5-4F7F-914C-BD734B4115A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCE638-0F02-457F-86FB-9D8614A949AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="143">
   <si>
     <t>Diagonali</t>
   </si>
@@ -523,6 +523,18 @@
   </si>
   <si>
     <t>Ci sta in quella pedana ma non si riesce a mettere perchè il nastro troppo lungo</t>
+  </si>
+  <si>
+    <t>Camion fuori STD</t>
+  </si>
+  <si>
+    <t>15000 (primo step)</t>
+  </si>
+  <si>
+    <t>2990 (2 step)</t>
+  </si>
+  <si>
+    <t>3° step è aumentare di nuovo la larghezza</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1190,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1398,6 +1410,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2935,10 +2950,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="93"/>
+      <c r="B1" s="94"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3472,21 +3487,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="94" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="95"/>
-      <c r="I1" s="97" t="s">
+      <c r="H1" s="96"/>
+      <c r="I1" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="98" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3515,8 +3530,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -3980,14 +3995,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4415,14 +4430,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4568,7 +4583,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="101" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -4591,7 +4606,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -4612,7 +4627,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="102"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -4624,7 +4639,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="101"/>
+      <c r="F19" s="102"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -4636,7 +4651,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="101"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -4648,7 +4663,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="101"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -4660,7 +4675,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="101"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -4672,7 +4687,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="102"/>
+      <c r="F23" s="103"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -4868,14 +4883,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5191,8 +5206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5220,35 +5235,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="103" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="103" t="s">
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="109" t="s">
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="110" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="109" t="s">
+      <c r="U1" s="110" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5310,8 +5325,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="110"/>
-      <c r="U2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="112"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -6710,27 +6725,55 @@
       <c r="U24" s="77"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="63"/>
+      <c r="A25" s="64">
+        <v>20210520</v>
+      </c>
+      <c r="B25" s="69">
+        <v>44621</v>
+      </c>
+      <c r="C25" s="52">
+        <v>61300</v>
+      </c>
+      <c r="D25" s="52">
+        <v>800</v>
+      </c>
+      <c r="E25" s="62">
+        <v>120</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>100</v>
+      </c>
       <c r="H25" s="60"/>
       <c r="I25" s="62"/>
       <c r="J25" s="62"/>
       <c r="K25" s="62"/>
       <c r="L25" s="62"/>
       <c r="M25" s="63"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="68"/>
+      <c r="N25" s="60">
+        <v>6500</v>
+      </c>
+      <c r="O25" s="62">
+        <v>950</v>
+      </c>
+      <c r="P25" s="62">
+        <v>1800</v>
+      </c>
+      <c r="Q25" s="62">
+        <v>7</v>
+      </c>
+      <c r="R25" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S25" s="68">
+        <v>1</v>
+      </c>
       <c r="T25" s="74"/>
-      <c r="U25" s="77"/>
+      <c r="U25" s="77" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="64"/>
@@ -7934,19 +7977,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1B73F-CED5-48D1-ADA9-1E1DEE931281}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8027,21 +8071,39 @@
       <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="B5" s="52">
+        <v>11800</v>
+      </c>
+      <c r="C5" s="52">
+        <v>2700</v>
+      </c>
+      <c r="D5" s="52">
+        <v>2150</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>115</v>
+      </c>
       <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
+      <c r="B6" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="92">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -8051,7 +8113,7 @@
         <v>13600</v>
       </c>
       <c r="C7" s="52">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="D7" s="52">
         <v>2450</v>
@@ -8060,6 +8122,24 @@
         <v>117</v>
       </c>
       <c r="F7" s="52"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="52">
+        <v>13600</v>
+      </c>
+      <c r="C8" s="52">
+        <v>3000</v>
+      </c>
+      <c r="D8" s="52">
+        <v>2450</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prende i nastri dal database
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCE638-0F02-457F-86FB-9D8614A949AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4EE4A-218E-4BF2-9E11-0AEEF3E90137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -5206,8 +5206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5470,7 +5470,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="64">
         <v>20210152</v>
       </c>
@@ -5555,14 +5555,14 @@
       <c r="G6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="71">
-        <v>8400</v>
+      <c r="H6" s="86">
+        <v>9500</v>
       </c>
       <c r="I6" s="62">
         <v>2230</v>
       </c>
       <c r="J6" s="62">
-        <v>2530</v>
+        <v>2240</v>
       </c>
       <c r="K6" s="62">
         <v>7</v>
@@ -5592,7 +5592,7 @@
         <v>2</v>
       </c>
       <c r="T6" s="74" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="U6" s="77" t="s">
         <v>137</v>
@@ -8152,7 +8152,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sistema il salvataggio degli imballi in ferro a dB
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4EE4A-218E-4BF2-9E11-0AEEF3E90137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F128356-1B31-46C3-96BE-5B1650D37765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
   <si>
     <t>Diagonali</t>
   </si>
@@ -535,6 +535,9 @@
   </si>
   <si>
     <t>3° step è aumentare di nuovo la larghezza</t>
+  </si>
+  <si>
+    <t>Non c'è bisongo del panino?</t>
   </si>
 </sst>
 </file>
@@ -1356,9 +1359,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1473,6 +1473,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2950,10 +2953,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="93"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3487,21 +3490,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="95" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="96"/>
-      <c r="I1" s="98" t="s">
+      <c r="H1" s="95"/>
+      <c r="I1" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="97" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3530,8 +3533,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -3995,14 +3998,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4430,14 +4433,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4583,7 +4586,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="101" t="s">
+      <c r="F16" s="100" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -4606,7 +4609,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="102"/>
+      <c r="F17" s="101"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -4627,7 +4630,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="102"/>
+      <c r="F18" s="101"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -4639,7 +4642,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="102"/>
+      <c r="F19" s="101"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -4651,7 +4654,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="102"/>
+      <c r="F20" s="101"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -4663,7 +4666,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="102"/>
+      <c r="F21" s="101"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -4675,7 +4678,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="102"/>
+      <c r="F22" s="101"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -4687,7 +4690,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="103"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -4883,14 +4886,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5207,7 +5210,7 @@
   <dimension ref="A1:AG75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5235,35 +5238,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="104" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="104" t="s">
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="110" t="s">
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="109" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="110" t="s">
+      <c r="U1" s="109" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5325,8 +5328,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="111"/>
-      <c r="U2" s="112"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="111"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -5398,10 +5401,10 @@
       <c r="S3" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T3" s="73" t="s">
+      <c r="T3" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="76" t="s">
+      <c r="U3" s="75" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5427,31 +5430,31 @@
       <c r="G4" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="86">
+      <c r="H4" s="85">
         <v>2400</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="86">
         <v>2400</v>
       </c>
-      <c r="J4" s="87">
+      <c r="J4" s="86">
         <v>1400</v>
       </c>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="87" t="s">
+      <c r="L4" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="M4" s="88" t="s">
+      <c r="M4" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="86">
+      <c r="N4" s="85">
         <v>3700</v>
       </c>
-      <c r="O4" s="87">
+      <c r="O4" s="86">
         <v>1350</v>
       </c>
-      <c r="P4" s="87">
+      <c r="P4" s="86">
         <v>2200</v>
       </c>
       <c r="Q4" s="62" t="s">
@@ -5463,10 +5466,10 @@
       <c r="S4" s="68">
         <v>1</v>
       </c>
-      <c r="T4" s="74" t="s">
+      <c r="T4" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="77" t="s">
+      <c r="U4" s="76" t="s">
         <v>138</v>
       </c>
     </row>
@@ -5492,28 +5495,28 @@
       <c r="G5" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="85">
         <v>7000</v>
       </c>
-      <c r="I5" s="87">
+      <c r="I5" s="86">
         <v>790</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="86">
         <v>2240</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="86">
         <v>7</v>
       </c>
-      <c r="L5" s="87" t="s">
+      <c r="L5" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="88">
+      <c r="M5" s="87">
         <v>1</v>
       </c>
-      <c r="N5" s="86">
+      <c r="N5" s="85">
         <v>5000</v>
       </c>
-      <c r="O5" s="87">
+      <c r="O5" s="86">
         <v>1600</v>
       </c>
       <c r="P5" s="62">
@@ -5525,13 +5528,13 @@
       <c r="R5" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="S5" s="72">
+      <c r="S5" s="71">
         <v>2</v>
       </c>
-      <c r="T5" s="74" t="s">
+      <c r="T5" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="77"/>
+      <c r="U5" s="76"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="64">
@@ -5555,7 +5558,7 @@
       <c r="G6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="86">
+      <c r="H6" s="85">
         <v>9500</v>
       </c>
       <c r="I6" s="62">
@@ -5573,7 +5576,7 @@
       <c r="M6" s="63">
         <v>2</v>
       </c>
-      <c r="N6" s="71">
+      <c r="N6" s="85">
         <v>9500</v>
       </c>
       <c r="O6" s="62">
@@ -5591,10 +5594,10 @@
       <c r="S6" s="68">
         <v>2</v>
       </c>
-      <c r="T6" s="74" t="s">
+      <c r="T6" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="77" t="s">
+      <c r="U6" s="76" t="s">
         <v>137</v>
       </c>
     </row>
@@ -5620,10 +5623,10 @@
       <c r="G7" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="85">
         <v>2000</v>
       </c>
-      <c r="I7" s="87">
+      <c r="I7" s="86">
         <v>2000</v>
       </c>
       <c r="J7" s="62">
@@ -5656,10 +5659,10 @@
       <c r="S7" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T7" s="74" t="s">
+      <c r="T7" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="77"/>
+      <c r="U7" s="76"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="64">
@@ -5719,10 +5722,10 @@
       <c r="S8" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T8" s="74" t="s">
+      <c r="T8" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U8" s="77"/>
+      <c r="U8" s="76"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="64">
@@ -5782,10 +5785,10 @@
       <c r="S9" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T9" s="74" t="s">
+      <c r="T9" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U9" s="77"/>
+      <c r="U9" s="76"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="64">
@@ -5845,10 +5848,10 @@
       <c r="S10" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T10" s="74" t="s">
+      <c r="T10" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U10" s="77"/>
+      <c r="U10" s="76"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="64">
@@ -5908,10 +5911,10 @@
       <c r="S11" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T11" s="74" t="s">
+      <c r="T11" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U11" s="77"/>
+      <c r="U11" s="76"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="64">
@@ -5971,10 +5974,10 @@
       <c r="S12" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T12" s="74" t="s">
+      <c r="T12" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U12" s="77"/>
+      <c r="U12" s="76"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="64">
@@ -6034,10 +6037,10 @@
       <c r="S13" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T13" s="74" t="s">
+      <c r="T13" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U13" s="77"/>
+      <c r="U13" s="76"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="64">
@@ -6097,10 +6100,10 @@
       <c r="S14" s="68">
         <v>2</v>
       </c>
-      <c r="T14" s="74" t="s">
+      <c r="T14" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U14" s="77"/>
+      <c r="U14" s="76"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="64">
@@ -6160,10 +6163,10 @@
       <c r="S15" s="68">
         <v>1</v>
       </c>
-      <c r="T15" s="74" t="s">
+      <c r="T15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U15" s="77"/>
+      <c r="U15" s="76"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="64">
@@ -6205,34 +6208,34 @@
       <c r="M16" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="86">
+      <c r="N16" s="85">
         <v>3000</v>
       </c>
-      <c r="O16" s="87">
+      <c r="O16" s="86">
         <v>1000</v>
       </c>
-      <c r="P16" s="87">
+      <c r="P16" s="86">
         <v>2240</v>
       </c>
-      <c r="Q16" s="87" t="s">
+      <c r="Q16" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="R16" s="87" t="s">
+      <c r="R16" s="86" t="s">
         <v>106</v>
       </c>
       <c r="S16" s="68">
         <v>1</v>
       </c>
-      <c r="T16" s="74" t="s">
+      <c r="T16" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U16" s="77"/>
+      <c r="U16" s="76"/>
     </row>
     <row r="17" spans="1:21" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>20210468</v>
       </c>
-      <c r="B17" s="79">
+      <c r="B17" s="78">
         <v>44592</v>
       </c>
       <c r="C17" s="17">
@@ -6241,52 +6244,52 @@
       <c r="D17" s="17">
         <v>650</v>
       </c>
-      <c r="E17" s="80">
+      <c r="E17" s="79">
         <v>200</v>
       </c>
-      <c r="F17" s="81" t="s">
+      <c r="F17" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="82" t="s">
+      <c r="G17" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="H17" s="89">
+      <c r="H17" s="88">
         <v>6700</v>
       </c>
-      <c r="I17" s="90">
+      <c r="I17" s="89">
         <v>790</v>
       </c>
-      <c r="J17" s="90">
+      <c r="J17" s="89">
         <v>2240</v>
       </c>
-      <c r="K17" s="90">
+      <c r="K17" s="89">
         <v>7</v>
       </c>
-      <c r="L17" s="90" t="s">
+      <c r="L17" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="M17" s="91">
+      <c r="M17" s="90">
         <v>1</v>
       </c>
-      <c r="N17" s="89">
+      <c r="N17" s="88">
         <v>6000</v>
       </c>
-      <c r="O17" s="90">
+      <c r="O17" s="89">
         <v>800</v>
       </c>
-      <c r="P17" s="90">
+      <c r="P17" s="89">
         <v>2450</v>
       </c>
-      <c r="Q17" s="80">
+      <c r="Q17" s="79">
         <v>7</v>
       </c>
-      <c r="R17" s="80" t="s">
+      <c r="R17" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="S17" s="81">
+      <c r="S17" s="80">
         <v>1</v>
       </c>
-      <c r="T17" s="83" t="s">
+      <c r="T17" s="82" t="s">
         <v>23</v>
       </c>
       <c r="U17" s="34" t="s">
@@ -6351,10 +6354,10 @@
       <c r="S18" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T18" s="74" t="s">
+      <c r="T18" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U18" s="77"/>
+      <c r="U18" s="76"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="64">
@@ -6400,10 +6403,10 @@
       <c r="S19" s="68">
         <v>1</v>
       </c>
-      <c r="T19" s="74" t="s">
+      <c r="T19" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="U19" s="77" t="s">
+      <c r="U19" s="76" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6465,10 +6468,10 @@
       <c r="S20" s="68">
         <v>1</v>
       </c>
-      <c r="T20" s="74" t="s">
+      <c r="T20" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="U20" s="77" t="s">
+      <c r="U20" s="76" t="s">
         <v>136</v>
       </c>
     </row>
@@ -6530,10 +6533,10 @@
       <c r="S21" s="68">
         <v>1</v>
       </c>
-      <c r="T21" s="74" t="s">
+      <c r="T21" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U21" s="77"/>
+      <c r="U21" s="76"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="64">
@@ -6593,10 +6596,10 @@
       <c r="S22" s="68">
         <v>2</v>
       </c>
-      <c r="T22" s="74" t="s">
+      <c r="T22" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U22" s="77"/>
+      <c r="U22" s="76"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="64">
@@ -6656,10 +6659,10 @@
       <c r="S23" s="68">
         <v>1</v>
       </c>
-      <c r="T23" s="74" t="s">
+      <c r="T23" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U23" s="77"/>
+      <c r="U23" s="76"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="64">
@@ -6719,10 +6722,10 @@
       <c r="S24" s="68">
         <v>1</v>
       </c>
-      <c r="T24" s="74" t="s">
+      <c r="T24" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="U24" s="77"/>
+      <c r="U24" s="76"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="64">
@@ -6746,12 +6749,24 @@
       <c r="G25" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="63"/>
+      <c r="H25" s="60">
+        <v>6300</v>
+      </c>
+      <c r="I25" s="62">
+        <v>940</v>
+      </c>
+      <c r="J25" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K25" s="62">
+        <v>1</v>
+      </c>
+      <c r="L25" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M25" s="63">
+        <v>1</v>
+      </c>
       <c r="N25" s="60">
         <v>6500</v>
       </c>
@@ -6770,79 +6785,201 @@
       <c r="S25" s="68">
         <v>1</v>
       </c>
-      <c r="T25" s="74"/>
-      <c r="U25" s="77" t="s">
-        <v>135</v>
-      </c>
+      <c r="T25" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="U25" s="76"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="62"/>
-      <c r="Q26" s="62"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="68"/>
-      <c r="T26" s="74"/>
-      <c r="U26" s="77"/>
+      <c r="A26" s="64">
+        <v>20210210</v>
+      </c>
+      <c r="B26" s="69">
+        <v>44666</v>
+      </c>
+      <c r="C26" s="52">
+        <v>85000</v>
+      </c>
+      <c r="D26" s="52">
+        <v>1600</v>
+      </c>
+      <c r="E26" s="62">
+        <v>300</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" s="60">
+        <v>11800</v>
+      </c>
+      <c r="I26" s="62">
+        <v>1740</v>
+      </c>
+      <c r="J26" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K26" s="62">
+        <v>7</v>
+      </c>
+      <c r="L26" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M26" s="112">
+        <v>1</v>
+      </c>
+      <c r="N26" s="60">
+        <v>11800</v>
+      </c>
+      <c r="O26" s="62">
+        <v>2200</v>
+      </c>
+      <c r="P26" s="62">
+        <v>2030</v>
+      </c>
+      <c r="Q26" s="62">
+        <v>1</v>
+      </c>
+      <c r="R26" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S26" s="68">
+        <v>2</v>
+      </c>
+      <c r="T26" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="U26" s="76" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="68"/>
-      <c r="T27" s="74"/>
-      <c r="U27" s="77"/>
+      <c r="A27" s="64">
+        <v>2022004</v>
+      </c>
+      <c r="B27" s="69">
+        <v>44666</v>
+      </c>
+      <c r="C27" s="52">
+        <v>46000</v>
+      </c>
+      <c r="D27" s="52">
+        <v>914</v>
+      </c>
+      <c r="E27" s="62">
+        <v>120</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="60">
+        <v>5800</v>
+      </c>
+      <c r="I27" s="62">
+        <v>1054</v>
+      </c>
+      <c r="J27" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K27" s="62">
+        <v>1</v>
+      </c>
+      <c r="L27" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M27" s="63">
+        <v>1</v>
+      </c>
+      <c r="N27" s="60">
+        <v>5000</v>
+      </c>
+      <c r="O27" s="62">
+        <v>1060</v>
+      </c>
+      <c r="P27" s="62">
+        <v>2240</v>
+      </c>
+      <c r="Q27" s="62">
+        <v>1</v>
+      </c>
+      <c r="R27" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S27" s="68">
+        <v>1</v>
+      </c>
+      <c r="T27" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" s="76"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="63"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="62"/>
-      <c r="R28" s="62"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="74"/>
-      <c r="U28" s="77"/>
+      <c r="A28" s="64">
+        <v>20210254</v>
+      </c>
+      <c r="B28" s="69">
+        <v>44617</v>
+      </c>
+      <c r="C28" s="52">
+        <v>71000</v>
+      </c>
+      <c r="D28" s="52">
+        <v>1200</v>
+      </c>
+      <c r="E28" s="62">
+        <v>240</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="60">
+        <v>11100</v>
+      </c>
+      <c r="I28" s="62">
+        <v>1340</v>
+      </c>
+      <c r="J28" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K28" s="62">
+        <v>7</v>
+      </c>
+      <c r="L28" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M28" s="63">
+        <v>1</v>
+      </c>
+      <c r="N28" s="60">
+        <v>10500</v>
+      </c>
+      <c r="O28" s="62">
+        <v>1200</v>
+      </c>
+      <c r="P28" s="62">
+        <v>2240</v>
+      </c>
+      <c r="Q28" s="62">
+        <v>1</v>
+      </c>
+      <c r="R28" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S28" s="68">
+        <v>1</v>
+      </c>
+      <c r="T28" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="U28" s="76"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
@@ -6864,8 +7001,8 @@
       <c r="Q29" s="62"/>
       <c r="R29" s="62"/>
       <c r="S29" s="68"/>
-      <c r="T29" s="74"/>
-      <c r="U29" s="77"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="76"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="64"/>
@@ -6887,8 +7024,8 @@
       <c r="Q30" s="62"/>
       <c r="R30" s="62"/>
       <c r="S30" s="68"/>
-      <c r="T30" s="74"/>
-      <c r="U30" s="77"/>
+      <c r="T30" s="73"/>
+      <c r="U30" s="76"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="64"/>
@@ -6910,8 +7047,8 @@
       <c r="Q31" s="62"/>
       <c r="R31" s="62"/>
       <c r="S31" s="68"/>
-      <c r="T31" s="74"/>
-      <c r="U31" s="77"/>
+      <c r="T31" s="73"/>
+      <c r="U31" s="76"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="64"/>
@@ -6933,8 +7070,8 @@
       <c r="Q32" s="62"/>
       <c r="R32" s="62"/>
       <c r="S32" s="68"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="77"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="76"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="64"/>
@@ -6956,8 +7093,8 @@
       <c r="Q33" s="62"/>
       <c r="R33" s="62"/>
       <c r="S33" s="68"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="77"/>
+      <c r="T33" s="73"/>
+      <c r="U33" s="76"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="64"/>
@@ -6979,8 +7116,8 @@
       <c r="Q34" s="62"/>
       <c r="R34" s="62"/>
       <c r="S34" s="68"/>
-      <c r="T34" s="74"/>
-      <c r="U34" s="77"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="76"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="64"/>
@@ -7002,8 +7139,8 @@
       <c r="Q35" s="62"/>
       <c r="R35" s="62"/>
       <c r="S35" s="68"/>
-      <c r="T35" s="74"/>
-      <c r="U35" s="77"/>
+      <c r="T35" s="73"/>
+      <c r="U35" s="76"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="64"/>
@@ -7025,8 +7162,8 @@
       <c r="Q36" s="62"/>
       <c r="R36" s="62"/>
       <c r="S36" s="68"/>
-      <c r="T36" s="74"/>
-      <c r="U36" s="77"/>
+      <c r="T36" s="73"/>
+      <c r="U36" s="76"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="64"/>
@@ -7048,8 +7185,8 @@
       <c r="Q37" s="62"/>
       <c r="R37" s="62"/>
       <c r="S37" s="68"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="77"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="76"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="64"/>
@@ -7071,8 +7208,8 @@
       <c r="Q38" s="62"/>
       <c r="R38" s="62"/>
       <c r="S38" s="68"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="77"/>
+      <c r="T38" s="73"/>
+      <c r="U38" s="76"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="64"/>
@@ -7094,8 +7231,8 @@
       <c r="Q39" s="62"/>
       <c r="R39" s="62"/>
       <c r="S39" s="68"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="77"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="76"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="64"/>
@@ -7117,8 +7254,8 @@
       <c r="Q40" s="62"/>
       <c r="R40" s="62"/>
       <c r="S40" s="68"/>
-      <c r="T40" s="74"/>
-      <c r="U40" s="77"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="76"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="64"/>
@@ -7140,8 +7277,8 @@
       <c r="Q41" s="62"/>
       <c r="R41" s="62"/>
       <c r="S41" s="68"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="77"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="76"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="64"/>
@@ -7163,8 +7300,8 @@
       <c r="Q42" s="62"/>
       <c r="R42" s="62"/>
       <c r="S42" s="68"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="77"/>
+      <c r="T42" s="73"/>
+      <c r="U42" s="76"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="64"/>
@@ -7186,8 +7323,8 @@
       <c r="Q43" s="62"/>
       <c r="R43" s="62"/>
       <c r="S43" s="68"/>
-      <c r="T43" s="74"/>
-      <c r="U43" s="77"/>
+      <c r="T43" s="73"/>
+      <c r="U43" s="76"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="64"/>
@@ -7209,8 +7346,8 @@
       <c r="Q44" s="62"/>
       <c r="R44" s="62"/>
       <c r="S44" s="68"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="77"/>
+      <c r="T44" s="73"/>
+      <c r="U44" s="76"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="64"/>
@@ -7232,8 +7369,8 @@
       <c r="Q45" s="62"/>
       <c r="R45" s="62"/>
       <c r="S45" s="68"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="77"/>
+      <c r="T45" s="73"/>
+      <c r="U45" s="76"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="64"/>
@@ -7255,8 +7392,8 @@
       <c r="Q46" s="62"/>
       <c r="R46" s="62"/>
       <c r="S46" s="68"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="77"/>
+      <c r="T46" s="73"/>
+      <c r="U46" s="76"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
@@ -7278,8 +7415,8 @@
       <c r="Q47" s="62"/>
       <c r="R47" s="62"/>
       <c r="S47" s="68"/>
-      <c r="T47" s="74"/>
-      <c r="U47" s="77"/>
+      <c r="T47" s="73"/>
+      <c r="U47" s="76"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="64"/>
@@ -7301,8 +7438,8 @@
       <c r="Q48" s="62"/>
       <c r="R48" s="62"/>
       <c r="S48" s="68"/>
-      <c r="T48" s="74"/>
-      <c r="U48" s="77"/>
+      <c r="T48" s="73"/>
+      <c r="U48" s="76"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="64"/>
@@ -7324,8 +7461,8 @@
       <c r="Q49" s="62"/>
       <c r="R49" s="62"/>
       <c r="S49" s="68"/>
-      <c r="T49" s="74"/>
-      <c r="U49" s="77"/>
+      <c r="T49" s="73"/>
+      <c r="U49" s="76"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="64"/>
@@ -7347,8 +7484,8 @@
       <c r="Q50" s="62"/>
       <c r="R50" s="62"/>
       <c r="S50" s="68"/>
-      <c r="T50" s="74"/>
-      <c r="U50" s="77"/>
+      <c r="T50" s="73"/>
+      <c r="U50" s="76"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="64"/>
@@ -7370,8 +7507,8 @@
       <c r="Q51" s="62"/>
       <c r="R51" s="62"/>
       <c r="S51" s="68"/>
-      <c r="T51" s="74"/>
-      <c r="U51" s="77"/>
+      <c r="T51" s="73"/>
+      <c r="U51" s="76"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="64"/>
@@ -7393,8 +7530,8 @@
       <c r="Q52" s="62"/>
       <c r="R52" s="62"/>
       <c r="S52" s="68"/>
-      <c r="T52" s="74"/>
-      <c r="U52" s="77"/>
+      <c r="T52" s="73"/>
+      <c r="U52" s="76"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="64"/>
@@ -7416,8 +7553,8 @@
       <c r="Q53" s="62"/>
       <c r="R53" s="62"/>
       <c r="S53" s="68"/>
-      <c r="T53" s="74"/>
-      <c r="U53" s="77"/>
+      <c r="T53" s="73"/>
+      <c r="U53" s="76"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="64"/>
@@ -7439,8 +7576,8 @@
       <c r="Q54" s="62"/>
       <c r="R54" s="62"/>
       <c r="S54" s="68"/>
-      <c r="T54" s="74"/>
-      <c r="U54" s="77"/>
+      <c r="T54" s="73"/>
+      <c r="U54" s="76"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="64"/>
@@ -7462,8 +7599,8 @@
       <c r="Q55" s="62"/>
       <c r="R55" s="62"/>
       <c r="S55" s="68"/>
-      <c r="T55" s="74"/>
-      <c r="U55" s="77"/>
+      <c r="T55" s="73"/>
+      <c r="U55" s="76"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="64"/>
@@ -7485,8 +7622,8 @@
       <c r="Q56" s="62"/>
       <c r="R56" s="62"/>
       <c r="S56" s="68"/>
-      <c r="T56" s="74"/>
-      <c r="U56" s="77"/>
+      <c r="T56" s="73"/>
+      <c r="U56" s="76"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="64"/>
@@ -7508,8 +7645,8 @@
       <c r="Q57" s="62"/>
       <c r="R57" s="62"/>
       <c r="S57" s="68"/>
-      <c r="T57" s="74"/>
-      <c r="U57" s="77"/>
+      <c r="T57" s="73"/>
+      <c r="U57" s="76"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="64"/>
@@ -7531,8 +7668,8 @@
       <c r="Q58" s="62"/>
       <c r="R58" s="62"/>
       <c r="S58" s="68"/>
-      <c r="T58" s="74"/>
-      <c r="U58" s="77"/>
+      <c r="T58" s="73"/>
+      <c r="U58" s="76"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="64"/>
@@ -7554,8 +7691,8 @@
       <c r="Q59" s="62"/>
       <c r="R59" s="62"/>
       <c r="S59" s="68"/>
-      <c r="T59" s="74"/>
-      <c r="U59" s="77"/>
+      <c r="T59" s="73"/>
+      <c r="U59" s="76"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="64"/>
@@ -7577,8 +7714,8 @@
       <c r="Q60" s="62"/>
       <c r="R60" s="62"/>
       <c r="S60" s="68"/>
-      <c r="T60" s="74"/>
-      <c r="U60" s="77"/>
+      <c r="T60" s="73"/>
+      <c r="U60" s="76"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="64"/>
@@ -7600,8 +7737,8 @@
       <c r="Q61" s="62"/>
       <c r="R61" s="62"/>
       <c r="S61" s="68"/>
-      <c r="T61" s="74"/>
-      <c r="U61" s="77"/>
+      <c r="T61" s="73"/>
+      <c r="U61" s="76"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="64"/>
@@ -7623,8 +7760,8 @@
       <c r="Q62" s="62"/>
       <c r="R62" s="62"/>
       <c r="S62" s="68"/>
-      <c r="T62" s="74"/>
-      <c r="U62" s="77"/>
+      <c r="T62" s="73"/>
+      <c r="U62" s="76"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="64"/>
@@ -7646,8 +7783,8 @@
       <c r="Q63" s="62"/>
       <c r="R63" s="62"/>
       <c r="S63" s="68"/>
-      <c r="T63" s="74"/>
-      <c r="U63" s="77"/>
+      <c r="T63" s="73"/>
+      <c r="U63" s="76"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="64"/>
@@ -7669,8 +7806,8 @@
       <c r="Q64" s="62"/>
       <c r="R64" s="62"/>
       <c r="S64" s="68"/>
-      <c r="T64" s="74"/>
-      <c r="U64" s="77"/>
+      <c r="T64" s="73"/>
+      <c r="U64" s="76"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="64"/>
@@ -7692,8 +7829,8 @@
       <c r="Q65" s="62"/>
       <c r="R65" s="62"/>
       <c r="S65" s="68"/>
-      <c r="T65" s="74"/>
-      <c r="U65" s="77"/>
+      <c r="T65" s="73"/>
+      <c r="U65" s="76"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="64"/>
@@ -7715,8 +7852,8 @@
       <c r="Q66" s="62"/>
       <c r="R66" s="62"/>
       <c r="S66" s="68"/>
-      <c r="T66" s="74"/>
-      <c r="U66" s="77"/>
+      <c r="T66" s="73"/>
+      <c r="U66" s="76"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="64"/>
@@ -7738,8 +7875,8 @@
       <c r="Q67" s="62"/>
       <c r="R67" s="62"/>
       <c r="S67" s="68"/>
-      <c r="T67" s="74"/>
-      <c r="U67" s="77"/>
+      <c r="T67" s="73"/>
+      <c r="U67" s="76"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="64"/>
@@ -7761,8 +7898,8 @@
       <c r="Q68" s="62"/>
       <c r="R68" s="62"/>
       <c r="S68" s="68"/>
-      <c r="T68" s="74"/>
-      <c r="U68" s="77"/>
+      <c r="T68" s="73"/>
+      <c r="U68" s="76"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="64"/>
@@ -7784,8 +7921,8 @@
       <c r="Q69" s="62"/>
       <c r="R69" s="62"/>
       <c r="S69" s="68"/>
-      <c r="T69" s="74"/>
-      <c r="U69" s="77"/>
+      <c r="T69" s="73"/>
+      <c r="U69" s="76"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="64"/>
@@ -7807,8 +7944,8 @@
       <c r="Q70" s="62"/>
       <c r="R70" s="62"/>
       <c r="S70" s="68"/>
-      <c r="T70" s="74"/>
-      <c r="U70" s="77"/>
+      <c r="T70" s="73"/>
+      <c r="U70" s="76"/>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="64"/>
@@ -7830,8 +7967,8 @@
       <c r="Q71" s="62"/>
       <c r="R71" s="62"/>
       <c r="S71" s="68"/>
-      <c r="T71" s="74"/>
-      <c r="U71" s="77"/>
+      <c r="T71" s="73"/>
+      <c r="U71" s="76"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="64"/>
@@ -7853,8 +7990,8 @@
       <c r="Q72" s="62"/>
       <c r="R72" s="62"/>
       <c r="S72" s="68"/>
-      <c r="T72" s="74"/>
-      <c r="U72" s="77"/>
+      <c r="T72" s="73"/>
+      <c r="U72" s="76"/>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="64"/>
@@ -7876,8 +8013,8 @@
       <c r="Q73" s="62"/>
       <c r="R73" s="62"/>
       <c r="S73" s="68"/>
-      <c r="T73" s="74"/>
-      <c r="U73" s="77"/>
+      <c r="T73" s="73"/>
+      <c r="U73" s="76"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="64"/>
@@ -7899,8 +8036,8 @@
       <c r="Q74" s="62"/>
       <c r="R74" s="62"/>
       <c r="S74" s="68"/>
-      <c r="T74" s="74"/>
-      <c r="U74" s="77"/>
+      <c r="T74" s="73"/>
+      <c r="U74" s="76"/>
     </row>
     <row r="75" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="65"/>
@@ -7922,8 +8059,8 @@
       <c r="Q75" s="62"/>
       <c r="R75" s="62"/>
       <c r="S75" s="68"/>
-      <c r="T75" s="75"/>
-      <c r="U75" s="78"/>
+      <c r="T75" s="74"/>
+      <c r="U75" s="77"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:T20" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
@@ -8014,19 +8151,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="85">
+      <c r="B2" s="84">
         <v>5898</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="84">
         <v>2240</v>
       </c>
-      <c r="D2" s="85">
+      <c r="D2" s="84">
         <v>2340</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="84" t="s">
         <v>115</v>
       </c>
       <c r="F2" s="50"/>
@@ -8041,7 +8178,7 @@
       <c r="C3" s="52">
         <v>2240</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="84">
         <v>2340</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -8059,7 +8196,7 @@
       <c r="C4" s="52">
         <v>2580</v>
       </c>
-      <c r="D4" s="85">
+      <c r="D4" s="84">
         <v>2340</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -8092,7 +8229,7 @@
       <c r="B6" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="92">
+      <c r="C6" s="91">
         <v>3000</v>
       </c>
       <c r="D6" s="52" t="s">

</xml_diff>

<commit_message>
Corregge la copiatura del nastro base quando si clona l'imballo
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F128356-1B31-46C3-96BE-5B1650D37765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E8A06-F674-4576-A9EA-7AB7732B7000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Rinforzi" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$28</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="145">
   <si>
     <t>Diagonali</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>Non c'è bisongo del panino?</t>
+  </si>
+  <si>
+    <t>OC 24526</t>
   </si>
 </sst>
 </file>
@@ -1414,6 +1417,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1473,9 +1479,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2953,10 +2956,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="93"/>
+      <c r="B1" s="94"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3490,21 +3493,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="94" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="95"/>
-      <c r="I1" s="97" t="s">
+      <c r="H1" s="96"/>
+      <c r="I1" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="98" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3533,8 +3536,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -3887,7 +3890,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3939,7 +3942,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="52">
@@ -3957,18 +3960,25 @@
         <v>67</v>
       </c>
       <c r="B4" s="1">
-        <v>100000</v>
+        <v>36000</v>
       </c>
       <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
+      <c r="D4" s="52">
+        <v>80</v>
+      </c>
+      <c r="E4" s="52">
+        <v>350</v>
+      </c>
+      <c r="F4" s="52">
+        <v>250</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="1">
-        <v>630</v>
+        <v>250</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -3979,7 +3989,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="1">
-        <v>900</v>
+        <v>350</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
@@ -3998,14 +4008,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4033,22 +4043,22 @@
       </c>
       <c r="B11" s="1">
         <f>B2-B6/2</f>
-        <v>14550</v>
+        <v>14825</v>
       </c>
       <c r="C11" s="1">
         <f>IF(ISEVEN(A11),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>1413.7166941154069</v>
+        <v>549.77871437821375</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
         <f>MAX(D11:D23)</f>
-        <v>2700</v>
+        <v>1050</v>
       </c>
       <c r="F11" s="1">
         <f>SUM(B11:B32) + SUM(C11:C32)</f>
-        <v>88029.357668809753</v>
+        <v>88721.482010778898</v>
       </c>
       <c r="N11">
         <f>2240/300</f>
@@ -4061,15 +4071,15 @@
       </c>
       <c r="B12" s="1">
         <f>IF(ISEVEN(A12),B11-$B$5*0.5-$B$3,B11-$B$5*0.5-$B$6*0.5)</f>
-        <v>14175</v>
+        <v>14620</v>
       </c>
       <c r="C12" s="1">
         <f>IF(ISEVEN(A12),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>1484.4025288211774</v>
+        <v>589.0486225480862</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ref="D12:D16" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
-        <v>900</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4078,15 +4088,15 @@
       </c>
       <c r="B13" s="1">
         <f>IF(ISEVEN(A13),B12-$B$5*0.5-$B$3,B12-$B$5*0.5-$B$6*0.5)</f>
-        <v>13410</v>
+        <v>14320</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:C16" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
-        <v>1413.7166941154069</v>
+        <v>549.77871437821375</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4095,15 +4105,15 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ref="B14:B16" si="2">IF(ISEVEN(A14),B13-$B$5*0.5-$B$3,B13-$B$5*0.5-$B$6*0.5)</f>
-        <v>13035</v>
+        <v>14115</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>1484.4025288211774</v>
+        <v>589.0486225480862</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4112,15 +4122,15 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="2"/>
-        <v>12270</v>
+        <v>13815</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>1413.7166941154069</v>
+        <v>549.77871437821375</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>810</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4129,15 +4139,15 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="2"/>
-        <v>11895</v>
+        <v>13610</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>1484.4025288211774</v>
+        <v>589.0486225480862</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4433,14 +4443,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -4586,7 +4596,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="101" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -4609,7 +4619,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -4630,7 +4640,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="102"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -4642,7 +4652,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="101"/>
+      <c r="F19" s="102"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -4654,7 +4664,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="101"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -4666,7 +4676,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="101"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -4678,7 +4688,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="101"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -4690,7 +4700,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="102"/>
+      <c r="F23" s="103"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -4886,14 +4896,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5210,7 +5220,7 @@
   <dimension ref="A1:AG75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5238,35 +5248,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="103" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="103" t="s">
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="109" t="s">
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="110" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="109" t="s">
+      <c r="U1" s="110" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5328,8 +5338,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="110"/>
-      <c r="U2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="112"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -6827,7 +6837,7 @@
       <c r="L26" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="M26" s="112">
+      <c r="M26" s="92">
         <v>1</v>
       </c>
       <c r="N26" s="60">
@@ -6982,26 +6992,66 @@
       <c r="U28" s="76"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="62"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="62"/>
-      <c r="R29" s="62"/>
-      <c r="S29" s="68"/>
-      <c r="T29" s="73"/>
+      <c r="A29" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="69">
+        <v>44582</v>
+      </c>
+      <c r="C29" s="52">
+        <v>75500</v>
+      </c>
+      <c r="D29" s="52">
+        <v>800</v>
+      </c>
+      <c r="E29" s="62">
+        <v>120</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="60">
+        <v>7300</v>
+      </c>
+      <c r="I29" s="62">
+        <v>2240</v>
+      </c>
+      <c r="J29" s="62">
+        <v>949</v>
+      </c>
+      <c r="K29" s="62">
+        <v>1</v>
+      </c>
+      <c r="L29" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M29" s="63">
+        <v>1</v>
+      </c>
+      <c r="N29" s="60">
+        <v>7500</v>
+      </c>
+      <c r="O29" s="62">
+        <v>950</v>
+      </c>
+      <c r="P29" s="62">
+        <v>2240</v>
+      </c>
+      <c r="Q29" s="62">
+        <v>1</v>
+      </c>
+      <c r="R29" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S29" s="68">
+        <v>1</v>
+      </c>
+      <c r="T29" s="73" t="s">
+        <v>23</v>
+      </c>
       <c r="U29" s="76"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -8063,7 +8113,7 @@
       <c r="U75" s="77"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T20" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
+  <autoFilter ref="A2:T28" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
   <mergeCells count="5">
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>

</xml_diff>

<commit_message>
Sistema imballi per nastri solo bordi e solo tazze
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E8A06-F674-4576-A9EA-7AB7732B7000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873D6E7-9965-4DFB-B367-85DF9B0164D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Rinforzi" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -5220,7 +5220,7 @@
   <dimension ref="A1:AG75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="D29" sqref="D29:P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8113,7 +8113,7 @@
       <c r="U75" s="77"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T28" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
+  <autoFilter ref="A2:T29" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
   <mergeCells count="5">
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>

</xml_diff>

<commit_message>
Aggiunge AY come qualità nei nastri base
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39ADF3D-D5B4-487B-9E69-29CBB7BE009C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9352D1D1-775A-4459-8D3D-EBF551EF884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -3827,7 +3827,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correzione per imballo 2021414
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9352D1D1-775A-4459-8D3D-EBF551EF884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505E9D3A-1AB9-4A57-8CFD-7157F04BC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="238">
   <si>
     <t>Diagonali</t>
   </si>
@@ -1736,6 +1736,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1803,34 +1831,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3309,10 +3309,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="108"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3826,7 +3826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DED6D3E-77D1-4B63-8B9E-33B280502E7D}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -4286,21 +4286,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="95" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="96"/>
-      <c r="I1" s="98" t="s">
+      <c r="H1" s="110"/>
+      <c r="I1" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="112" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4329,8 +4329,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -4801,14 +4801,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5236,14 +5236,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5389,7 +5389,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="101" t="s">
+      <c r="F16" s="115" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -5412,7 +5412,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="102"/>
+      <c r="F17" s="116"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -5433,7 +5433,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="102"/>
+      <c r="F18" s="116"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -5445,7 +5445,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="102"/>
+      <c r="F19" s="116"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -5457,7 +5457,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="102"/>
+      <c r="F20" s="116"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -5469,7 +5469,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="102"/>
+      <c r="F21" s="116"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -5481,7 +5481,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="102"/>
+      <c r="F22" s="116"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -5493,7 +5493,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="103"/>
+      <c r="F23" s="117"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -5689,14 +5689,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -6012,8 +6012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6041,35 +6041,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="104" t="s">
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="104" t="s">
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="110" t="s">
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="124" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="110" t="s">
+      <c r="U1" s="124" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6131,8 +6131,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="111"/>
-      <c r="U2" s="112"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="126"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -7911,26 +7911,66 @@
       <c r="U30" s="76"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="62"/>
-      <c r="R31" s="62"/>
-      <c r="S31" s="68"/>
-      <c r="T31" s="73"/>
+      <c r="A31" s="64">
+        <v>20210414</v>
+      </c>
+      <c r="B31" s="69">
+        <v>44666</v>
+      </c>
+      <c r="C31" s="52">
+        <v>67000</v>
+      </c>
+      <c r="D31" s="52">
+        <v>1600</v>
+      </c>
+      <c r="E31" s="62">
+        <v>280</v>
+      </c>
+      <c r="F31" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" s="60">
+        <v>13600</v>
+      </c>
+      <c r="I31" s="62">
+        <v>1740</v>
+      </c>
+      <c r="J31" s="62">
+        <v>2240</v>
+      </c>
+      <c r="K31" s="62">
+        <v>1</v>
+      </c>
+      <c r="L31" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M31" s="63">
+        <v>1</v>
+      </c>
+      <c r="N31" s="60">
+        <v>13500</v>
+      </c>
+      <c r="O31" s="62">
+        <v>1800</v>
+      </c>
+      <c r="P31" s="62">
+        <v>2500</v>
+      </c>
+      <c r="Q31" s="62">
+        <v>1</v>
+      </c>
+      <c r="R31" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S31" s="68">
+        <v>1</v>
+      </c>
+      <c r="T31" s="73" t="s">
+        <v>23</v>
+      </c>
       <c r="U31" s="76"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -9272,34 +9312,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="118"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="113" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="127" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="113" t="s">
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="127" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="115"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="129"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="101" t="s">
         <v>113</v>
       </c>
       <c r="C2" s="64" t="s">
@@ -9323,7 +9363,7 @@
       <c r="I2" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="116" t="s">
+      <c r="J2" s="93" t="s">
         <v>178</v>
       </c>
       <c r="K2" s="64" t="s">
@@ -9347,7 +9387,7 @@
       <c r="Q2" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="R2" s="116" t="s">
+      <c r="R2" s="93" t="s">
         <v>173</v>
       </c>
     </row>
@@ -9355,7 +9395,7 @@
       <c r="A3" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="125"/>
+      <c r="B3" s="102"/>
       <c r="C3" s="64" t="s">
         <v>164</v>
       </c>
@@ -9368,7 +9408,7 @@
       <c r="F3" s="52">
         <v>1000</v>
       </c>
-      <c r="G3" s="122" t="s">
+      <c r="G3" s="99" t="s">
         <v>171</v>
       </c>
       <c r="H3" s="52" t="s">
@@ -9377,14 +9417,14 @@
       <c r="I3" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="117" t="s">
+      <c r="J3" s="94" t="s">
         <v>102</v>
       </c>
       <c r="K3" s="64" t="s">
         <v>164</v>
       </c>
       <c r="L3" s="52"/>
-      <c r="M3" s="122" t="s">
+      <c r="M3" s="99" t="s">
         <v>171</v>
       </c>
       <c r="N3" s="52" t="s">
@@ -9395,7 +9435,7 @@
         <v>1000</v>
       </c>
       <c r="Q3" s="52"/>
-      <c r="R3" s="116" t="s">
+      <c r="R3" s="93" t="s">
         <v>175</v>
       </c>
     </row>
@@ -9403,7 +9443,7 @@
       <c r="A4" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="126"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="60" t="s">
         <v>165</v>
       </c>
@@ -9423,13 +9463,13 @@
       <c r="I4" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="J4" s="120">
+      <c r="J4" s="97">
         <v>120</v>
       </c>
       <c r="K4" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="L4" s="122" t="s">
+      <c r="L4" s="99" t="s">
         <v>179</v>
       </c>
       <c r="M4" s="52" t="s">
@@ -9443,13 +9483,13 @@
       <c r="Q4" s="52">
         <v>120</v>
       </c>
-      <c r="R4" s="120"/>
+      <c r="R4" s="97"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="64"/>
       <c r="D5" s="52" t="s">
         <v>181</v>
@@ -9458,13 +9498,13 @@
         <v>171</v>
       </c>
       <c r="F5" s="52"/>
-      <c r="G5" s="122" t="s">
+      <c r="G5" s="99" t="s">
         <v>178</v>
       </c>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="122" t="s">
+      <c r="J5" s="97"/>
+      <c r="K5" s="99" t="s">
         <v>181</v>
       </c>
       <c r="M5" s="52" t="s">
@@ -9473,16 +9513,16 @@
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
       <c r="P5" s="52"/>
-      <c r="Q5" s="122" t="s">
+      <c r="Q5" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="R5" s="120"/>
+      <c r="R5" s="97"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="B6" s="125"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="64" t="s">
         <v>189</v>
       </c>
@@ -9494,18 +9534,18 @@
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
-      <c r="H6" s="128" t="s">
+      <c r="H6" s="105" t="s">
         <v>190</v>
       </c>
       <c r="I6" s="52"/>
-      <c r="J6" s="120"/>
+      <c r="J6" s="97"/>
       <c r="K6" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="L6" s="122" t="s">
+      <c r="L6" s="99" t="s">
         <v>179</v>
       </c>
-      <c r="M6" s="122" t="s">
+      <c r="M6" s="99" t="s">
         <v>171</v>
       </c>
       <c r="N6" s="52"/>
@@ -9514,13 +9554,13 @@
       <c r="Q6" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="R6" s="120"/>
+      <c r="R6" s="97"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="102" t="s">
         <v>185</v>
       </c>
       <c r="C7" s="64"/>
@@ -9530,8 +9570,8 @@
       <c r="G7" s="52"/>
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="122" t="s">
+      <c r="J7" s="97"/>
+      <c r="K7" s="99" t="s">
         <v>182</v>
       </c>
       <c r="M7" s="52" t="s">
@@ -9545,13 +9585,13 @@
       <c r="Q7" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="R7" s="120"/>
+      <c r="R7" s="97"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="102" t="s">
         <v>192</v>
       </c>
       <c r="C8" s="64"/>
@@ -9560,28 +9600,28 @@
         <v>191</v>
       </c>
       <c r="F8" s="52"/>
-      <c r="G8" s="122" t="s">
+      <c r="G8" s="99" t="s">
         <v>178</v>
       </c>
       <c r="H8" s="52"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="120"/>
+      <c r="J8" s="97"/>
       <c r="K8" s="64"/>
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
-      <c r="Q8" s="122" t="s">
+      <c r="Q8" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="R8" s="120"/>
+      <c r="R8" s="97"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="102" t="s">
         <v>192</v>
       </c>
       <c r="C9" s="64"/>
@@ -9590,12 +9630,12 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="52"/>
-      <c r="G9" s="122" t="s">
+      <c r="G9" s="99" t="s">
         <v>178</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="52"/>
-      <c r="J9" s="120"/>
+      <c r="J9" s="97"/>
       <c r="K9" s="52" t="s">
         <v>183</v>
       </c>
@@ -9604,16 +9644,16 @@
       <c r="N9" s="52"/>
       <c r="O9" s="52"/>
       <c r="P9" s="52"/>
-      <c r="Q9" s="122" t="s">
+      <c r="Q9" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="R9" s="120"/>
+      <c r="R9" s="97"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="102" t="s">
         <v>193</v>
       </c>
       <c r="C10" s="64"/>
@@ -9625,7 +9665,7 @@
       <c r="G10" s="52"/>
       <c r="H10" s="52"/>
       <c r="I10" s="52"/>
-      <c r="J10" s="120" t="s">
+      <c r="J10" s="97" t="s">
         <v>178</v>
       </c>
       <c r="K10" s="52" t="s">
@@ -9641,13 +9681,13 @@
       <c r="Q10" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="R10" s="120"/>
+      <c r="R10" s="97"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="102" t="s">
         <v>192</v>
       </c>
       <c r="C11" s="64" t="s">
@@ -9660,12 +9700,12 @@
         <v>164</v>
       </c>
       <c r="F11" s="52"/>
-      <c r="G11" s="122" t="s">
+      <c r="G11" s="99" t="s">
         <v>178</v>
       </c>
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
-      <c r="J11" s="120"/>
+      <c r="J11" s="97"/>
       <c r="K11" s="64" t="s">
         <v>201</v>
       </c>
@@ -9674,16 +9714,16 @@
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
       <c r="P11" s="52"/>
-      <c r="Q11" s="122" t="s">
+      <c r="Q11" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="R11" s="120"/>
+      <c r="R11" s="97"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="76" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="102" t="s">
         <v>197</v>
       </c>
       <c r="C12" s="64"/>
@@ -9694,12 +9734,12 @@
         <v>166</v>
       </c>
       <c r="F12" s="52"/>
-      <c r="G12" s="122" t="s">
+      <c r="G12" s="99" t="s">
         <v>178</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
-      <c r="J12" s="120"/>
+      <c r="J12" s="97"/>
       <c r="K12" s="64" t="s">
         <v>166</v>
       </c>
@@ -9709,13 +9749,13 @@
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
       <c r="Q12" s="52"/>
-      <c r="R12" s="120"/>
+      <c r="R12" s="97"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="125" t="s">
+      <c r="B13" s="102" t="s">
         <v>197</v>
       </c>
       <c r="C13" s="64"/>
@@ -9725,27 +9765,27 @@
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
       <c r="I13" s="52"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="129" t="s">
+      <c r="J13" s="97"/>
+      <c r="K13" s="106" t="s">
         <v>198</v>
       </c>
       <c r="L13" s="52"/>
-      <c r="M13" s="122" t="s">
+      <c r="M13" s="99" t="s">
         <v>171</v>
       </c>
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
-      <c r="Q13" s="122" t="s">
+      <c r="Q13" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="R13" s="120"/>
+      <c r="R13" s="97"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="125"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="64"/>
       <c r="D14" s="52"/>
       <c r="E14" s="52"/>
@@ -9753,7 +9793,7 @@
       <c r="G14" s="52"/>
       <c r="H14" s="52"/>
       <c r="I14" s="52"/>
-      <c r="J14" s="120"/>
+      <c r="J14" s="97"/>
       <c r="K14" s="64" t="s">
         <v>199</v>
       </c>
@@ -9763,13 +9803,13 @@
       <c r="O14" s="52"/>
       <c r="P14" s="52"/>
       <c r="Q14" s="52"/>
-      <c r="R14" s="120"/>
+      <c r="R14" s="97"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="125" t="s">
+      <c r="B15" s="102" t="s">
         <v>200</v>
       </c>
       <c r="C15" s="64"/>
@@ -9779,7 +9819,7 @@
       <c r="G15" s="52"/>
       <c r="H15" s="52"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="120"/>
+      <c r="J15" s="97"/>
       <c r="K15" s="64"/>
       <c r="L15" s="52"/>
       <c r="M15" s="52"/>
@@ -9787,13 +9827,13 @@
       <c r="O15" s="52"/>
       <c r="P15" s="52"/>
       <c r="Q15" s="52"/>
-      <c r="R15" s="120"/>
+      <c r="R15" s="97"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="125"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="64"/>
       <c r="D16" s="52"/>
       <c r="E16" s="52"/>
@@ -9801,7 +9841,7 @@
       <c r="G16" s="52"/>
       <c r="H16" s="52"/>
       <c r="I16" s="52"/>
-      <c r="J16" s="120"/>
+      <c r="J16" s="97"/>
       <c r="K16" s="64"/>
       <c r="L16" s="52"/>
       <c r="M16" s="52"/>
@@ -9809,13 +9849,13 @@
       <c r="O16" s="52"/>
       <c r="P16" s="52"/>
       <c r="Q16" s="52"/>
-      <c r="R16" s="120"/>
+      <c r="R16" s="97"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>159</v>
       </c>
-      <c r="B17" s="125"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="64"/>
       <c r="D17" s="52"/>
       <c r="E17" s="52"/>
@@ -9825,7 +9865,7 @@
       </c>
       <c r="H17" s="52"/>
       <c r="I17" s="52"/>
-      <c r="J17" s="120"/>
+      <c r="J17" s="97"/>
       <c r="K17" s="64"/>
       <c r="L17" s="52"/>
       <c r="M17" s="52"/>
@@ -9833,13 +9873,13 @@
       <c r="O17" s="52"/>
       <c r="P17" s="52"/>
       <c r="Q17" s="52"/>
-      <c r="R17" s="120"/>
+      <c r="R17" s="97"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="64"/>
       <c r="D18" s="52"/>
       <c r="E18" s="52"/>
@@ -9847,7 +9887,7 @@
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
       <c r="I18" s="52"/>
-      <c r="J18" s="120"/>
+      <c r="J18" s="97"/>
       <c r="K18" s="64"/>
       <c r="L18" s="52"/>
       <c r="M18" s="52"/>
@@ -9855,13 +9895,13 @@
       <c r="O18" s="52"/>
       <c r="P18" s="52"/>
       <c r="Q18" s="52"/>
-      <c r="R18" s="120"/>
+      <c r="R18" s="97"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="125"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="64"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
@@ -9869,7 +9909,7 @@
       <c r="G19" s="52"/>
       <c r="H19" s="52"/>
       <c r="I19" s="52"/>
-      <c r="J19" s="120"/>
+      <c r="J19" s="97"/>
       <c r="K19" s="64"/>
       <c r="L19" s="52"/>
       <c r="M19" s="52"/>
@@ -9877,13 +9917,13 @@
       <c r="O19" s="52"/>
       <c r="P19" s="52"/>
       <c r="Q19" s="52"/>
-      <c r="R19" s="120"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="125"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="64"/>
       <c r="D20" s="52"/>
       <c r="E20" s="52"/>
@@ -9891,7 +9931,7 @@
       <c r="G20" s="52"/>
       <c r="H20" s="52"/>
       <c r="I20" s="52"/>
-      <c r="J20" s="120"/>
+      <c r="J20" s="97"/>
       <c r="K20" s="64"/>
       <c r="L20" s="52"/>
       <c r="M20" s="52"/>
@@ -9899,13 +9939,13 @@
       <c r="O20" s="52"/>
       <c r="P20" s="52"/>
       <c r="Q20" s="52"/>
-      <c r="R20" s="120"/>
+      <c r="R20" s="97"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="B21" s="127"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="65"/>
       <c r="D21" s="66"/>
       <c r="E21" s="66"/>
@@ -9913,7 +9953,7 @@
       <c r="G21" s="66"/>
       <c r="H21" s="66"/>
       <c r="I21" s="66"/>
-      <c r="J21" s="121"/>
+      <c r="J21" s="98"/>
       <c r="K21" s="65"/>
       <c r="L21" s="66"/>
       <c r="M21" s="66"/>
@@ -9921,7 +9961,7 @@
       <c r="O21" s="66"/>
       <c r="P21" s="66"/>
       <c r="Q21" s="66"/>
-      <c r="R21" s="121"/>
+      <c r="R21" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Controllo sulla larghezza se troppo alta
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505E9D3A-1AB9-4A57-8CFD-7157F04BC97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CB6F2B-9630-4A7A-A954-AFE8B394C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
@@ -2324,8 +2324,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13535025" y="3343275"/>
-          <a:ext cx="600075" cy="1371600"/>
+          <a:off x="13535025" y="2524125"/>
+          <a:ext cx="600075" cy="2190750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4682,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5572EF6F-715B-412F-9B2D-240169A3DEA6}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4717,7 +4717,7 @@
         <v>65</v>
       </c>
       <c r="B2" s="1">
-        <v>15000</v>
+        <v>5800</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="52">
@@ -4735,7 +4735,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="52">
@@ -4753,7 +4753,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="1">
-        <v>36000</v>
+        <v>50000</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="52">
@@ -4774,8 +4774,15 @@
         <v>250</v>
       </c>
       <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
+      <c r="D5" s="53">
+        <v>60</v>
+      </c>
+      <c r="E5" s="53">
+        <v>350</v>
+      </c>
+      <c r="F5" s="53">
+        <v>250</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -4836,7 +4843,7 @@
       </c>
       <c r="B11" s="1">
         <f>B2-B6/2</f>
-        <v>14825</v>
+        <v>5625</v>
       </c>
       <c r="C11" s="1">
         <f>IF(ISEVEN(A11),$B$5*PI()*0.75,$B$6*PI()/2)</f>
@@ -4847,11 +4854,11 @@
       </c>
       <c r="E11" s="1">
         <f>MAX(D11:D23)</f>
-        <v>1050</v>
+        <v>1400</v>
       </c>
       <c r="F11" s="1">
         <f>SUM(B11:B32) + SUM(C11:C32)</f>
-        <v>88721.482010778898</v>
+        <v>47230.088062083414</v>
       </c>
       <c r="N11">
         <f>2240/300</f>
@@ -4864,14 +4871,14 @@
       </c>
       <c r="B12" s="1">
         <f>IF(ISEVEN(A12),B11-$B$5*0.5-$B$3,B11-$B$5*0.5-$B$6*0.5)</f>
-        <v>14620</v>
+        <v>5440</v>
       </c>
       <c r="C12" s="1">
         <f>IF(ISEVEN(A12),$B$5*PI()*0.75,$B$6*PI()/2)</f>
         <v>589.0486225480862</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D16" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
+        <f t="shared" ref="D12:D19" si="0">IF(ISEVEN(A12),A12/2*$B$6,(A12-((A12-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>350</v>
       </c>
     </row>
@@ -4881,15 +4888,19 @@
       </c>
       <c r="B13" s="1">
         <f>IF(ISEVEN(A13),B12-$B$5*0.5-$B$3,B12-$B$5*0.5-$B$6*0.5)</f>
-        <v>14320</v>
+        <v>5140</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:C16" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
+        <f t="shared" ref="C13:C19" si="1">IF(ISEVEN(A13),$B$5*PI()*0.75,$B$6*PI()/2)</f>
         <v>549.77871437821375</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>370</v>
+      </c>
+      <c r="E13">
+        <f>6*350</f>
+        <v>2100</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4897,8 +4908,8 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:B16" si="2">IF(ISEVEN(A14),B13-$B$5*0.5-$B$3,B13-$B$5*0.5-$B$6*0.5)</f>
-        <v>14115</v>
+        <f t="shared" ref="B14:B19" si="2">IF(ISEVEN(A14),B13-$B$5*0.5-$B$3,B13-$B$5*0.5-$B$6*0.5)</f>
+        <v>4955</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
@@ -4915,7 +4926,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="2"/>
-        <v>13815</v>
+        <v>4655</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
@@ -4923,7 +4934,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>490</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4932,7 +4943,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="2"/>
-        <v>13610</v>
+        <v>4470</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
@@ -4947,25 +4958,52 @@
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="B17" s="1">
+        <f t="shared" si="2"/>
+        <v>4170</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>549.77871437821375</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="1">
+        <f t="shared" si="2"/>
+        <v>3985</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>589.0486225480862</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="B19" s="1">
+        <f t="shared" si="2"/>
+        <v>3685</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>549.77871437821375</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
       <c r="I19">
         <v>280</v>
       </c>
@@ -6012,7 +6050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corregge la scelta del trasporto. Veniva confuso il 40ft con il 40ft HQ
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CB6F2B-9630-4A7A-A954-AFE8B394C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD9DB60-9366-4C73-8DCD-8F0C604ED80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPrezziPesi" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$29</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,8 +35,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -104,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="240">
   <si>
     <t>Diagonali</t>
   </si>
@@ -599,9 +602,6 @@
     <t>Movimentazione</t>
   </si>
   <si>
-    <t>Cd_ARGruppo1</t>
-  </si>
-  <si>
     <t>NAS</t>
   </si>
   <si>
@@ -611,12 +611,6 @@
     <t>FIX</t>
   </si>
   <si>
-    <t>Cd_ARGruppo2</t>
-  </si>
-  <si>
-    <t>Cd_ARGruppo3</t>
-  </si>
-  <si>
     <t>LarghezzaMKS</t>
   </si>
   <si>
@@ -650,9 +644,6 @@
     <t>Presenza tele</t>
   </si>
   <si>
-    <t>Cd_ARClasse1</t>
-  </si>
-  <si>
     <t>RAB</t>
   </si>
   <si>
@@ -668,9 +659,6 @@
     <t>Fare un articolo per ogni tipo di raspatura?</t>
   </si>
   <si>
-    <t>Cd_ARClasse2</t>
-  </si>
-  <si>
     <t>Forma</t>
   </si>
   <si>
@@ -822,6 +810,27 @@
   </si>
   <si>
     <t>UM</t>
+  </si>
+  <si>
+    <t>Da rivedere la configurazione</t>
+  </si>
+  <si>
+    <t>Famiglia</t>
+  </si>
+  <si>
+    <t>Gruppo</t>
+  </si>
+  <si>
+    <t>Sottogruppo</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Nella tabella ho indicato in giallo i campi che cambierei</t>
+  </si>
+  <si>
+    <t>Bordo basso, da rivedere la configurazione.</t>
   </si>
 </sst>
 </file>
@@ -832,7 +841,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -897,6 +906,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1512,7 +1529,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1764,6 +1781,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3309,10 +3336,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="108"/>
+      <c r="B1" s="112"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -3840,27 +3867,27 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D2" s="1">
         <v>65</v>
@@ -3868,16 +3895,16 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D3" s="1">
         <v>130</v>
@@ -3885,16 +3912,16 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D4" s="1">
         <v>130</v>
@@ -3902,16 +3929,16 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D5" s="1">
         <v>53</v>
@@ -3919,16 +3946,16 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D6" s="1">
         <v>53</v>
@@ -3936,16 +3963,16 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -3953,16 +3980,16 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D8" s="1">
         <v>130</v>
@@ -3970,16 +3997,16 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1">
         <v>100</v>
@@ -3987,33 +4014,33 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D11" s="1">
         <v>200</v>
@@ -4021,16 +4048,16 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D12" s="1">
         <v>200</v>
@@ -4038,13 +4065,13 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>156</v>
@@ -4055,16 +4082,16 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D14" s="1">
         <v>200</v>
@@ -4072,7 +4099,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4085,16 +4112,16 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -4102,16 +4129,16 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -4119,16 +4146,16 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -4136,7 +4163,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4153,7 +4180,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>114</v>
@@ -4164,13 +4191,13 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>114</v>
@@ -4181,7 +4208,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4286,21 +4313,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="109" t="s">
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="110"/>
-      <c r="I1" s="112" t="s">
+      <c r="H1" s="114"/>
+      <c r="I1" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="112" t="s">
+      <c r="J1" s="116" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4329,8 +4356,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -4682,7 +4709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5572EF6F-715B-412F-9B2D-240169A3DEA6}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -4808,14 +4835,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5274,14 +5301,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5427,7 +5454,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="115" t="s">
+      <c r="F16" s="119" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -5450,7 +5477,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="116"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -5471,7 +5498,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="116"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -5483,7 +5510,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="116"/>
+      <c r="F19" s="120"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -5495,7 +5522,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="116"/>
+      <c r="F20" s="120"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -5507,7 +5534,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="116"/>
+      <c r="F21" s="120"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -5519,7 +5546,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="116"/>
+      <c r="F22" s="120"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -5531,7 +5558,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="117"/>
+      <c r="F23" s="121"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -5727,14 +5754,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -6050,8 +6077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6079,35 +6106,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="125" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="118" t="s">
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="122" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="118" t="s">
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="120"/>
-      <c r="T1" s="124" t="s">
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="124" t="s">
+      <c r="U1" s="128" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6169,8 +6196,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="125"/>
-      <c r="U2" s="126"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="130"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -8012,50 +8039,122 @@
       <c r="U31" s="76"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62"/>
-      <c r="S32" s="68"/>
-      <c r="T32" s="73"/>
-      <c r="U32" s="76"/>
+      <c r="A32" s="64">
+        <v>5501780338</v>
+      </c>
+      <c r="B32" s="69">
+        <v>44718</v>
+      </c>
+      <c r="C32" s="52">
+        <v>69000</v>
+      </c>
+      <c r="D32" s="52">
+        <v>650</v>
+      </c>
+      <c r="E32" s="62">
+        <v>80</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="107">
+        <v>6000</v>
+      </c>
+      <c r="I32" s="62">
+        <v>800</v>
+      </c>
+      <c r="J32" s="70">
+        <v>1720</v>
+      </c>
+      <c r="K32" s="62">
+        <v>7</v>
+      </c>
+      <c r="L32" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M32" s="63">
+        <v>1</v>
+      </c>
+      <c r="N32" s="107">
+        <v>6800</v>
+      </c>
+      <c r="O32" s="62">
+        <v>790</v>
+      </c>
+      <c r="P32" s="70">
+        <v>2240</v>
+      </c>
+      <c r="Q32" s="62">
+        <v>1</v>
+      </c>
+      <c r="R32" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S32" s="68">
+        <v>1</v>
+      </c>
+      <c r="T32" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="U32" s="76" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="63"/>
+      <c r="A33" s="64">
+        <v>20220223</v>
+      </c>
+      <c r="B33" s="69">
+        <v>44754</v>
+      </c>
+      <c r="C33" s="52">
+        <v>40200</v>
+      </c>
+      <c r="D33" s="52">
+        <v>750</v>
+      </c>
+      <c r="E33" s="62">
+        <v>80</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>100</v>
+      </c>
       <c r="H33" s="60"/>
       <c r="I33" s="62"/>
       <c r="J33" s="62"/>
       <c r="K33" s="62"/>
       <c r="L33" s="62"/>
       <c r="M33" s="63"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="68"/>
-      <c r="T33" s="73"/>
-      <c r="U33" s="76"/>
+      <c r="N33" s="60">
+        <v>4000</v>
+      </c>
+      <c r="O33" s="62">
+        <v>900</v>
+      </c>
+      <c r="P33" s="62">
+        <v>1560</v>
+      </c>
+      <c r="Q33" s="62">
+        <v>7</v>
+      </c>
+      <c r="R33" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S33" s="68">
+        <v>1</v>
+      </c>
+      <c r="T33" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="U33" s="76" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="64"/>
@@ -9327,10 +9426,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451D1C50-D088-43D7-86DC-704533E8A29D}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9352,26 +9451,26 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="95"/>
       <c r="B1" s="100"/>
-      <c r="C1" s="127" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="127" t="s">
-        <v>177</v>
-      </c>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="129"/>
+      <c r="C1" s="131" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="131" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="133"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -9380,53 +9479,53 @@
       <c r="B2" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="52" t="s">
+      <c r="H2" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="93" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="L2" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="M2" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="N2" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="O2" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="P2" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q2" s="52" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="93" t="s">
-        <v>173</v>
+      <c r="I2" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" s="109" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -9435,38 +9534,38 @@
       </c>
       <c r="B3" s="102"/>
       <c r="C3" s="64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" s="52">
         <v>1000</v>
       </c>
       <c r="G3" s="99" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="52" t="s">
-        <v>174</v>
-      </c>
       <c r="I3" s="53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J3" s="94" t="s">
         <v>102</v>
       </c>
       <c r="K3" s="64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L3" s="52"/>
       <c r="M3" s="99" t="s">
+        <v>168</v>
+      </c>
+      <c r="N3" s="52" t="s">
         <v>171</v>
-      </c>
-      <c r="N3" s="52" t="s">
-        <v>174</v>
       </c>
       <c r="O3" s="52"/>
       <c r="P3" s="52">
@@ -9474,7 +9573,7 @@
       </c>
       <c r="Q3" s="52"/>
       <c r="R3" s="93" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -9483,35 +9582,35 @@
       </c>
       <c r="B4" s="103"/>
       <c r="C4" s="60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F4" s="62">
         <v>50</v>
       </c>
       <c r="G4" s="62"/>
       <c r="H4" s="70" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I4" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J4" s="97">
         <v>120</v>
       </c>
       <c r="K4" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L4" s="99" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M4" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N4" s="52"/>
       <c r="O4" s="52"/>
@@ -9530,67 +9629,67 @@
       <c r="B5" s="102"/>
       <c r="C5" s="64"/>
       <c r="D5" s="52" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F5" s="52"/>
       <c r="G5" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="97"/>
       <c r="K5" s="99" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M5" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
       <c r="P5" s="52"/>
       <c r="Q5" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R5" s="97"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B6" s="102"/>
       <c r="C6" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
       <c r="H6" s="105" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I6" s="52"/>
       <c r="J6" s="97"/>
       <c r="K6" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L6" s="99" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M6" s="99" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N6" s="52"/>
       <c r="O6" s="52"/>
       <c r="P6" s="52"/>
       <c r="Q6" s="52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R6" s="97"/>
     </row>
@@ -9599,7 +9698,7 @@
         <v>149</v>
       </c>
       <c r="B7" s="102" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C7" s="64"/>
       <c r="D7" s="52"/>
@@ -9610,18 +9709,18 @@
       <c r="I7" s="52"/>
       <c r="J7" s="97"/>
       <c r="K7" s="99" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M7" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N7" s="52"/>
       <c r="O7" s="52" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="P7" s="52"/>
       <c r="Q7" s="52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R7" s="97"/>
     </row>
@@ -9630,16 +9729,16 @@
         <v>150</v>
       </c>
       <c r="B8" s="102" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C8" s="64"/>
       <c r="D8" s="52"/>
       <c r="E8" s="52" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H8" s="52"/>
       <c r="I8" s="52"/>
@@ -9651,7 +9750,7 @@
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
       <c r="Q8" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R8" s="97"/>
     </row>
@@ -9660,22 +9759,22 @@
         <v>151</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C9" s="64"/>
       <c r="D9" s="52" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="52"/>
       <c r="G9" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="52"/>
       <c r="J9" s="97"/>
       <c r="K9" s="52" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="L9" s="52"/>
       <c r="M9" s="52"/>
@@ -9683,7 +9782,7 @@
       <c r="O9" s="52"/>
       <c r="P9" s="52"/>
       <c r="Q9" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R9" s="97"/>
     </row>
@@ -9692,11 +9791,11 @@
         <v>152</v>
       </c>
       <c r="B10" s="102" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C10" s="64"/>
       <c r="D10" s="52" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="52"/>
@@ -9704,20 +9803,20 @@
       <c r="H10" s="52"/>
       <c r="I10" s="52"/>
       <c r="J10" s="97" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K10" s="52" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L10" s="52"/>
       <c r="M10" s="52" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="N10" s="52"/>
       <c r="O10" s="52"/>
       <c r="P10" s="52"/>
       <c r="Q10" s="52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R10" s="97"/>
     </row>
@@ -9726,26 +9825,26 @@
         <v>153</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
       <c r="J11" s="97"/>
       <c r="K11" s="64" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L11" s="52"/>
       <c r="M11" s="52"/>
@@ -9753,7 +9852,7 @@
       <c r="O11" s="52"/>
       <c r="P11" s="52"/>
       <c r="Q11" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R11" s="97"/>
     </row>
@@ -9762,24 +9861,24 @@
         <v>154</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C12" s="64"/>
       <c r="D12" s="52" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="52"/>
       <c r="G12" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
       <c r="J12" s="97"/>
       <c r="K12" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
@@ -9794,7 +9893,7 @@
         <v>155</v>
       </c>
       <c r="B13" s="102" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C13" s="64"/>
       <c r="D13" s="52"/>
@@ -9805,17 +9904,17 @@
       <c r="I13" s="52"/>
       <c r="J13" s="97"/>
       <c r="K13" s="106" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L13" s="52"/>
       <c r="M13" s="99" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
       <c r="Q13" s="99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R13" s="97"/>
     </row>
@@ -9833,7 +9932,7 @@
       <c r="I14" s="52"/>
       <c r="J14" s="97"/>
       <c r="K14" s="64" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="L14" s="52"/>
       <c r="M14" s="52"/>
@@ -9848,7 +9947,7 @@
         <v>157</v>
       </c>
       <c r="B15" s="102" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C15" s="64"/>
       <c r="D15" s="52"/>
@@ -9899,7 +9998,7 @@
       <c r="E17" s="52"/>
       <c r="F17" s="52"/>
       <c r="G17" s="52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H17" s="52"/>
       <c r="I17" s="52"/>
@@ -10001,6 +10100,14 @@
       <c r="Q21" s="66"/>
       <c r="R21" s="98"/>
     </row>
+    <row r="23" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="110" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:J1"/>

</xml_diff>

<commit_message>
Corregge configurazione 6 e 7
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD9DB60-9366-4C73-8DCD-8F0C604ED80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A8CC47-2C46-4B6D-B843-29F17D653A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <sheet name="CheckDiBa" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Database!$A$2:$T$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="240">
   <si>
     <t>Diagonali</t>
   </si>
@@ -1529,7 +1529,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1779,9 +1779,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3336,10 +3333,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="111"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -4313,21 +4310,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="113" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="114"/>
-      <c r="I1" s="116" t="s">
+      <c r="H1" s="113"/>
+      <c r="I1" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="116" t="s">
+      <c r="J1" s="115" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4356,8 +4353,8 @@
       <c r="H2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
@@ -4710,7 +4707,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,14 +4832,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5179,7 +5176,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G25"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5301,14 +5298,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5454,7 +5451,7 @@
         <f>IF(ISEVEN(A16),(A16-2)/2*$B$6,(A16-((A16-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1800</v>
       </c>
-      <c r="F16" s="119" t="s">
+      <c r="F16" s="118" t="s">
         <v>84</v>
       </c>
       <c r="G16" s="1">
@@ -5477,7 +5474,7 @@
         <f>IF(ISEVEN(A17),(A17-2)/2*$B$6,(A17-((A17-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>1750</v>
       </c>
-      <c r="F17" s="120"/>
+      <c r="F17" s="119"/>
       <c r="G17" s="1">
         <v>302</v>
       </c>
@@ -5498,7 +5495,7 @@
         <f>IF(ISEVEN(A18),(A18-2)/2*$B$6,(A18-((A18-1)/2)*$B$7)*$B$3+$B$5)</f>
         <v>2700</v>
       </c>
-      <c r="F18" s="120"/>
+      <c r="F18" s="119"/>
       <c r="G18" s="1">
         <v>302</v>
       </c>
@@ -5510,7 +5507,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="120"/>
+      <c r="F19" s="119"/>
       <c r="G19" s="1">
         <v>302</v>
       </c>
@@ -5522,7 +5519,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="120"/>
+      <c r="F20" s="119"/>
       <c r="G20" s="1">
         <v>302</v>
       </c>
@@ -5534,7 +5531,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="120"/>
+      <c r="F21" s="119"/>
       <c r="G21" s="1">
         <v>302</v>
       </c>
@@ -5546,7 +5543,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="120"/>
+      <c r="F22" s="119"/>
       <c r="G22" s="1">
         <v>302</v>
       </c>
@@ -5558,7 +5555,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="121"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="1">
         <v>302</v>
       </c>
@@ -5754,14 +5751,14 @@
       <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="117" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -6077,8 +6074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,35 +6103,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="124" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="122" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="121" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="122" t="s">
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="128" t="s">
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="123"/>
+      <c r="T1" s="127" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="128" t="s">
+      <c r="U1" s="127" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6196,8 +6193,8 @@
       <c r="S2" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="129"/>
-      <c r="U2" s="130"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="129"/>
       <c r="V2" s="56"/>
       <c r="W2" s="56"/>
       <c r="X2" s="56"/>
@@ -8060,44 +8057,44 @@
       <c r="G32" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H32" s="107">
-        <v>6000</v>
-      </c>
-      <c r="I32" s="62">
+      <c r="H32" s="85">
+        <v>5800</v>
+      </c>
+      <c r="I32" s="86">
         <v>800</v>
       </c>
-      <c r="J32" s="70">
+      <c r="J32" s="86">
         <v>1720</v>
       </c>
-      <c r="K32" s="62">
+      <c r="K32" s="86">
         <v>7</v>
       </c>
-      <c r="L32" s="62" t="s">
+      <c r="L32" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="M32" s="63">
+      <c r="M32" s="87">
         <v>1</v>
       </c>
-      <c r="N32" s="107">
-        <v>6800</v>
-      </c>
-      <c r="O32" s="62">
+      <c r="N32" s="85">
+        <v>5800</v>
+      </c>
+      <c r="O32" s="86">
         <v>790</v>
       </c>
-      <c r="P32" s="70">
-        <v>2240</v>
-      </c>
-      <c r="Q32" s="62">
+      <c r="P32" s="86">
+        <v>1780</v>
+      </c>
+      <c r="Q32" s="86">
         <v>1</v>
       </c>
-      <c r="R32" s="62" t="s">
+      <c r="R32" s="86" t="s">
         <v>106</v>
       </c>
       <c r="S32" s="68">
         <v>1</v>
       </c>
       <c r="T32" s="73" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="U32" s="76" t="s">
         <v>233</v>
@@ -8125,12 +8122,24 @@
       <c r="G33" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="H33" s="60"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="63"/>
+      <c r="H33" s="60">
+        <v>3600</v>
+      </c>
+      <c r="I33" s="62">
+        <v>890</v>
+      </c>
+      <c r="J33" s="62">
+        <v>1920</v>
+      </c>
+      <c r="K33" s="62">
+        <v>7</v>
+      </c>
+      <c r="L33" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M33" s="63">
+        <v>1</v>
+      </c>
       <c r="N33" s="60">
         <v>4000</v>
       </c>
@@ -8150,7 +8159,7 @@
         <v>1</v>
       </c>
       <c r="T33" s="73" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="U33" s="76" t="s">
         <v>239</v>
@@ -9123,7 +9132,7 @@
       <c r="U75" s="77"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T29" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
+  <autoFilter ref="A2:T33" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
   <mergeCells count="5">
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>
@@ -9451,26 +9460,26 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="95"/>
       <c r="B1" s="100"/>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="130" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="131" t="s">
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="130" t="s">
         <v>174</v>
       </c>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="133"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="132"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -9479,7 +9488,7 @@
       <c r="B2" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="107" t="s">
         <v>234</v>
       </c>
       <c r="D2" s="50" t="s">
@@ -9500,10 +9509,10 @@
       <c r="I2" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="109" t="s">
+      <c r="J2" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="107" t="s">
         <v>234</v>
       </c>
       <c r="L2" s="50" t="s">
@@ -9524,7 +9533,7 @@
       <c r="Q2" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="109" t="s">
+      <c r="R2" s="108" t="s">
         <v>170</v>
       </c>
     </row>
@@ -10101,7 +10110,7 @@
       <c r="R21" s="98"/>
     </row>
     <row r="23" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="109" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="8" t="s">

</xml_diff>

<commit_message>
Aggiorna le distinte in base all' aggiornamento del dB
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDDE8E5-84F3-404E-8B10-593726E77D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87002E45-7111-4DAE-9B61-3026D8A6865C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="241">
   <si>
     <t>Diagonali</t>
   </si>
@@ -831,6 +831,9 @@
   </si>
   <si>
     <t>Bordo basso, da rivedere la configurazione.</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -3318,7 +3321,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,7 +3355,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>10.6</v>
+        <v>4.7</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -3367,7 +3370,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>1.2</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -3385,7 +3388,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>2.2200000000000002</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -3404,7 +3407,7 @@
       </c>
       <c r="B5" s="2" t="str">
         <f>IF(B2&gt;=8,"Si","No")</f>
-        <v>Si</v>
+        <v>No</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>29</v>
@@ -3439,7 +3442,7 @@
         <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>240</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>58</v>
@@ -3456,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>240</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>59</v>
@@ -3482,7 +3485,7 @@
       </c>
       <c r="B10" s="2">
         <f>B2-ROUNDDOWN(B2/2,0)*2</f>
-        <v>0.59999999999999964</v>
+        <v>0.70000000000000018</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3498,7 +3501,7 @@
       </c>
       <c r="F12" s="13">
         <f>SUM(B18,B36)</f>
-        <v>1797.0907848489171</v>
+        <v>808.32172296022236</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3516,7 +3519,7 @@
       </c>
       <c r="F13" s="14">
         <f>C36</f>
-        <v>983.25969711501227</v>
+        <v>428.28624767046585</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3525,7 +3528,7 @@
       </c>
       <c r="B14" s="3">
         <f>IF(B5="Si",200,0)</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>23</v>
@@ -3549,7 +3552,7 @@
       </c>
       <c r="B16" s="3">
         <f>IF(B7="Si",250,0)</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>23</v>
@@ -3561,7 +3564,7 @@
       </c>
       <c r="B17" s="3">
         <f>IF(AND(B8="Si",B2&lt;9),200,IF(AND(B8="Si",B2&gt;=9),250,0))</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>23</v>
@@ -3573,7 +3576,7 @@
       </c>
       <c r="B18" s="5">
         <f>SUM(B13:B17)</f>
-        <v>1220</v>
+        <v>520</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" s="47"/>
@@ -3605,11 +3608,11 @@
       </c>
       <c r="B21" s="3">
         <f>B2*G3*4</f>
-        <v>190.79999999999998</v>
+        <v>84.600000000000009</v>
       </c>
       <c r="C21" s="11">
         <f>B2*F3*4</f>
-        <v>325.84501759999995</v>
+        <v>144.47845119999999</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="49"/>
@@ -3621,11 +3624,11 @@
       </c>
       <c r="B22" s="3">
         <f>IF(B2&gt;=8,B9*G3*4,0)</f>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C22" s="11">
         <f>IF(B2&gt;=8,B9*F3*4,0)</f>
-        <v>61.480191999999995</v>
+        <v>0</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16"/>
@@ -3636,11 +3639,11 @@
       </c>
       <c r="B23" s="3">
         <f>ROUND((B2+1),0)*G3*B3</f>
-        <v>64.8</v>
+        <v>30.779999999999998</v>
       </c>
       <c r="C23" s="11">
         <f>ROUND((B2+1),0)*F3*B3</f>
-        <v>110.66434559999999</v>
+        <v>52.565564159999994</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
@@ -3651,11 +3654,11 @@
       </c>
       <c r="B24" s="3">
         <f>ROUND(((B2/2)+1),0)*G4*B3</f>
-        <v>14.399999999999999</v>
+        <v>6.84</v>
       </c>
       <c r="C24" s="11">
         <f>ROUND(((B2/2)+1),0)*F4*B3</f>
-        <v>25.171603200000003</v>
+        <v>11.956511520000001</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
@@ -3666,11 +3669,11 @@
       </c>
       <c r="B25" s="3">
         <f>ROUND((B2+1),0)*B4*G4</f>
-        <v>53.28</v>
+        <v>26.880000000000003</v>
       </c>
       <c r="C25" s="11">
         <f>ROUND((B2+1),0)*B4*F4</f>
-        <v>93.134931840000007</v>
+        <v>46.986992640000011</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
@@ -3681,11 +3684,11 @@
       </c>
       <c r="B26" s="3">
         <f>SQRT(2^2+B4^2)*ROUNDDOWN(B2,0)*G4</f>
-        <v>59.760856754233373</v>
+        <v>24.023455205278029</v>
       </c>
       <c r="C26" s="11">
         <f>SQRT(2^2+B4^2)*ROUNDDOWN(B2,0)*F4</f>
-        <v>104.46365091038906</v>
+        <v>41.993672355571746</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
@@ -3696,11 +3699,11 @@
       </c>
       <c r="B27" s="3">
         <f>SQRT(B10^2+B4^2)*G4*2</f>
-        <v>9.1986085904336647</v>
+        <v>9.3873105839745179</v>
       </c>
       <c r="C27" s="11">
         <f>SQRT(B10^2+B4^2)*F4*2</f>
-        <v>16.079425377118579</v>
+        <v>16.40928174548381</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
@@ -3711,11 +3714,11 @@
       </c>
       <c r="B28" s="3">
         <f>SQRT(2^2+B4^2)*ROUNDDOWN(B2,0)*G5</f>
-        <v>22.410321282837515</v>
+        <v>9.0087957019792615</v>
       </c>
       <c r="C28" s="11">
         <f>SQRT(2^2+B4^2)*ROUNDDOWN(B2,0)*F5</f>
-        <v>56.175338081781035</v>
+        <v>22.582101250638736</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
@@ -3726,11 +3729,11 @@
       </c>
       <c r="B29" s="3">
         <f>SQRT(B10^2+B4^2)*G5*2</f>
-        <v>3.4494782214126243</v>
+        <v>3.5202414689904442</v>
       </c>
       <c r="C29" s="11">
         <f>SQRT(B10^2+B4^2)*F5*2</f>
-        <v>8.6467125057236007</v>
+        <v>8.8240927987715683</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
@@ -3741,11 +3744,11 @@
       </c>
       <c r="B30" s="3">
         <f>B2*B4*2*G6</f>
-        <v>13.177920000000002</v>
+        <v>5.8956800000000023</v>
       </c>
       <c r="C30" s="11">
         <f>B2*B4*2*F6</f>
-        <v>139.78008</v>
+        <v>62.536320000000018</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16"/>
@@ -3756,11 +3759,11 @@
       </c>
       <c r="B31" s="3">
         <f>B2*B3*G6</f>
-        <v>3.5615999999999999</v>
+        <v>1.50024</v>
       </c>
       <c r="C31" s="11">
         <f>B2*B3*F6</f>
-        <v>37.778399999999998</v>
+        <v>15.913259999999999</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
@@ -3807,11 +3810,11 @@
       </c>
       <c r="B35" s="3">
         <f>(B2*B4*2+B2*B3*2)*G7</f>
-        <v>36.251999999999995</v>
+        <v>15.886000000000003</v>
       </c>
       <c r="C35" s="11">
         <f>F7*(B2*B4*2+B2*B3*2)</f>
-        <v>14.500799999999998</v>
+        <v>6.3544000000000018</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="16"/>
@@ -3822,11 +3825,11 @@
       </c>
       <c r="B36" s="10">
         <f>SUM(B21:B35)</f>
-        <v>577.09078484891711</v>
+        <v>288.3217229602223</v>
       </c>
       <c r="C36" s="12">
         <f>SUM(C21:C34)</f>
-        <v>983.25969711501227</v>
+        <v>428.28624767046585</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16"/>
@@ -3835,7 +3838,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B8" xr:uid="{889F7A08-76CA-49FF-B344-072017510DBF}">
       <formula1>"Si,No,"</formula1>
     </dataValidation>
@@ -6072,7 +6075,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AG75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -6209,7 +6211,7 @@
       <c r="AF2" s="56"/>
       <c r="AG2" s="56"/>
     </row>
-    <row r="3" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="60">
         <v>20210538</v>
       </c>
@@ -6274,7 +6276,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="64">
         <v>20210304</v>
       </c>
@@ -6402,7 +6404,7 @@
       </c>
       <c r="U5" s="76"/>
     </row>
-    <row r="6" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="64">
         <v>20210164</v>
       </c>
@@ -6467,7 +6469,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="64">
         <v>20210296</v>
       </c>
@@ -6530,7 +6532,7 @@
       </c>
       <c r="U7" s="76"/>
     </row>
-    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="64">
         <v>20210250</v>
       </c>
@@ -6593,7 +6595,7 @@
       </c>
       <c r="U8" s="76"/>
     </row>
-    <row r="9" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="64">
         <v>20210187</v>
       </c>
@@ -6656,7 +6658,7 @@
       </c>
       <c r="U9" s="76"/>
     </row>
-    <row r="10" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="64">
         <v>20210272</v>
       </c>
@@ -6719,7 +6721,7 @@
       </c>
       <c r="U10" s="76"/>
     </row>
-    <row r="11" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="64">
         <v>20210264</v>
       </c>
@@ -6782,7 +6784,7 @@
       </c>
       <c r="U11" s="76"/>
     </row>
-    <row r="12" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="64">
         <v>20210235</v>
       </c>
@@ -6845,7 +6847,7 @@
       </c>
       <c r="U12" s="76"/>
     </row>
-    <row r="13" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="64">
         <v>20210245</v>
       </c>
@@ -6908,7 +6910,7 @@
       </c>
       <c r="U13" s="76"/>
     </row>
-    <row r="14" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="64">
         <v>20200269</v>
       </c>
@@ -7034,7 +7036,7 @@
       </c>
       <c r="U15" s="76"/>
     </row>
-    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="64">
         <v>20200306</v>
       </c>
@@ -7162,7 +7164,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="64">
         <v>20210423</v>
       </c>
@@ -7225,7 +7227,7 @@
       </c>
       <c r="U18" s="76"/>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="64">
         <v>20210312</v>
       </c>
@@ -7276,7 +7278,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="64">
         <v>20210133</v>
       </c>
@@ -7404,7 +7406,7 @@
       </c>
       <c r="U21" s="76"/>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="64">
         <v>20210528</v>
       </c>
@@ -9133,13 +9135,7 @@
       <c r="U75" s="77"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T33" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:T33" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}"/>
   <mergeCells count="5">
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>

</xml_diff>

<commit_message>
Fix generazione DiBa con nastri solo tazze
</commit_message>
<xml_diff>
--- a/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
+++ b/DocumentazioneBeltsPack/Test/TestPrezziPesi_Imballi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ale\Lavoro\Morinat\BeltsPack\DocumentazioneBeltsPack\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BFDFBB-72A6-4157-B874-94CF70EC3645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0353502F-0271-4CAD-A5F0-A99042053D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{9ECB03AF-49BE-4AD4-B3CF-CBBBD005DDA1}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="251">
   <si>
     <t>Diagonali</t>
   </si>
@@ -1563,7 +1563,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1851,9 +1851,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3037,7 +3034,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33A19757-1B1A-4917-3D22-620EF6231B38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6752,8 +6749,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754F06D9-22FC-4A67-B491-7C126D95A070}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8868,7 +8866,7 @@
       <c r="H34" s="51">
         <v>11800</v>
       </c>
-      <c r="I34" s="115">
+      <c r="I34" s="53">
         <v>2530</v>
       </c>
       <c r="J34" s="53">
@@ -8889,7 +8887,7 @@
       <c r="O34" s="53">
         <v>1900</v>
       </c>
-      <c r="P34" s="115">
+      <c r="P34" s="53">
         <v>2450</v>
       </c>
       <c r="Q34" s="53">
@@ -8909,95 +8907,255 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="59"/>
-      <c r="T35" s="64"/>
+      <c r="A35" s="55">
+        <v>20220114</v>
+      </c>
+      <c r="B35" s="60">
+        <v>44819</v>
+      </c>
+      <c r="C35" s="44">
+        <v>139000</v>
+      </c>
+      <c r="D35" s="44">
+        <v>750</v>
+      </c>
+      <c r="E35" s="53">
+        <v>160</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H35" s="51">
+        <v>8700</v>
+      </c>
+      <c r="I35" s="53">
+        <v>2100</v>
+      </c>
+      <c r="J35" s="53">
+        <v>1730</v>
+      </c>
+      <c r="K35" s="53">
+        <v>1</v>
+      </c>
+      <c r="L35" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="M35" s="54">
+        <v>2</v>
+      </c>
+      <c r="N35" s="51">
+        <v>9000</v>
+      </c>
+      <c r="O35" s="53">
+        <v>2100</v>
+      </c>
+      <c r="P35" s="53">
+        <v>1750</v>
+      </c>
+      <c r="Q35" s="53">
+        <v>1</v>
+      </c>
+      <c r="R35" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="S35" s="59">
+        <v>2</v>
+      </c>
+      <c r="T35" s="64" t="s">
+        <v>23</v>
+      </c>
       <c r="U35" s="67"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="64"/>
+      <c r="A36" s="55">
+        <v>20220336</v>
+      </c>
+      <c r="B36" s="60">
+        <v>44838</v>
+      </c>
+      <c r="C36" s="44">
+        <v>37000</v>
+      </c>
+      <c r="D36" s="44">
+        <v>800</v>
+      </c>
+      <c r="E36" s="53">
+        <v>160</v>
+      </c>
+      <c r="F36" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H36" s="51">
+        <v>5800</v>
+      </c>
+      <c r="I36" s="53">
+        <v>940</v>
+      </c>
+      <c r="J36" s="53">
+        <v>2240</v>
+      </c>
+      <c r="K36" s="53">
+        <v>1</v>
+      </c>
+      <c r="L36" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="M36" s="54">
+        <v>1</v>
+      </c>
+      <c r="N36" s="51">
+        <v>5500</v>
+      </c>
+      <c r="O36" s="53">
+        <v>950</v>
+      </c>
+      <c r="P36" s="53">
+        <v>2240</v>
+      </c>
+      <c r="Q36" s="53">
+        <v>1</v>
+      </c>
+      <c r="R36" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="S36" s="59">
+        <v>1</v>
+      </c>
+      <c r="T36" s="64" t="s">
+        <v>23</v>
+      </c>
       <c r="U36" s="67"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="64"/>
+      <c r="A37" s="55">
+        <v>20220313</v>
+      </c>
+      <c r="B37" s="60">
+        <v>44846</v>
+      </c>
+      <c r="C37" s="44">
+        <v>60000</v>
+      </c>
+      <c r="D37" s="44">
+        <v>800</v>
+      </c>
+      <c r="E37" s="53">
+        <v>200</v>
+      </c>
+      <c r="F37" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37" s="51">
+        <v>9400</v>
+      </c>
+      <c r="I37" s="53">
+        <v>940</v>
+      </c>
+      <c r="J37" s="53">
+        <v>2240</v>
+      </c>
+      <c r="K37" s="53">
+        <v>1</v>
+      </c>
+      <c r="L37" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="M37" s="54">
+        <v>1</v>
+      </c>
+      <c r="N37" s="51">
+        <v>9400</v>
+      </c>
+      <c r="O37" s="53">
+        <v>950</v>
+      </c>
+      <c r="P37" s="53">
+        <v>2240</v>
+      </c>
+      <c r="Q37" s="53">
+        <v>1</v>
+      </c>
+      <c r="R37" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="S37" s="59">
+        <v>1</v>
+      </c>
+      <c r="T37" s="64" t="s">
+        <v>23</v>
+      </c>
       <c r="U37" s="67"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="59"/>
-      <c r="T38" s="64"/>
+      <c r="A38" s="55">
+        <v>20220375</v>
+      </c>
+      <c r="B38" s="60">
+        <v>44837</v>
+      </c>
+      <c r="C38" s="44">
+        <v>46100</v>
+      </c>
+      <c r="D38" s="44">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="53">
+        <v>160</v>
+      </c>
+      <c r="F38" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38" s="51">
+        <v>5800</v>
+      </c>
+      <c r="I38" s="53">
+        <v>1140</v>
+      </c>
+      <c r="J38" s="53">
+        <v>2530</v>
+      </c>
+      <c r="K38" s="53">
+        <v>1</v>
+      </c>
+      <c r="L38" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="M38" s="54">
+        <v>1</v>
+      </c>
+      <c r="N38" s="51">
+        <v>5800</v>
+      </c>
+      <c r="O38" s="53">
+        <v>1140</v>
+      </c>
+      <c r="P38" s="53">
+        <v>2100</v>
+      </c>
+      <c r="Q38" s="53">
+        <v>1</v>
+      </c>
+      <c r="R38" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="S38" s="59">
+        <v>1</v>
+      </c>
+      <c r="T38" s="64" t="s">
+        <v>23</v>
+      </c>
       <c r="U38" s="67"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -9875,10 +10033,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K75 Q3:Q75" xr:uid="{1680938F-FEBA-4BD0-AD9E-C379B9D51075}">
       <formula1>"1,2,3,4,5,6,7,-,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L75 R3:R75" xr:uid="{52775BBC-9B41-4CCF-8CE4-E19D926CD49C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R75 L3:L75" xr:uid="{52775BBC-9B41-4CCF-8CE4-E19D926CD49C}">
       <formula1>"Cassa in ferro, Cassa in legno,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M75 S3:S75" xr:uid="{F60DF200-FBE7-451E-8A72-514BC952C463}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S75 M3:M75" xr:uid="{F60DF200-FBE7-451E-8A72-514BC952C463}">
       <formula1>"1,2,-,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F75" xr:uid="{5865F76D-6592-4088-891A-E3BB5A14F46D}">

</xml_diff>